<commit_message>
feat: altri dati: costo gas, carbone; capex solare, eolico, nucleare, battery Li-ion
</commit_message>
<xml_diff>
--- a/dati_casoStudioItalia/altri_dati.xlsx
+++ b/dati_casoStudioItalia/altri_dati.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DrinDrin\dati_casoStudioItalia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/gianvito_colucci_polito_it/Documents/Jobs/DRIN DRIN/Energy mix/DrinDrin---Mix-energetico/dati_casoStudioItalia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{629DCDB6-94E5-432A-9179-03575796D74D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="503" documentId="8_{629DCDB6-94E5-432A-9179-03575796D74D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FA79E20-9E4E-41B0-A680-C53B0847AEF6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B845255D-815F-49EA-8438-49CAB31B3547}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{B845255D-815F-49EA-8438-49CAB31B3547}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="raw_data_commodity" sheetId="2" r:id="rId2"/>
+    <sheet name="raw_data_techs" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,8 +37,186 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Gianvito Colucci</author>
+  </authors>
+  <commentList>
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{F8A21B29-A55C-40FB-85BB-5003BBC2961C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gianvito Colucci:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+i.e., TTF</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{3DF5F49D-28A5-4E85-A45D-63D24C8533ED}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gianvito Colucci:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+i.e., TTF</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{0A822877-4EA8-43DA-81FF-4BE357D7609F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gianvito Colucci:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+i.e., TTF</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{8B999BFB-05E6-48CE-AC0A-32E692B1A9DC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gianvito Colucci:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+i.e., TTF</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{08953F1C-2B5C-4237-AF37-8A03AABAC566}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gianvito Colucci:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+i.e., TTF</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{9611ACF5-D7D0-4416-B766-4F113160A59E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gianvito Colucci:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+i.e., TTF</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{D7C951DD-479A-40B4-B216-10E08A4A8B25}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gianvito Colucci:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+i.e., TTF</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="57">
   <si>
     <t>value</t>
   </si>
@@ -96,16 +276,202 @@
   </si>
   <si>
     <t>costo combustibile carbone</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>($2010/mt)</t>
+  </si>
+  <si>
+    <t>World Bank</t>
+  </si>
+  <si>
+    <t>($2010/mmbtu)</t>
+  </si>
+  <si>
+    <t>Conversion</t>
+  </si>
+  <si>
+    <t>Multiplier</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Harmonised Index of Consumer Prices (HICP)</t>
+  </si>
+  <si>
+    <t>Natural gas, Europe</t>
+  </si>
+  <si>
+    <t>Coal, Australian</t>
+  </si>
+  <si>
+    <t>€2020/$2010</t>
+  </si>
+  <si>
+    <t>MWh/mmbtu</t>
+  </si>
+  <si>
+    <t>MWh/kcal</t>
+  </si>
+  <si>
+    <t>Standard heating value of thermal coal (kcal/kg)</t>
+  </si>
+  <si>
+    <t>(€2020/MWh)</t>
+  </si>
+  <si>
+    <t>€2020/$2020</t>
+  </si>
+  <si>
+    <t>(M$2020/GW)</t>
+  </si>
+  <si>
+    <t>TEMOA-Italy</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Entry voice</t>
+  </si>
+  <si>
+    <t>Model unit</t>
+  </si>
+  <si>
+    <t>Model input value</t>
+  </si>
+  <si>
+    <t>Dati elaborati da NREL</t>
+  </si>
+  <si>
+    <t>(€2020/MW)</t>
+  </si>
+  <si>
+    <t>Tech type</t>
+  </si>
+  <si>
+    <t>Utility scale</t>
+  </si>
+  <si>
+    <t>Onshore</t>
+  </si>
+  <si>
+    <t>Offshore</t>
+  </si>
+  <si>
+    <t>Offshore acque profonde</t>
+  </si>
+  <si>
+    <t>LWR (credo sia AP1000)</t>
+  </si>
+  <si>
+    <t>SMR (credo sia AP1000)</t>
+  </si>
+  <si>
+    <t>Comment 2</t>
+  </si>
+  <si>
+    <t>Comment 1</t>
+  </si>
+  <si>
+    <t>Include il decommissioning</t>
+  </si>
+  <si>
+    <t>Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno "storage duration" di 6 ore. Per ulteriori info, vedere questo paper</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0E+00"/>
+  </numFmts>
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -128,14 +494,87 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{E74E4B4E-3625-467E-8352-5D2088EA65F7}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -470,16 +909,18 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -490,7 +931,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -498,7 +939,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -506,7 +947,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -514,7 +955,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -522,7 +963,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -530,7 +971,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -538,7 +979,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -546,7 +987,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -554,7 +995,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -562,7 +1003,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -570,7 +1011,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -578,7 +1019,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -586,7 +1027,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -597,4 +1038,1284 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42806216-DB6B-4ED6-9AA4-BC1B162122E7}">
+  <dimension ref="A1:Y27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="6" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="20">
+        <v>2018</v>
+      </c>
+      <c r="C2" s="21">
+        <v>7.5414094383199997</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="9">
+        <f t="shared" ref="G2:G8" si="0">C2*$M$3/$M$4</f>
+        <v>21.805545521741941</v>
+      </c>
+      <c r="H2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="20">
+        <v>2019</v>
+      </c>
+      <c r="C3" s="21">
+        <v>4.8274540271299999</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="9">
+        <f t="shared" si="0"/>
+        <v>13.958301747657082</v>
+      </c>
+      <c r="H3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" s="11">
+        <v>0.85</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="W3" s="2"/>
+      <c r="Y3" s="6"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="20">
+        <v>2020</v>
+      </c>
+      <c r="C4" s="21">
+        <v>3.3115669452400409</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="9">
+        <f t="shared" si="0"/>
+        <v>9.5752026677938797</v>
+      </c>
+      <c r="H4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="12">
+        <v>0.29397099999999998</v>
+      </c>
+      <c r="N4" s="8"/>
+      <c r="W4" s="2"/>
+      <c r="Y4" s="4"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="20">
+        <v>2021</v>
+      </c>
+      <c r="C5" s="21">
+        <v>14.731149861407678</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="9">
+        <f t="shared" si="0"/>
+        <v>42.594260597802254</v>
+      </c>
+      <c r="H5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="M5" s="14">
+        <f>1.622*10^-6</f>
+        <v>1.6220000000000001E-6</v>
+      </c>
+      <c r="W5" s="2"/>
+      <c r="Y5" s="5"/>
+    </row>
+    <row r="6" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="20">
+        <v>2022</v>
+      </c>
+      <c r="C6" s="21">
+        <v>34.346664233461041</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="9">
+        <f t="shared" si="0"/>
+        <v>99.311376286919071</v>
+      </c>
+      <c r="H6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="M6" s="11">
+        <v>6000</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y6" s="10"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="20">
+        <v>2023</v>
+      </c>
+      <c r="C7" s="21">
+        <v>11.492903809114813</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="9">
+        <f t="shared" si="0"/>
+        <v>33.23106101536407</v>
+      </c>
+      <c r="H7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" s="13"/>
+      <c r="Y7" s="10"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="20">
+        <v>2024</v>
+      </c>
+      <c r="C8" s="21">
+        <v>9.52416119251955</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="9">
+        <f t="shared" si="0"/>
+        <v>27.538556570687646</v>
+      </c>
+      <c r="H8" t="s">
+        <v>34</v>
+      </c>
+      <c r="M8" s="13"/>
+      <c r="Y8" s="10"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="20">
+        <v>2018</v>
+      </c>
+      <c r="C9" s="21">
+        <v>105.06823090515999</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="9">
+        <f t="shared" ref="G9:G15" si="1">C9*$M$3/$M$6/$M$5/1000</f>
+        <v>9.1767361559171796</v>
+      </c>
+      <c r="H9" t="s">
+        <v>34</v>
+      </c>
+      <c r="M9" s="13"/>
+      <c r="Y9" s="10"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="20">
+        <v>2019</v>
+      </c>
+      <c r="C10" s="21">
+        <v>78.292956708220004</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="9">
+        <f t="shared" si="1"/>
+        <v>6.8381641185765512</v>
+      </c>
+      <c r="H10" t="s">
+        <v>34</v>
+      </c>
+      <c r="M10" s="13"/>
+      <c r="Y10" s="10"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="20">
+        <v>2020</v>
+      </c>
+      <c r="C11" s="21">
+        <v>62.08886618998978</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="9">
+        <f t="shared" si="1"/>
+        <v>5.4228869976871463</v>
+      </c>
+      <c r="H11" t="s">
+        <v>34</v>
+      </c>
+      <c r="M11" s="13"/>
+      <c r="Y11" s="10"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="20">
+        <v>2021</v>
+      </c>
+      <c r="C12" s="21">
+        <v>126.18829981718464</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="9">
+        <f t="shared" si="1"/>
+        <v>11.021378426285136</v>
+      </c>
+      <c r="H12" t="s">
+        <v>34</v>
+      </c>
+      <c r="M12" s="13"/>
+      <c r="Y12" s="10"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="20">
+        <v>2022</v>
+      </c>
+      <c r="C13" s="21">
+        <v>293.6511990918093</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="9">
+        <f t="shared" si="1"/>
+        <v>25.647710565971831</v>
+      </c>
+      <c r="H13" t="s">
+        <v>34</v>
+      </c>
+      <c r="M13" s="13"/>
+      <c r="Y13" s="10"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A14" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="20">
+        <v>2023</v>
+      </c>
+      <c r="C14" s="21">
+        <v>151.42784107508328</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="9">
+        <f t="shared" si="1"/>
+        <v>13.225818425176818</v>
+      </c>
+      <c r="H14" t="s">
+        <v>34</v>
+      </c>
+      <c r="M14" s="13"/>
+      <c r="Y14" s="10"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A15" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="20">
+        <v>2024</v>
+      </c>
+      <c r="C15" s="21">
+        <v>118.28554879814943</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="9">
+        <f t="shared" si="1"/>
+        <v>10.331146370574086</v>
+      </c>
+      <c r="H15" t="s">
+        <v>34</v>
+      </c>
+      <c r="M15" s="13"/>
+      <c r="Y15" s="10"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="M16" s="13"/>
+      <c r="Y16" s="4"/>
+    </row>
+    <row r="17" spans="13:25" x14ac:dyDescent="0.25">
+      <c r="M17" s="13"/>
+      <c r="Y17" s="5"/>
+    </row>
+    <row r="18" spans="13:25" x14ac:dyDescent="0.25">
+      <c r="M18" s="13"/>
+      <c r="Y18" s="9"/>
+    </row>
+    <row r="19" spans="13:25" x14ac:dyDescent="0.25">
+      <c r="M19" s="13"/>
+      <c r="Y19" s="9"/>
+    </row>
+    <row r="20" spans="13:25" x14ac:dyDescent="0.25">
+      <c r="Y20" s="9"/>
+    </row>
+    <row r="27" spans="13:25" x14ac:dyDescent="0.25">
+      <c r="Q27" s="17"/>
+      <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="N6" r:id="rId1" xr:uid="{DF57DE7B-1BFB-46E2-A367-B6ECAC30D28E}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{43CE2A3A-56DA-4553-9E4F-92362EE5CD04}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{9754E331-82B7-49C8-B626-F4CF5E7C173E}"/>
+    <hyperlink ref="E4" r:id="rId4" xr:uid="{EF383D0A-15F0-4B08-A733-3C043077C9F9}"/>
+    <hyperlink ref="E5" r:id="rId5" xr:uid="{944C0B5A-49D5-4D80-93EF-C6B85DB6304A}"/>
+    <hyperlink ref="E6" r:id="rId6" xr:uid="{6988E22D-F804-4C62-8C7B-7F83ED9B3CB7}"/>
+    <hyperlink ref="E7" r:id="rId7" xr:uid="{DE760FD1-0CEE-4185-9625-11A99D9355EA}"/>
+    <hyperlink ref="E8" r:id="rId8" xr:uid="{A6CF3B73-709A-4F91-97B5-6A913B5528DA}"/>
+    <hyperlink ref="E9:E15" r:id="rId9" display="World Bank" xr:uid="{80874292-EDDF-4056-827D-D7F6914B6036}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId10"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F958822-C8DD-4CF0-BC79-5189EFFDF89D}">
+  <dimension ref="A1:T28"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" customWidth="1"/>
+    <col min="8" max="8" width="42.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="8">
+        <v>2020</v>
+      </c>
+      <c r="D2" s="23">
+        <v>1333</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="24"/>
+      <c r="I2" s="8">
+        <f>D2*$Q$3*10^3</f>
+        <v>1173040</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="8">
+        <v>2030</v>
+      </c>
+      <c r="D3" s="23">
+        <v>754</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="24"/>
+      <c r="I3" s="8">
+        <f t="shared" ref="I3:I8" si="0">D3*$Q$3*10^3</f>
+        <v>663520</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="P3" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" s="11">
+        <v>0.88</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="8">
+        <v>2020</v>
+      </c>
+      <c r="D4" s="23">
+        <v>1462</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="24"/>
+      <c r="I4" s="8">
+        <f t="shared" si="0"/>
+        <v>1286560</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="8">
+        <v>2030</v>
+      </c>
+      <c r="D5" s="23">
+        <v>956</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="24"/>
+      <c r="I5" s="8">
+        <f t="shared" si="0"/>
+        <v>841280</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="8">
+        <v>2020</v>
+      </c>
+      <c r="D6" s="23">
+        <v>3739</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="24"/>
+      <c r="I6" s="8">
+        <f t="shared" si="0"/>
+        <v>3290320</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="8">
+        <v>2030</v>
+      </c>
+      <c r="D7" s="23">
+        <v>2758</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="24"/>
+      <c r="I7" s="8">
+        <f t="shared" si="0"/>
+        <v>2427040</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="8">
+        <v>2020</v>
+      </c>
+      <c r="D8" s="23">
+        <v>4049</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" s="24"/>
+      <c r="I8" s="8">
+        <f t="shared" si="0"/>
+        <v>3563120</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="8">
+        <v>2030</v>
+      </c>
+      <c r="D9" s="23">
+        <v>3467</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="24"/>
+      <c r="I9" s="8">
+        <f>D9*$Q$3*10^3</f>
+        <v>3050960</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="8">
+        <v>2035</v>
+      </c>
+      <c r="D10" s="23">
+        <v>6160.0000000000009</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10" s="8">
+        <f t="shared" ref="I10:I16" si="1">D10*$Q$3*10^3</f>
+        <v>5420800.0000000009</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="8">
+        <v>2050</v>
+      </c>
+      <c r="D11" s="23">
+        <v>5500</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="8">
+        <f t="shared" si="1"/>
+        <v>4840000</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="8">
+        <v>2035</v>
+      </c>
+      <c r="D12" s="23">
+        <v>6820.0000000000009</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" s="8">
+        <f t="shared" si="1"/>
+        <v>6001600.0000000009</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="8">
+        <v>2050</v>
+      </c>
+      <c r="D13" s="23">
+        <v>6050.0000000000009</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13" s="8">
+        <f t="shared" si="1"/>
+        <v>5324000.0000000009</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8">
+        <v>2020</v>
+      </c>
+      <c r="D14" s="18">
+        <v>2466</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="I14" s="8">
+        <f t="shared" si="1"/>
+        <v>2170080</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="R14" s="2"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+    </row>
+    <row r="15" spans="1:20" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8">
+        <v>2030</v>
+      </c>
+      <c r="D15" s="18">
+        <v>1210</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="I15" s="8">
+        <f t="shared" si="1"/>
+        <v>1064800</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="R15" s="2"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+    </row>
+    <row r="16" spans="1:20" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8">
+        <v>2050</v>
+      </c>
+      <c r="D16" s="18">
+        <v>908</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="I16" s="8">
+        <f t="shared" si="1"/>
+        <v>799040</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="R16" s="2"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="10"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="10"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" display="World Bank" xr:uid="{3BCD531E-88E2-4617-BE0D-57C0BE0CDE4C}"/>
+    <hyperlink ref="G2" r:id="rId2" xr:uid="{E134E359-0624-4ADD-AE0D-E6195FFD25A4}"/>
+    <hyperlink ref="F3" r:id="rId3" display="World Bank" xr:uid="{11649A99-BBF5-429D-92C0-B1AB39DFCDAB}"/>
+    <hyperlink ref="G3" r:id="rId4" xr:uid="{63198A70-1594-447D-BF39-AD7C3371EF67}"/>
+    <hyperlink ref="F4" r:id="rId5" display="World Bank" xr:uid="{234A250E-341C-41EF-9E6C-5F70C9AD1AA2}"/>
+    <hyperlink ref="F5" r:id="rId6" display="World Bank" xr:uid="{24ED7D87-6BA0-4591-B8FB-8DBFC7C67291}"/>
+    <hyperlink ref="F6" r:id="rId7" display="World Bank" xr:uid="{4E4A5E32-C5B0-4B55-BC1D-A8BCB8AB3343}"/>
+    <hyperlink ref="F7" r:id="rId8" display="World Bank" xr:uid="{34A735C2-398A-4AF0-AC92-CDE49E221E44}"/>
+    <hyperlink ref="F8" r:id="rId9" display="World Bank" xr:uid="{D82100BF-E290-4C7F-83FE-7ACF88644A48}"/>
+    <hyperlink ref="F9" r:id="rId10" display="World Bank" xr:uid="{F0A57130-2B16-425F-838B-37D425B23764}"/>
+    <hyperlink ref="G4" r:id="rId11" xr:uid="{74C7DDA8-7917-4F78-B0B5-A38959B43587}"/>
+    <hyperlink ref="G5" r:id="rId12" xr:uid="{EA35BC2E-0439-4BB5-8635-24C6E1A59507}"/>
+    <hyperlink ref="G6" r:id="rId13" xr:uid="{CB8B6EC7-D21F-4093-AE53-04FF92EE23C3}"/>
+    <hyperlink ref="G7" r:id="rId14" xr:uid="{4BC76F65-9AF5-43B2-95D0-0E17535DD882}"/>
+    <hyperlink ref="G8" r:id="rId15" xr:uid="{254A0ED1-9B59-4B3A-800D-0B7D5611C9F8}"/>
+    <hyperlink ref="G9" r:id="rId16" xr:uid="{53F61002-38D5-4F86-850D-731FF68607AC}"/>
+    <hyperlink ref="F10" r:id="rId17" display="World Bank" xr:uid="{F0DC3470-B776-4B2D-B27E-08A0A05751B0}"/>
+    <hyperlink ref="F11" r:id="rId18" display="World Bank" xr:uid="{69B713EC-CE42-44B4-85A8-A3466168667C}"/>
+    <hyperlink ref="F12" r:id="rId19" display="World Bank" xr:uid="{0EE4B772-3B1C-40C1-8489-D0631B2D4463}"/>
+    <hyperlink ref="F13" r:id="rId20" display="World Bank" xr:uid="{C22641C2-FA38-48D9-BCB2-1FCE72A643D6}"/>
+    <hyperlink ref="G10" r:id="rId21" xr:uid="{1BCFB97B-FADB-43D9-B44E-ADA05CA17A73}"/>
+    <hyperlink ref="F14" r:id="rId22" display="World Bank" xr:uid="{AF15079B-1809-4BD8-A648-4D62ABE8C206}"/>
+    <hyperlink ref="G14" r:id="rId23" xr:uid="{0CA73A59-1222-47DA-A59D-000D8B582034}"/>
+    <hyperlink ref="F15" r:id="rId24" display="World Bank" xr:uid="{199C7D2F-21A1-4692-9440-4CC169B6F2F2}"/>
+    <hyperlink ref="G15" r:id="rId25" xr:uid="{CECC446B-999A-4D89-A0D6-D3177C929A3D}"/>
+    <hyperlink ref="F16" r:id="rId26" display="World Bank" xr:uid="{8716B52B-0C43-4E99-8CCE-17C58FE13622}"/>
+    <hyperlink ref="G16" r:id="rId27" xr:uid="{85050209-E008-45C2-8A24-F79F70751A59}"/>
+    <hyperlink ref="G11:G13" r:id="rId28" display="Dati elaborati da NREL" xr:uid="{8CAF9D49-1D95-457A-AD06-EF2B25EC7C48}"/>
+    <hyperlink ref="H14" r:id="rId29" xr:uid="{BD06F35F-2859-4868-A250-9877196A2A8B}"/>
+    <hyperlink ref="H15:H16" r:id="rId30" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{D5926397-0CC0-4EED-B446-ADD3939AFBF8}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: assume costo gas, carbone; capex solare, onshore, offshore
</commit_message>
<xml_diff>
--- a/dati_casoStudioItalia/altri_dati.xlsx
+++ b/dati_casoStudioItalia/altri_dati.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/gianvito_colucci_polito_it/Documents/Jobs/DRIN DRIN/Energy mix/DrinDrin---Mix-energetico/dati_casoStudioItalia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="503" documentId="8_{629DCDB6-94E5-432A-9179-03575796D74D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FA79E20-9E4E-41B0-A680-C53B0847AEF6}"/>
+  <xr:revisionPtr revIDLastSave="549" documentId="8_{629DCDB6-94E5-432A-9179-03575796D74D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E2B2D76-C037-4DB0-BDA6-721CF029CDB1}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{B845255D-815F-49EA-8438-49CAB31B3547}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{B845255D-815F-49EA-8438-49CAB31B3547}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -216,7 +216,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="62">
   <si>
     <t>value</t>
   </si>
@@ -387,6 +387,21 @@
   </si>
   <si>
     <t>Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno "storage duration" di 6 ore. Per ulteriori info, vedere questo paper</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>Average annual value, 2024</t>
+  </si>
+  <si>
+    <t>CAPEX eolico onshore</t>
+  </si>
+  <si>
+    <t>CAPEX eolico offshore</t>
+  </si>
+  <si>
+    <t>Average, 2020-2030</t>
   </si>
 </sst>
 </file>
@@ -906,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C372154-4B0A-49B9-8FF3-F49D60098BF7}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,10 +932,11 @@
     <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.85546875" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -930,112 +946,190 @@
       <c r="D1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="E1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" s="18">
+        <v>27.538556570687646</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D2" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B3" s="8">
+        <v>10.331146370574086</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="D3" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B5" s="8">
+        <v>918280</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="8">
+        <v>1063920</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="D6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="8">
+        <v>3082860</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C7" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" t="s">
+      <c r="B9" s="8"/>
+      <c r="C9" s="8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C9" t="s">
+      <c r="B10" s="8"/>
+      <c r="C10" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C10" t="s">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C11" t="s">
+      <c r="B12" s="8"/>
+      <c r="C12" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C12" t="s">
+      <c r="B13" s="8"/>
+      <c r="C13" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C13" t="s">
+      <c r="B14" s="8"/>
+      <c r="C14" s="8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C14" t="s">
+      <c r="B15" s="8"/>
+      <c r="C15" s="8" t="s">
         <v>10</v>
       </c>
+      <c r="D15" s="8"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{B66498B8-EE20-4806-A7DF-B085A43B81A8}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{B66BD1F3-C8A1-406D-BC7B-C4AD639B5C2B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1045,7 +1139,7 @@
   <dimension ref="A1:Y27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,7 +1147,8 @@
     <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="6" width="13.85546875" customWidth="1"/>
+    <col min="4" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
     <col min="9" max="9" width="18.140625" customWidth="1"/>
@@ -1585,7 +1680,7 @@
   <dimension ref="A1:T28"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
feat: Costo nuclear fuel, CAPEX nucleare, CAPEX batterie
</commit_message>
<xml_diff>
--- a/dati_casoStudioItalia/altri_dati.xlsx
+++ b/dati_casoStudioItalia/altri_dati.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/gianvito_colucci_polito_it/Documents/Jobs/DRIN DRIN/Energy mix/DrinDrin---Mix-energetico/dati_casoStudioItalia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="549" documentId="8_{629DCDB6-94E5-432A-9179-03575796D74D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E2B2D76-C037-4DB0-BDA6-721CF029CDB1}"/>
+  <xr:revisionPtr revIDLastSave="723" documentId="8_{629DCDB6-94E5-432A-9179-03575796D74D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC0ACA9E-59F6-4193-A55D-ECDFB74E3E8D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{B845255D-815F-49EA-8438-49CAB31B3547}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B845255D-815F-49EA-8438-49CAB31B3547}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -38,6 +38,40 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Gianvito Colucci</author>
+  </authors>
+  <commentList>
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{5CF03D84-CFD5-4BC9-8BE2-A62E05876F5C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gianvito Colucci:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+EUR/MW, da dividere per il tempo di carica/scarica del modello per passare a EUR/MWh</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Gianvito Colucci</author>
@@ -216,7 +250,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="81">
   <si>
     <t>value</t>
   </si>
@@ -371,12 +405,6 @@
     <t>Offshore acque profonde</t>
   </si>
   <si>
-    <t>LWR (credo sia AP1000)</t>
-  </si>
-  <si>
-    <t>SMR (credo sia AP1000)</t>
-  </si>
-  <si>
     <t>Comment 2</t>
   </si>
   <si>
@@ -386,9 +414,6 @@
     <t>Include il decommissioning</t>
   </si>
   <si>
-    <t>Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno "storage duration" di 6 ore. Per ulteriori info, vedere questo paper</t>
-  </si>
-  <si>
     <t>comment</t>
   </si>
   <si>
@@ -402,6 +427,72 @@
   </si>
   <si>
     <t>Average, 2020-2030</t>
+  </si>
+  <si>
+    <t>(M$2025/GW)</t>
+  </si>
+  <si>
+    <t>IAEA</t>
+  </si>
+  <si>
+    <t>Overnight cost suggerito da Lorenzo Mazzocco, portato dal 2020 al 2025 tramite inflazione di circa il 33% (vedi messaggio discord su Coordinamento energia)</t>
+  </si>
+  <si>
+    <t>EPR</t>
+  </si>
+  <si>
+    <t>2020 (EPR Francia)</t>
+  </si>
+  <si>
+    <t>EPR Francia</t>
+  </si>
+  <si>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>4h</t>
+  </si>
+  <si>
+    <t>Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno "storage duration" di 2 ore. Per ulteriori info, vedere questo paper</t>
+  </si>
+  <si>
+    <t>Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno "storage duration" di 4 ore. Per ulteriori info, vedere questo paper</t>
+  </si>
+  <si>
+    <t>Average 2h-4h, 2020-2030</t>
+  </si>
+  <si>
+    <t>(c$2021/kWh)</t>
+  </si>
+  <si>
+    <t>World Nuclear Association</t>
+  </si>
+  <si>
+    <t>€2020/$2021</t>
+  </si>
+  <si>
+    <t>SMR</t>
+  </si>
+  <si>
+    <t>AP1000</t>
+  </si>
+  <si>
+    <t>EIA</t>
+  </si>
+  <si>
+    <t>NREL</t>
+  </si>
+  <si>
+    <t>2020-2040</t>
+  </si>
+  <si>
+    <t>($2020/MWh)</t>
+  </si>
+  <si>
+    <t>Average between values found (2020-2021)</t>
+  </si>
+  <si>
+    <t>World Nuclear Association, EIA, NREL</t>
   </si>
 </sst>
 </file>
@@ -412,7 +503,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0E+00"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -491,6 +582,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -514,7 +619,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -584,6 +689,28 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -602,6 +729,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -920,23 +1051,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C372154-4B0A-49B9-8FF3-F49D60098BF7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C372154-4B0A-49B9-8FF3-F49D60098BF7}">
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -947,14 +1078,14 @@
         <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="18">
+      <c r="B2" s="23">
         <v>27.538556570687646</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -964,14 +1095,14 @@
         <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="23">
         <v>10.331146370574086</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -981,20 +1112,27 @@
         <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="23">
+        <v>4.8</v>
+      </c>
       <c r="C4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>1</v>
       </c>
@@ -1008,12 +1146,12 @@
         <v>37</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B6" s="8">
         <v>1063920</v>
@@ -1025,12 +1163,12 @@
         <v>37</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B7" s="8">
         <v>3082860</v>
@@ -1042,30 +1180,44 @@
         <v>37</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="8"/>
+      <c r="B8" s="8">
+        <v>3154360</v>
+      </c>
       <c r="C8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="8"/>
+      <c r="B9" s="30">
+        <v>1005598.9652225529</v>
+      </c>
       <c r="C9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
@@ -1073,9 +1225,10 @@
       <c r="C10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="8"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" s="6"/>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>13</v>
       </c>
@@ -1083,9 +1236,10 @@
       <c r="C11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="8"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11" s="6"/>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>14</v>
       </c>
@@ -1093,9 +1247,10 @@
       <c r="C12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="8"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D12" s="6"/>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>15</v>
       </c>
@@ -1103,9 +1258,10 @@
       <c r="C13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="8"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D13" s="6"/>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>16</v>
       </c>
@@ -1113,9 +1269,10 @@
       <c r="C14" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="8"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D14" s="6"/>
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>17</v>
       </c>
@@ -1123,14 +1280,17 @@
       <c r="C15" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="8"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{B66498B8-EE20-4806-A7DF-B085A43B81A8}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{B66BD1F3-C8A1-406D-BC7B-C4AD639B5C2B}"/>
+    <hyperlink ref="D8" r:id="rId3" xr:uid="{76843948-9A3E-4EB0-A540-24DF6B66F999}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -1138,27 +1298,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42806216-DB6B-4ED6-9AA4-BC1B162122E7}">
   <dimension ref="A1:Y27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16:G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" customWidth="1"/>
-    <col min="12" max="12" width="16.42578125" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" customWidth="1"/>
+    <col min="9" max="9" width="18.109375" customWidth="1"/>
+    <col min="12" max="12" width="16.44140625" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>41</v>
       </c>
@@ -1186,7 +1347,7 @@
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>18</v>
       </c>
@@ -1224,7 +1385,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>18</v>
       </c>
@@ -1264,7 +1425,7 @@
       <c r="W3" s="2"/>
       <c r="Y3" s="6"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>18</v>
       </c>
@@ -1300,7 +1461,7 @@
       <c r="W4" s="2"/>
       <c r="Y4" s="4"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>18</v>
       </c>
@@ -1336,7 +1497,7 @@
       <c r="W5" s="2"/>
       <c r="Y5" s="5"/>
     </row>
-    <row r="6" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>18</v>
       </c>
@@ -1373,7 +1534,7 @@
       </c>
       <c r="Y6" s="10"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>18</v>
       </c>
@@ -1399,10 +1560,18 @@
       <c r="H7" t="s">
         <v>34</v>
       </c>
-      <c r="M7" s="13"/>
+      <c r="L7" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="M7" s="11">
+        <v>0.82</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="Y7" s="10"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>18</v>
       </c>
@@ -1428,10 +1597,18 @@
       <c r="H8" t="s">
         <v>34</v>
       </c>
-      <c r="M8" s="13"/>
+      <c r="L8" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="M8" s="11">
+        <v>0.88</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="Y8" s="10"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>19</v>
       </c>
@@ -1460,7 +1637,7 @@
       <c r="M9" s="13"/>
       <c r="Y9" s="10"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>19</v>
       </c>
@@ -1489,7 +1666,7 @@
       <c r="M10" s="13"/>
       <c r="Y10" s="10"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>19</v>
       </c>
@@ -1518,7 +1695,7 @@
       <c r="M11" s="13"/>
       <c r="Y11" s="10"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>19</v>
       </c>
@@ -1547,7 +1724,7 @@
       <c r="M12" s="13"/>
       <c r="Y12" s="10"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>19</v>
       </c>
@@ -1576,7 +1753,7 @@
       <c r="M13" s="13"/>
       <c r="Y13" s="10"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
         <v>19</v>
       </c>
@@ -1605,7 +1782,7 @@
       <c r="M14" s="13"/>
       <c r="Y14" s="10"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>19</v>
       </c>
@@ -1634,26 +1811,99 @@
       <c r="M15" s="13"/>
       <c r="Y15" s="10"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="20">
+        <v>2021</v>
+      </c>
+      <c r="C16" s="21">
+        <v>0.46</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" s="9">
+        <f>C16*M7/100*1000</f>
+        <v>3.7719999999999998</v>
+      </c>
+      <c r="H16" t="s">
+        <v>34</v>
+      </c>
       <c r="M16" s="13"/>
       <c r="Y16" s="4"/>
     </row>
-    <row r="17" spans="13:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="21">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="G17" s="9">
+        <f>C17*M7</f>
+        <v>5.7399999999999993</v>
+      </c>
+      <c r="H17" t="s">
+        <v>34</v>
+      </c>
       <c r="M17" s="13"/>
       <c r="Y17" s="5"/>
     </row>
-    <row r="18" spans="13:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="20">
+        <v>2021</v>
+      </c>
+      <c r="C18" s="21">
+        <v>0.61</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="G18" s="9">
+        <f>C18*M7/100*1000</f>
+        <v>5.0019999999999998</v>
+      </c>
+      <c r="H18" t="s">
+        <v>34</v>
+      </c>
       <c r="M18" s="13"/>
       <c r="Y18" s="9"/>
     </row>
-    <row r="19" spans="13:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="M19" s="13"/>
       <c r="Y19" s="9"/>
     </row>
-    <row r="20" spans="13:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="E20" s="22"/>
       <c r="Y20" s="9"/>
     </row>
-    <row r="27" spans="13:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="E21" s="24"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="E22" s="31"/>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="Q27" s="17"/>
       <c r="R27" s="9"/>
       <c r="S27" s="9"/>
@@ -1669,36 +1919,41 @@
     <hyperlink ref="E7" r:id="rId7" xr:uid="{DE760FD1-0CEE-4185-9625-11A99D9355EA}"/>
     <hyperlink ref="E8" r:id="rId8" xr:uid="{A6CF3B73-709A-4F91-97B5-6A913B5528DA}"/>
     <hyperlink ref="E9:E15" r:id="rId9" display="World Bank" xr:uid="{80874292-EDDF-4056-827D-D7F6914B6036}"/>
+    <hyperlink ref="E16" r:id="rId10" xr:uid="{0A15B76E-514E-4B75-ACAD-E2793D18E38A}"/>
+    <hyperlink ref="N7" r:id="rId11" xr:uid="{A37BA78B-11DC-41F6-ACA1-CD3B620CB840}"/>
+    <hyperlink ref="E18" r:id="rId12" xr:uid="{CE540549-CF28-48F8-B699-8C84C681D4A9}"/>
+    <hyperlink ref="E17" r:id="rId13" display="Dati elaborati da NREL" xr:uid="{FA34371D-7714-4F4E-BC99-DC72274713CD}"/>
+    <hyperlink ref="N8" r:id="rId14" xr:uid="{B5C929D6-B267-4086-B524-D47FDFA68A60}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId10"/>
+  <legacyDrawing r:id="rId15"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F958822-C8DD-4CF0-BC79-5189EFFDF89D}">
-  <dimension ref="A1:T28"/>
+  <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3:R3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="27.140625" customWidth="1"/>
-    <col min="8" max="8" width="42.7109375" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="27.109375" customWidth="1"/>
+    <col min="8" max="8" width="42.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" customWidth="1"/>
+    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>41</v>
       </c>
@@ -1718,10 +1973,10 @@
         <v>26</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>43</v>
@@ -1730,7 +1985,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -1753,7 +2008,7 @@
         <v>44</v>
       </c>
       <c r="H2" s="24"/>
-      <c r="I2" s="8">
+      <c r="I2" s="23">
         <f>D2*$Q$3*10^3</f>
         <v>1173040</v>
       </c>
@@ -1770,7 +2025,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
@@ -1793,7 +2048,7 @@
         <v>44</v>
       </c>
       <c r="H3" s="24"/>
-      <c r="I3" s="8">
+      <c r="I3" s="23">
         <f t="shared" ref="I3:I8" si="0">D3*$Q$3*10^3</f>
         <v>663520</v>
       </c>
@@ -1810,7 +2065,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
@@ -1833,7 +2088,7 @@
         <v>44</v>
       </c>
       <c r="H4" s="24"/>
-      <c r="I4" s="8">
+      <c r="I4" s="23">
         <f t="shared" si="0"/>
         <v>1286560</v>
       </c>
@@ -1841,7 +2096,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
@@ -1864,7 +2119,7 @@
         <v>44</v>
       </c>
       <c r="H5" s="24"/>
-      <c r="I5" s="8">
+      <c r="I5" s="23">
         <f t="shared" si="0"/>
         <v>841280</v>
       </c>
@@ -1872,7 +2127,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>5</v>
       </c>
@@ -1895,7 +2150,7 @@
         <v>44</v>
       </c>
       <c r="H6" s="24"/>
-      <c r="I6" s="8">
+      <c r="I6" s="23">
         <f t="shared" si="0"/>
         <v>3290320</v>
       </c>
@@ -1903,7 +2158,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
@@ -1926,7 +2181,7 @@
         <v>44</v>
       </c>
       <c r="H7" s="24"/>
-      <c r="I7" s="8">
+      <c r="I7" s="23">
         <f t="shared" si="0"/>
         <v>2427040</v>
       </c>
@@ -1934,7 +2189,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>5</v>
       </c>
@@ -1957,7 +2212,7 @@
         <v>44</v>
       </c>
       <c r="H8" s="24"/>
-      <c r="I8" s="8">
+      <c r="I8" s="23">
         <f t="shared" si="0"/>
         <v>3563120</v>
       </c>
@@ -1965,7 +2220,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>5</v>
       </c>
@@ -1988,7 +2243,7 @@
         <v>44</v>
       </c>
       <c r="H9" s="24"/>
-      <c r="I9" s="8">
+      <c r="I9" s="23">
         <f>D9*$Q$3*10^3</f>
         <v>3050960</v>
       </c>
@@ -1996,12 +2251,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="C10" s="8">
         <v>2035</v>
@@ -2019,22 +2274,22 @@
         <v>44</v>
       </c>
       <c r="H10" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="I10" s="8">
-        <f t="shared" ref="I10:I16" si="1">D10*$Q$3*10^3</f>
+        <v>53</v>
+      </c>
+      <c r="I10" s="23">
+        <f t="shared" ref="I10:I17" si="1">D10*$Q$3*10^3</f>
         <v>5420800.0000000009</v>
       </c>
       <c r="J10" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="C11" s="8">
         <v>2050</v>
@@ -2052,9 +2307,9 @@
         <v>44</v>
       </c>
       <c r="H11" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="I11" s="8">
+        <v>53</v>
+      </c>
+      <c r="I11" s="23">
         <f t="shared" si="1"/>
         <v>4840000</v>
       </c>
@@ -2062,12 +2317,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="C12" s="8">
         <v>2035</v>
@@ -2085,9 +2340,9 @@
         <v>44</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="I12" s="8">
+        <v>53</v>
+      </c>
+      <c r="I12" s="23">
         <f t="shared" si="1"/>
         <v>6001600.0000000009</v>
       </c>
@@ -2095,12 +2350,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="C13" s="8">
         <v>2050</v>
@@ -2118,9 +2373,9 @@
         <v>44</v>
       </c>
       <c r="H13" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="I13" s="8">
+        <v>53</v>
+      </c>
+      <c r="I13" s="23">
         <f t="shared" si="1"/>
         <v>5324000.0000000009</v>
       </c>
@@ -2128,50 +2383,51 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="8"/>
+        <v>6</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>62</v>
+      </c>
       <c r="C14" s="8">
-        <v>2020</v>
-      </c>
-      <c r="D14" s="18">
-        <v>2466</v>
+        <v>2025</v>
+      </c>
+      <c r="D14" s="23">
+        <v>5350</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G14" s="24" t="s">
-        <v>44</v>
+        <v>59</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" s="25" t="s">
+        <v>64</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="I14" s="8">
-        <f t="shared" si="1"/>
-        <v>2170080</v>
+        <v>61</v>
+      </c>
+      <c r="I14" s="23">
+        <f>D14*$Q$3*10^3*0.67</f>
+        <v>3154360</v>
       </c>
       <c r="J14" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="R14" s="2"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6"/>
-    </row>
-    <row r="15" spans="1:20" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:20" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="8"/>
+      <c r="B15" s="8" t="s">
+        <v>65</v>
+      </c>
       <c r="C15" s="8">
-        <v>2030</v>
-      </c>
-      <c r="D15" s="18">
-        <v>1210</v>
+        <v>2020</v>
+      </c>
+      <c r="D15" s="28">
+        <v>988.32170015695567</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>36</v>
@@ -2183,29 +2439,31 @@
         <v>44</v>
       </c>
       <c r="H15" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="I15" s="8">
+        <v>67</v>
+      </c>
+      <c r="I15" s="23">
         <f t="shared" si="1"/>
-        <v>1064800</v>
+        <v>869723.09613812109</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>45</v>
       </c>
       <c r="R15" s="2"/>
-      <c r="S15" s="4"/>
-      <c r="T15" s="4"/>
-    </row>
-    <row r="16" spans="1:20" ht="75" x14ac:dyDescent="0.25">
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+    </row>
+    <row r="16" spans="1:20" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="8"/>
+      <c r="B16" s="8" t="s">
+        <v>65</v>
+      </c>
       <c r="C16" s="8">
-        <v>2050</v>
-      </c>
-      <c r="D16" s="18">
-        <v>908</v>
+        <v>2030</v>
+      </c>
+      <c r="D16" s="28">
+        <v>681.62247956991291</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>36</v>
@@ -2217,76 +2475,163 @@
         <v>44</v>
       </c>
       <c r="H16" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="I16" s="8">
+        <v>67</v>
+      </c>
+      <c r="I16" s="23">
         <f t="shared" si="1"/>
-        <v>799040</v>
+        <v>599827.78202152334</v>
       </c>
       <c r="J16" s="8" t="s">
         <v>45</v>
       </c>
       <c r="R16" s="2"/>
-      <c r="S16" s="5"/>
-      <c r="T16" s="5"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="S17" s="9"/>
-      <c r="T17" s="10"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+    </row>
+    <row r="17" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="8">
+        <v>2050</v>
+      </c>
+      <c r="D17" s="29">
+        <v>681.62247956991291</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="I17" s="23">
+        <f t="shared" si="1"/>
+        <v>599827.78202152334</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="R17" s="2"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+    </row>
+    <row r="18" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="8">
+        <v>2020</v>
+      </c>
+      <c r="D18" s="28">
+        <v>1727.2344448095646</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="I18" s="23">
+        <f t="shared" ref="I18:I20" si="2">D18*$Q$3*10^3</f>
+        <v>1519966.3114324168</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>45</v>
+      </c>
       <c r="S18" s="9"/>
       <c r="T18" s="10"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="8">
+        <v>2030</v>
+      </c>
+      <c r="D19" s="28">
+        <v>1173.7257628388072</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G19" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="I19" s="23">
+        <f t="shared" si="2"/>
+        <v>1032878.6712981503</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="S19" s="9"/>
+      <c r="T19" s="10"/>
+    </row>
+    <row r="20" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="8">
+        <v>2050</v>
+      </c>
+      <c r="D20" s="29">
+        <v>1173.7257628388072</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="I20" s="23">
+        <f t="shared" si="2"/>
+        <v>1032878.6712981503</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
-      <c r="D21" s="18"/>
+      <c r="D21" s="28"/>
       <c r="E21" s="1"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
@@ -2294,7 +2639,7 @@
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -2303,10 +2648,13 @@
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
+      <c r="I22" s="23">
+        <f>AVERAGE(I18,I19,I15,I16)</f>
+        <v>1005598.9652225529</v>
+      </c>
       <c r="J22" s="8"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -2318,7 +2666,7 @@
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -2330,7 +2678,7 @@
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -2342,7 +2690,7 @@
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -2354,7 +2702,7 @@
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
@@ -2366,7 +2714,7 @@
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
@@ -2377,6 +2725,18 @@
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2401,15 +2761,27 @@
     <hyperlink ref="F12" r:id="rId19" display="World Bank" xr:uid="{0EE4B772-3B1C-40C1-8489-D0631B2D4463}"/>
     <hyperlink ref="F13" r:id="rId20" display="World Bank" xr:uid="{C22641C2-FA38-48D9-BCB2-1FCE72A643D6}"/>
     <hyperlink ref="G10" r:id="rId21" xr:uid="{1BCFB97B-FADB-43D9-B44E-ADA05CA17A73}"/>
-    <hyperlink ref="F14" r:id="rId22" display="World Bank" xr:uid="{AF15079B-1809-4BD8-A648-4D62ABE8C206}"/>
-    <hyperlink ref="G14" r:id="rId23" xr:uid="{0CA73A59-1222-47DA-A59D-000D8B582034}"/>
-    <hyperlink ref="F15" r:id="rId24" display="World Bank" xr:uid="{199C7D2F-21A1-4692-9440-4CC169B6F2F2}"/>
-    <hyperlink ref="G15" r:id="rId25" xr:uid="{CECC446B-999A-4D89-A0D6-D3177C929A3D}"/>
-    <hyperlink ref="F16" r:id="rId26" display="World Bank" xr:uid="{8716B52B-0C43-4E99-8CCE-17C58FE13622}"/>
-    <hyperlink ref="G16" r:id="rId27" xr:uid="{85050209-E008-45C2-8A24-F79F70751A59}"/>
+    <hyperlink ref="F15" r:id="rId22" display="World Bank" xr:uid="{AF15079B-1809-4BD8-A648-4D62ABE8C206}"/>
+    <hyperlink ref="G15" r:id="rId23" xr:uid="{0CA73A59-1222-47DA-A59D-000D8B582034}"/>
+    <hyperlink ref="F16" r:id="rId24" display="World Bank" xr:uid="{199C7D2F-21A1-4692-9440-4CC169B6F2F2}"/>
+    <hyperlink ref="G16" r:id="rId25" xr:uid="{CECC446B-999A-4D89-A0D6-D3177C929A3D}"/>
+    <hyperlink ref="F17" r:id="rId26" display="World Bank" xr:uid="{8716B52B-0C43-4E99-8CCE-17C58FE13622}"/>
+    <hyperlink ref="G17" r:id="rId27" xr:uid="{85050209-E008-45C2-8A24-F79F70751A59}"/>
     <hyperlink ref="G11:G13" r:id="rId28" display="Dati elaborati da NREL" xr:uid="{8CAF9D49-1D95-457A-AD06-EF2B25EC7C48}"/>
-    <hyperlink ref="H14" r:id="rId29" xr:uid="{BD06F35F-2859-4868-A250-9877196A2A8B}"/>
-    <hyperlink ref="H15:H16" r:id="rId30" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{D5926397-0CC0-4EED-B446-ADD3939AFBF8}"/>
+    <hyperlink ref="H15" r:id="rId29" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{BD06F35F-2859-4868-A250-9877196A2A8B}"/>
+    <hyperlink ref="H16:H17" r:id="rId30" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{D5926397-0CC0-4EED-B446-ADD3939AFBF8}"/>
+    <hyperlink ref="R3" r:id="rId31" xr:uid="{1F188A66-AA31-42D5-BF68-5F94EC7F5B80}"/>
+    <hyperlink ref="F14" r:id="rId32" xr:uid="{BBB5C12E-09F8-42A0-BC0B-98E2FE229F3F}"/>
+    <hyperlink ref="H14" r:id="rId33" display="Overnight cost, suggerito da Lorenzo Mazzocco (vedi messaggio discord su Coordinamento energia)" xr:uid="{7623CF7E-7357-466F-811C-79E8E0B20885}"/>
+    <hyperlink ref="F18" r:id="rId34" display="World Bank" xr:uid="{A46629F6-B5CF-4B20-92CC-DAAA37FA0295}"/>
+    <hyperlink ref="G18" r:id="rId35" xr:uid="{4C8330BE-8E6C-45DA-8011-98C7288331BF}"/>
+    <hyperlink ref="H18" r:id="rId36" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{DBA68ACF-849E-462B-8CC2-2BE6A9705126}"/>
+    <hyperlink ref="F19" r:id="rId37" display="World Bank" xr:uid="{E1E46D67-8566-4081-8026-9282FEEA7794}"/>
+    <hyperlink ref="F20" r:id="rId38" display="World Bank" xr:uid="{C2B4C806-3E78-4AEF-A359-42B49AF6C869}"/>
+    <hyperlink ref="G19" r:id="rId39" xr:uid="{A07DD3DB-85F5-450E-BE7A-F242BAF7D635}"/>
+    <hyperlink ref="G20" r:id="rId40" xr:uid="{CB5BF0A4-3E46-40DE-9A2B-D68DCB0772EB}"/>
+    <hyperlink ref="H19" r:id="rId41" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{2364EE2D-C0F7-4609-B6E2-FD4BE059C070}"/>
+    <hyperlink ref="H20" r:id="rId42" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{222C5FBD-1584-4E8E-8AE1-8423CB925839}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Coded update_technology_cost, added definition of techs per node instead of global
</commit_message>
<xml_diff>
--- a/dati_casoStudioItalia/altri_dati.xlsx
+++ b/dati_casoStudioItalia/altri_dati.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/gianvito_colucci_polito_it/Documents/Jobs/DRIN DRIN/Energy mix/DrinDrin---Mix-energetico/dati_casoStudioItalia/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DrinDrin\dati_casoStudioItalia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="723" documentId="8_{629DCDB6-94E5-432A-9179-03575796D74D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC0ACA9E-59F6-4193-A55D-ECDFB74E3E8D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7477C9-189D-4E68-9F97-E7E8A462E5F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B845255D-815F-49EA-8438-49CAB31B3547}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B845255D-815F-49EA-8438-49CAB31B3547}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
-    <sheet name="raw_data_commodity" sheetId="2" r:id="rId2"/>
-    <sheet name="raw_data_techs" sheetId="3" r:id="rId3"/>
+    <sheet name="CAPEX" sheetId="1" r:id="rId1"/>
+    <sheet name="Fuel_cost" sheetId="5" r:id="rId2"/>
+    <sheet name="Transmission_abroad" sheetId="4" r:id="rId3"/>
+    <sheet name="raw_data_commodity" sheetId="2" r:id="rId4"/>
+    <sheet name="raw_data_techs" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,10 +42,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Gianvito Colucci</author>
+    <author>Bertoni, L. (Luca)</author>
   </authors>
   <commentList>
-    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{5CF03D84-CFD5-4BC9-8BE2-A62E05876F5C}">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{52950CF3-9BD0-40D6-94D2-8E0C1D67B00B}">
       <text>
         <r>
           <rPr>
@@ -53,7 +55,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Gianvito Colucci:</t>
+          <t>Bertoni, L. (Luca):</t>
         </r>
         <r>
           <rPr>
@@ -63,7 +65,57 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-EUR/MW, da dividere per il tempo di carica/scarica del modello per passare a EUR/MWh</t>
+in MWh
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{6042687D-A9B5-4779-9A54-E22AF9FBB252}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bertoni, L. (Luca):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Tutti I tipi</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{ACE5EF51-CB51-4DAB-B6B4-87E92D626050}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bertoni, L. (Luca):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+in MWh
+</t>
         </r>
       </text>
     </comment>
@@ -250,7 +302,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="87">
   <si>
     <t>value</t>
   </si>
@@ -285,21 +337,9 @@
     <t>EUR/MWh</t>
   </si>
   <si>
-    <t>Trasmissione Francia</t>
-  </si>
-  <si>
     <t>MW</t>
   </si>
   <si>
-    <t>Trasmissione Svizzera</t>
-  </si>
-  <si>
-    <t>Trasmissione Austria</t>
-  </si>
-  <si>
-    <t>Trasmissione Slovenia</t>
-  </si>
-  <si>
     <t xml:space="preserve">Prezzo import </t>
   </si>
   <si>
@@ -420,12 +460,6 @@
     <t>Average annual value, 2024</t>
   </si>
   <si>
-    <t>CAPEX eolico onshore</t>
-  </si>
-  <si>
-    <t>CAPEX eolico offshore</t>
-  </si>
-  <si>
     <t>Average, 2020-2030</t>
   </si>
   <si>
@@ -493,6 +527,42 @@
   </si>
   <si>
     <t>World Nuclear Association, EIA, NREL</t>
+  </si>
+  <si>
+    <t>CAPEX</t>
+  </si>
+  <si>
+    <t>Hydro_Reservoir</t>
+  </si>
+  <si>
+    <t>GasTurbine_simple</t>
+  </si>
+  <si>
+    <t>Photovoltaic</t>
+  </si>
+  <si>
+    <t>CoalPlant</t>
+  </si>
+  <si>
+    <t>Storage_Battery</t>
+  </si>
+  <si>
+    <t>PumpedHydro_Closed</t>
+  </si>
+  <si>
+    <t>NuclearPlant</t>
+  </si>
+  <si>
+    <t>Trasmissione tot NORD</t>
+  </si>
+  <si>
+    <t>electricity map</t>
+  </si>
+  <si>
+    <t>Include francia, svizzera, slovenia, austria</t>
+  </si>
+  <si>
+    <t>WindTurbine_Onshore_4000</t>
   </si>
 </sst>
 </file>
@@ -503,7 +573,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0E+00"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -578,13 +648,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -702,15 +765,15 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -729,10 +792,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1052,10 +1111,139 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C372154-4B0A-49B9-8FF3-F49D60098BF7}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="8">
+        <v>918280</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1063920</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="8">
+        <v>3154360</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="33">
+        <f>1005598.96522255*0.3</f>
+        <v>301679.68956676498</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{76843948-9A3E-4EB0-A540-24DF6B66F999}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F36F9B7-E410-4418-9AFE-4DC5A9893242}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1078,12 +1266,12 @@
         <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B2" s="23">
         <v>27.538556570687646</v>
@@ -1092,15 +1280,15 @@
         <v>3</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B3" s="23">
         <v>10.331146370574086</v>
@@ -1109,10 +1297,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.3">
@@ -1125,176 +1313,98 @@
       <c r="C4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="33" t="s">
-        <v>80</v>
+      <c r="D4" s="32" t="s">
+        <v>74</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="8">
-        <v>918280</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="8">
-        <v>1063920</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" s="8">
-        <v>3082860</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="8">
-        <v>3154360</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" s="27" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="30">
-        <v>1005598.9652225529</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="8"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="8"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="8"/>
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{B66498B8-EE20-4806-A7DF-B085A43B81A8}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{B66BD1F3-C8A1-406D-BC7B-C4AD639B5C2B}"/>
-    <hyperlink ref="D8" r:id="rId3" xr:uid="{76843948-9A3E-4EB0-A540-24DF6B66F999}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{899EB925-18FE-4D0F-90A7-19454D63E70C}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{8C713812-7D41-41B1-95A2-AD8C3456DC0C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25E773EF-BD6E-41C4-818D-318BE958C680}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="8">
+        <v>10138</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42806216-DB6B-4ED6-9AA4-BC1B162122E7}">
   <dimension ref="A1:Y27"/>
   <sheetViews>
@@ -1321,35 +1431,35 @@
   <sheetData>
     <row r="1" spans="1:25" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B2" s="20">
         <v>2018</v>
@@ -1358,36 +1468,36 @@
         <v>7.5414094383199997</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G2" s="9">
         <f t="shared" ref="G2:G8" si="0">C2*$M$3/$M$4</f>
         <v>21.805545521741941</v>
       </c>
       <c r="H2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B3" s="20">
         <v>2019</v>
@@ -1396,38 +1506,38 @@
         <v>4.8274540271299999</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G3" s="9">
         <f t="shared" si="0"/>
         <v>13.958301747657082</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
       <c r="L3" s="15" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="M3" s="11">
         <v>0.85</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="W3" s="2"/>
       <c r="Y3" s="6"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B4" s="20">
         <v>2020</v>
@@ -1436,23 +1546,23 @@
         <v>3.3115669452400409</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G4" s="9">
         <f t="shared" si="0"/>
         <v>9.5752026677938797</v>
       </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="L4" s="15" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="M4" s="12">
         <v>0.29397099999999998</v>
@@ -1463,7 +1573,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B5" s="20">
         <v>2021</v>
@@ -1472,23 +1582,23 @@
         <v>14.731149861407678</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G5" s="9">
         <f t="shared" si="0"/>
         <v>42.594260597802254</v>
       </c>
       <c r="H5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="L5" s="15" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="M5" s="14">
         <f>1.622*10^-6</f>
@@ -1499,7 +1609,7 @@
     </row>
     <row r="6" spans="1:25" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B6" s="20">
         <v>2022</v>
@@ -1508,35 +1618,35 @@
         <v>34.346664233461041</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G6" s="9">
         <f t="shared" si="0"/>
         <v>99.311376286919071</v>
       </c>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="M6" s="11">
         <v>6000</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="Y6" s="10"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B7" s="20">
         <v>2023</v>
@@ -1545,35 +1655,35 @@
         <v>11.492903809114813</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G7" s="9">
         <f t="shared" si="0"/>
         <v>33.23106101536407</v>
       </c>
       <c r="H7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="L7" s="15" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="M7" s="11">
         <v>0.82</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="Y7" s="10"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B8" s="20">
         <v>2024</v>
@@ -1582,35 +1692,35 @@
         <v>9.52416119251955</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G8" s="9">
         <f t="shared" si="0"/>
         <v>27.538556570687646</v>
       </c>
       <c r="H8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="L8" s="15" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="M8" s="11">
         <v>0.88</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="Y8" s="10"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B9" s="20">
         <v>2018</v>
@@ -1619,27 +1729,27 @@
         <v>105.06823090515999</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G9" s="9">
         <f t="shared" ref="G9:G15" si="1">C9*$M$3/$M$6/$M$5/1000</f>
         <v>9.1767361559171796</v>
       </c>
       <c r="H9" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="M9" s="13"/>
       <c r="Y9" s="10"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B10" s="20">
         <v>2019</v>
@@ -1648,27 +1758,27 @@
         <v>78.292956708220004</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G10" s="9">
         <f t="shared" si="1"/>
         <v>6.8381641185765512</v>
       </c>
       <c r="H10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="M10" s="13"/>
       <c r="Y10" s="10"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B11" s="20">
         <v>2020</v>
@@ -1677,27 +1787,27 @@
         <v>62.08886618998978</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G11" s="9">
         <f t="shared" si="1"/>
         <v>5.4228869976871463</v>
       </c>
       <c r="H11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="M11" s="13"/>
       <c r="Y11" s="10"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B12" s="20">
         <v>2021</v>
@@ -1706,27 +1816,27 @@
         <v>126.18829981718464</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G12" s="9">
         <f t="shared" si="1"/>
         <v>11.021378426285136</v>
       </c>
       <c r="H12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="M12" s="13"/>
       <c r="Y12" s="10"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B13" s="20">
         <v>2022</v>
@@ -1735,27 +1845,27 @@
         <v>293.6511990918093</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G13" s="9">
         <f t="shared" si="1"/>
         <v>25.647710565971831</v>
       </c>
       <c r="H13" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="M13" s="13"/>
       <c r="Y13" s="10"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B14" s="20">
         <v>2023</v>
@@ -1764,27 +1874,27 @@
         <v>151.42784107508328</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G14" s="9">
         <f t="shared" si="1"/>
         <v>13.225818425176818</v>
       </c>
       <c r="H14" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="M14" s="13"/>
       <c r="Y14" s="10"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B15" s="20">
         <v>2024</v>
@@ -1793,20 +1903,20 @@
         <v>118.28554879814943</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G15" s="9">
         <f t="shared" si="1"/>
         <v>10.331146370574086</v>
       </c>
       <c r="H15" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="M15" s="13"/>
       <c r="Y15" s="10"/>
@@ -1822,17 +1932,17 @@
         <v>0.46</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="G16" s="9">
         <f>C16*M7/100*1000</f>
         <v>3.7719999999999998</v>
       </c>
       <c r="H16" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="M16" s="13"/>
       <c r="Y16" s="4"/>
@@ -1841,24 +1951,24 @@
       <c r="A17" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="32" t="s">
-        <v>77</v>
+      <c r="B17" s="31" t="s">
+        <v>71</v>
       </c>
       <c r="C17" s="21">
         <v>7</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G17" s="9">
         <f>C17*M7</f>
         <v>5.7399999999999993</v>
       </c>
       <c r="H17" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="M17" s="13"/>
       <c r="Y17" s="5"/>
@@ -1874,17 +1984,17 @@
         <v>0.61</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G18" s="9">
         <f>C18*M7/100*1000</f>
         <v>5.0019999999999998</v>
       </c>
       <c r="H18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="M18" s="13"/>
       <c r="Y18" s="9"/>
@@ -1901,7 +2011,7 @@
       <c r="E21" s="24"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="E22" s="31"/>
+      <c r="E22" s="30"/>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="Q27" s="17"/>
@@ -1930,7 +2040,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F958822-C8DD-4CF0-BC79-5189EFFDF89D}">
   <dimension ref="A1:T29"/>
   <sheetViews>
@@ -1955,34 +2065,34 @@
   <sheetData>
     <row r="1" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="J1" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
@@ -1990,7 +2100,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C2" s="8">
         <v>2020</v>
@@ -1999,13 +2109,13 @@
         <v>1333</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H2" s="24"/>
       <c r="I2" s="23">
@@ -2013,16 +2123,16 @@
         <v>1173040</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
@@ -2030,7 +2140,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C3" s="8">
         <v>2030</v>
@@ -2039,13 +2149,13 @@
         <v>754</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H3" s="24"/>
       <c r="I3" s="23">
@@ -2053,16 +2163,16 @@
         <v>663520</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="P3" s="15" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="Q3" s="11">
         <v>0.88</v>
       </c>
       <c r="R3" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
@@ -2070,7 +2180,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C4" s="8">
         <v>2020</v>
@@ -2079,13 +2189,13 @@
         <v>1462</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H4" s="24"/>
       <c r="I4" s="23">
@@ -2093,7 +2203,7 @@
         <v>1286560</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
@@ -2101,7 +2211,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C5" s="8">
         <v>2030</v>
@@ -2110,13 +2220,13 @@
         <v>956</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H5" s="24"/>
       <c r="I5" s="23">
@@ -2124,7 +2234,7 @@
         <v>841280</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
@@ -2132,7 +2242,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C6" s="8">
         <v>2020</v>
@@ -2141,13 +2251,13 @@
         <v>3739</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H6" s="24"/>
       <c r="I6" s="23">
@@ -2155,7 +2265,7 @@
         <v>3290320</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
@@ -2163,7 +2273,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C7" s="8">
         <v>2030</v>
@@ -2172,13 +2282,13 @@
         <v>2758</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H7" s="24"/>
       <c r="I7" s="23">
@@ -2186,7 +2296,7 @@
         <v>2427040</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
@@ -2194,7 +2304,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C8" s="8">
         <v>2020</v>
@@ -2203,13 +2313,13 @@
         <v>4049</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H8" s="24"/>
       <c r="I8" s="23">
@@ -2217,7 +2327,7 @@
         <v>3563120</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
@@ -2225,7 +2335,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C9" s="8">
         <v>2030</v>
@@ -2234,13 +2344,13 @@
         <v>3467</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H9" s="24"/>
       <c r="I9" s="23">
@@ -2248,7 +2358,7 @@
         <v>3050960</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
@@ -2256,7 +2366,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C10" s="8">
         <v>2035</v>
@@ -2265,23 +2375,23 @@
         <v>6160.0000000000009</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G10" s="24" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H10" s="25" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I10" s="23">
         <f t="shared" ref="I10:I17" si="1">D10*$Q$3*10^3</f>
         <v>5420800.0000000009</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
@@ -2289,7 +2399,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C11" s="8">
         <v>2050</v>
@@ -2298,23 +2408,23 @@
         <v>5500</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G11" s="24" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H11" s="25" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I11" s="23">
         <f t="shared" si="1"/>
         <v>4840000</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
@@ -2322,7 +2432,7 @@
         <v>6</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C12" s="8">
         <v>2035</v>
@@ -2331,23 +2441,23 @@
         <v>6820.0000000000009</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G12" s="24" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I12" s="23">
         <f t="shared" si="1"/>
         <v>6001600.0000000009</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
@@ -2355,7 +2465,7 @@
         <v>6</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C13" s="8">
         <v>2050</v>
@@ -2364,23 +2474,23 @@
         <v>6050.0000000000009</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G13" s="24" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H13" s="25" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I13" s="23">
         <f t="shared" si="1"/>
         <v>5324000.0000000009</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
@@ -2388,7 +2498,7 @@
         <v>6</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C14" s="8">
         <v>2025</v>
@@ -2397,23 +2507,23 @@
         <v>5350</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F14" s="26" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="G14" s="25" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="I14" s="23">
         <f>D14*$Q$3*10^3*0.67</f>
         <v>3154360</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="72" x14ac:dyDescent="0.3">
@@ -2421,7 +2531,7 @@
         <v>7</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C15" s="8">
         <v>2020</v>
@@ -2430,23 +2540,23 @@
         <v>988.32170015695567</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H15" s="24" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="I15" s="23">
         <f t="shared" si="1"/>
         <v>869723.09613812109</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="R15" s="2"/>
       <c r="S15" s="6"/>
@@ -2457,7 +2567,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C16" s="8">
         <v>2030</v>
@@ -2466,23 +2576,23 @@
         <v>681.62247956991291</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H16" s="24" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="I16" s="23">
         <f t="shared" si="1"/>
         <v>599827.78202152334</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="R16" s="2"/>
       <c r="S16" s="4"/>
@@ -2493,7 +2603,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C17" s="8">
         <v>2050</v>
@@ -2502,23 +2612,23 @@
         <v>681.62247956991291</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H17" s="24" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="I17" s="23">
         <f t="shared" si="1"/>
         <v>599827.78202152334</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="R17" s="2"/>
       <c r="S17" s="5"/>
@@ -2529,7 +2639,7 @@
         <v>7</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C18" s="8">
         <v>2020</v>
@@ -2538,23 +2648,23 @@
         <v>1727.2344448095646</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G18" s="24" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H18" s="24" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="I18" s="23">
         <f t="shared" ref="I18:I20" si="2">D18*$Q$3*10^3</f>
         <v>1519966.3114324168</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="S18" s="9"/>
       <c r="T18" s="10"/>
@@ -2564,7 +2674,7 @@
         <v>7</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C19" s="8">
         <v>2030</v>
@@ -2573,23 +2683,23 @@
         <v>1173.7257628388072</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H19" s="24" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="I19" s="23">
         <f t="shared" si="2"/>
         <v>1032878.6712981503</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="S19" s="9"/>
       <c r="T19" s="10"/>
@@ -2599,7 +2709,7 @@
         <v>7</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C20" s="8">
         <v>2050</v>
@@ -2608,23 +2718,23 @@
         <v>1173.7257628388072</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H20" s="24" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="I20" s="23">
         <f t="shared" si="2"/>
         <v>1032878.6712981503</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
feat: CAPEX gas (ciclo combinato) e carbone (ciclo a vapore)
</commit_message>
<xml_diff>
--- a/dati_casoStudioItalia/altri_dati.xlsx
+++ b/dati_casoStudioItalia/altri_dati.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/gianvito_colucci_polito_it/Documents/Jobs/DRIN DRIN/Energy mix/DrinDrin---Mix-energetico/dati_casoStudioItalia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="723" documentId="8_{629DCDB6-94E5-432A-9179-03575796D74D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC0ACA9E-59F6-4193-A55D-ECDFB74E3E8D}"/>
+  <xr:revisionPtr revIDLastSave="778" documentId="8_{629DCDB6-94E5-432A-9179-03575796D74D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D131766D-960B-401D-97E4-990DB27333E4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B845255D-815F-49EA-8438-49CAB31B3547}"/>
   </bookViews>
@@ -64,6 +64,54 @@
           </rPr>
           <t xml:space="preserve">
 EUR/MW, da dividere per il tempo di carica/scarica del modello per passare a EUR/MWh</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{9268CEBC-CA26-47CA-9A6F-B6483AED7888}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gianvito Colucci:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Ha senso inserire un capex? Secondo me la capacità esistente è già la massima sfruttabile</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{011B247D-6DEC-4E3E-B41E-D67D270E60E7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gianvito Colucci:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Ha senso inserire un capex? Secondo me la capacità esistente è già la massima sfruttabile</t>
         </r>
       </text>
     </comment>
@@ -250,7 +298,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="87">
   <si>
     <t>value</t>
   </si>
@@ -493,6 +541,24 @@
   </si>
   <si>
     <t>World Nuclear Association, EIA, NREL</t>
+  </si>
+  <si>
+    <t>CAPEX idroelettrico</t>
+  </si>
+  <si>
+    <t>CAPEX PHS</t>
+  </si>
+  <si>
+    <t>CAPEX carbone</t>
+  </si>
+  <si>
+    <t>CAPEX gas</t>
+  </si>
+  <si>
+    <t>Ciclo combinato</t>
+  </si>
+  <si>
+    <t>Ciclo a vapore</t>
   </si>
 </sst>
 </file>
@@ -619,7 +685,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -712,6 +778,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -729,10 +798,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1052,10 +1117,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C372154-4B0A-49B9-8FF3-F49D60098BF7}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1217,71 +1282,135 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="8"/>
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="30"/>
       <c r="C10" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="8"/>
+        <v>8</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="30"/>
       <c r="C11" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="8"/>
+        <v>83</v>
+      </c>
+      <c r="B12" s="34">
+        <v>2338600</v>
+      </c>
       <c r="C12" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="8"/>
+        <v>84</v>
+      </c>
+      <c r="B13" s="34">
+        <v>825440</v>
+      </c>
       <c r="C13" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="8"/>
+        <v>8</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1298,8 +1427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42806216-DB6B-4ED6-9AA4-BC1B162122E7}">
   <dimension ref="A1:Y27"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16:G18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1932,10 +2061,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F958822-C8DD-4CF0-BC79-5189EFFDF89D}">
-  <dimension ref="A1:T29"/>
+  <dimension ref="A1:T37"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3:R3"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1953,7 +2082,7 @@
     <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>41</v>
       </c>
@@ -1985,7 +2114,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -2025,7 +2154,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
@@ -2065,7 +2194,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
@@ -2096,7 +2225,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2127,7 +2256,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>5</v>
       </c>
@@ -2158,7 +2287,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
@@ -2189,7 +2318,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>5</v>
       </c>
@@ -2220,7 +2349,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>5</v>
       </c>
@@ -2251,7 +2380,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>6</v>
       </c>
@@ -2277,14 +2406,14 @@
         <v>53</v>
       </c>
       <c r="I10" s="23">
-        <f t="shared" ref="I10:I17" si="1">D10*$Q$3*10^3</f>
+        <f t="shared" ref="I10:I25" si="1">D10*$Q$3*10^3</f>
         <v>5420800.0000000009</v>
       </c>
       <c r="J10" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>6</v>
       </c>
@@ -2317,7 +2446,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>6</v>
       </c>
@@ -2350,7 +2479,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>6</v>
       </c>
@@ -2383,52 +2512,42 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>62</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="B14" s="8"/>
       <c r="C14" s="8">
-        <v>2025</v>
-      </c>
-      <c r="D14" s="23">
-        <v>5350</v>
-      </c>
+        <v>2020</v>
+      </c>
+      <c r="D14" s="23"/>
       <c r="E14" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F14" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="G14" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="H14" s="24" t="s">
-        <v>61</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" s="25"/>
       <c r="I14" s="23">
-        <f>D14*$Q$3*10^3*0.67</f>
-        <v>3154360</v>
+        <f t="shared" ref="I14:I21" si="2">D14*$Q$3*10^3</f>
+        <v>0</v>
       </c>
       <c r="J14" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>65</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="B15" s="8"/>
       <c r="C15" s="8">
-        <v>2020</v>
-      </c>
-      <c r="D15" s="28">
-        <v>988.32170015695567</v>
-      </c>
+        <v>2030</v>
+      </c>
+      <c r="D15" s="23"/>
       <c r="E15" s="1" t="s">
         <v>36</v>
       </c>
@@ -2438,305 +2557,555 @@
       <c r="G15" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="H15" s="24" t="s">
+      <c r="H15" s="25"/>
+      <c r="I15" s="23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8">
+        <v>2020</v>
+      </c>
+      <c r="D16" s="23"/>
+      <c r="E16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" s="25"/>
+      <c r="I16" s="23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8">
+        <v>2030</v>
+      </c>
+      <c r="D17" s="23"/>
+      <c r="E17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" s="25"/>
+      <c r="I17" s="23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" s="8">
+        <v>2020</v>
+      </c>
+      <c r="D18" s="23">
+        <v>3075</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" s="25"/>
+      <c r="I18" s="23">
+        <f t="shared" si="2"/>
+        <v>2706000</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="8">
+        <v>2030</v>
+      </c>
+      <c r="D19" s="23">
+        <v>2240</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G19" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H19" s="25"/>
+      <c r="I19" s="23">
+        <f t="shared" si="2"/>
+        <v>1971200</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="K19" s="10">
+        <f>AVERAGE(I18:I19)</f>
+        <v>2338600</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="8">
+        <v>2020</v>
+      </c>
+      <c r="D20" s="23">
+        <v>1038</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H20" s="25"/>
+      <c r="I20" s="23">
+        <f t="shared" si="2"/>
+        <v>913440</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="K20" s="10">
+        <f>AVERAGE(I20:I21)</f>
+        <v>825440</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="8">
+        <v>2030</v>
+      </c>
+      <c r="D21" s="23">
+        <v>838</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H21" s="25"/>
+      <c r="I21" s="23">
+        <f t="shared" si="2"/>
+        <v>737440</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="8">
+        <v>2025</v>
+      </c>
+      <c r="D22" s="23">
+        <v>5350</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F22" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="G22" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="H22" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="I22" s="23">
+        <f>D22*$Q$3*10^3*0.67</f>
+        <v>3154360</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="8">
+        <v>2020</v>
+      </c>
+      <c r="D23" s="28">
+        <v>988.32170015695567</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G23" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H23" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="I15" s="23">
+      <c r="I23" s="23">
         <f t="shared" si="1"/>
         <v>869723.09613812109</v>
       </c>
-      <c r="J15" s="8" t="s">
+      <c r="J23" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="R15" s="2"/>
-      <c r="S15" s="6"/>
-      <c r="T15" s="6"/>
-    </row>
-    <row r="16" spans="1:20" ht="72" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
+      <c r="R23" s="2"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="6"/>
+    </row>
+    <row r="24" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B24" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C24" s="8">
         <v>2030</v>
       </c>
-      <c r="D16" s="28">
+      <c r="D24" s="28">
         <v>681.62247956991291</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F16" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G16" s="24" t="s">
+      <c r="F24" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G24" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="H16" s="24" t="s">
+      <c r="H24" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="I16" s="23">
+      <c r="I24" s="23">
         <f t="shared" si="1"/>
         <v>599827.78202152334</v>
       </c>
-      <c r="J16" s="8" t="s">
+      <c r="J24" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="R16" s="2"/>
-      <c r="S16" s="4"/>
-      <c r="T16" s="4"/>
-    </row>
-    <row r="17" spans="1:20" ht="72" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
+      <c r="R24" s="2"/>
+      <c r="S24" s="4"/>
+      <c r="T24" s="4"/>
+    </row>
+    <row r="25" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B25" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C25" s="8">
         <v>2050</v>
       </c>
-      <c r="D17" s="29">
+      <c r="D25" s="29">
         <v>681.62247956991291</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F17" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G17" s="24" t="s">
+      <c r="F25" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G25" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="H17" s="24" t="s">
+      <c r="H25" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="I17" s="23">
+      <c r="I25" s="23">
         <f t="shared" si="1"/>
         <v>599827.78202152334</v>
       </c>
-      <c r="J17" s="8" t="s">
+      <c r="J25" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="R17" s="2"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
-    </row>
-    <row r="18" spans="1:20" ht="72" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
+      <c r="R25" s="2"/>
+      <c r="S25" s="5"/>
+      <c r="T25" s="5"/>
+    </row>
+    <row r="26" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+      <c r="A26" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B26" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C26" s="8">
         <v>2020</v>
       </c>
-      <c r="D18" s="28">
+      <c r="D26" s="28">
         <v>1727.2344448095646</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F18" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G18" s="24" t="s">
+      <c r="F26" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G26" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="H18" s="24" t="s">
+      <c r="H26" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="I18" s="23">
-        <f t="shared" ref="I18:I20" si="2">D18*$Q$3*10^3</f>
+      <c r="I26" s="23">
+        <f t="shared" ref="I26:I28" si="3">D26*$Q$3*10^3</f>
         <v>1519966.3114324168</v>
       </c>
-      <c r="J18" s="8" t="s">
+      <c r="J26" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="S18" s="9"/>
-      <c r="T18" s="10"/>
-    </row>
-    <row r="19" spans="1:20" ht="72" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
+      <c r="S26" s="9"/>
+      <c r="T26" s="10"/>
+    </row>
+    <row r="27" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B27" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C27" s="8">
         <v>2030</v>
       </c>
-      <c r="D19" s="28">
+      <c r="D27" s="28">
         <v>1173.7257628388072</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F19" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G19" s="24" t="s">
+      <c r="F27" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G27" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="H19" s="24" t="s">
+      <c r="H27" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="I19" s="23">
-        <f t="shared" si="2"/>
+      <c r="I27" s="23">
+        <f t="shared" si="3"/>
         <v>1032878.6712981503</v>
       </c>
-      <c r="J19" s="8" t="s">
+      <c r="J27" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="S19" s="9"/>
-      <c r="T19" s="10"/>
-    </row>
-    <row r="20" spans="1:20" ht="72" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
+      <c r="S27" s="9"/>
+      <c r="T27" s="10"/>
+    </row>
+    <row r="28" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+      <c r="A28" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B28" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C28" s="8">
         <v>2050</v>
       </c>
-      <c r="D20" s="29">
+      <c r="D28" s="29">
         <v>1173.7257628388072</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G20" s="24" t="s">
+      <c r="F28" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G28" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="H20" s="24" t="s">
+      <c r="H28" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="I20" s="23">
-        <f t="shared" si="2"/>
+      <c r="I28" s="23">
+        <f t="shared" si="3"/>
         <v>1032878.6712981503</v>
       </c>
-      <c r="J20" s="8" t="s">
+      <c r="J28" s="8" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="23">
-        <f>AVERAGE(I18,I19,I15,I16)</f>
-        <v>1005598.9652225529</v>
-      </c>
-      <c r="J22" s="8"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
-      <c r="D29" s="18"/>
+      <c r="D29" s="28"/>
       <c r="E29" s="1"/>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="23">
+        <f>AVERAGE(I26,I27,I23,I24)</f>
+        <v>1005598.9652225529</v>
+      </c>
+      <c r="J30" s="8"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A31" s="8"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="8"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2761,27 +3130,43 @@
     <hyperlink ref="F12" r:id="rId19" display="World Bank" xr:uid="{0EE4B772-3B1C-40C1-8489-D0631B2D4463}"/>
     <hyperlink ref="F13" r:id="rId20" display="World Bank" xr:uid="{C22641C2-FA38-48D9-BCB2-1FCE72A643D6}"/>
     <hyperlink ref="G10" r:id="rId21" xr:uid="{1BCFB97B-FADB-43D9-B44E-ADA05CA17A73}"/>
-    <hyperlink ref="F15" r:id="rId22" display="World Bank" xr:uid="{AF15079B-1809-4BD8-A648-4D62ABE8C206}"/>
-    <hyperlink ref="G15" r:id="rId23" xr:uid="{0CA73A59-1222-47DA-A59D-000D8B582034}"/>
-    <hyperlink ref="F16" r:id="rId24" display="World Bank" xr:uid="{199C7D2F-21A1-4692-9440-4CC169B6F2F2}"/>
-    <hyperlink ref="G16" r:id="rId25" xr:uid="{CECC446B-999A-4D89-A0D6-D3177C929A3D}"/>
-    <hyperlink ref="F17" r:id="rId26" display="World Bank" xr:uid="{8716B52B-0C43-4E99-8CCE-17C58FE13622}"/>
-    <hyperlink ref="G17" r:id="rId27" xr:uid="{85050209-E008-45C2-8A24-F79F70751A59}"/>
+    <hyperlink ref="F23" r:id="rId22" display="World Bank" xr:uid="{AF15079B-1809-4BD8-A648-4D62ABE8C206}"/>
+    <hyperlink ref="G23" r:id="rId23" xr:uid="{0CA73A59-1222-47DA-A59D-000D8B582034}"/>
+    <hyperlink ref="F24" r:id="rId24" display="World Bank" xr:uid="{199C7D2F-21A1-4692-9440-4CC169B6F2F2}"/>
+    <hyperlink ref="G24" r:id="rId25" xr:uid="{CECC446B-999A-4D89-A0D6-D3177C929A3D}"/>
+    <hyperlink ref="F25" r:id="rId26" display="World Bank" xr:uid="{8716B52B-0C43-4E99-8CCE-17C58FE13622}"/>
+    <hyperlink ref="G25" r:id="rId27" xr:uid="{85050209-E008-45C2-8A24-F79F70751A59}"/>
     <hyperlink ref="G11:G13" r:id="rId28" display="Dati elaborati da NREL" xr:uid="{8CAF9D49-1D95-457A-AD06-EF2B25EC7C48}"/>
-    <hyperlink ref="H15" r:id="rId29" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{BD06F35F-2859-4868-A250-9877196A2A8B}"/>
-    <hyperlink ref="H16:H17" r:id="rId30" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{D5926397-0CC0-4EED-B446-ADD3939AFBF8}"/>
+    <hyperlink ref="H23" r:id="rId29" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{BD06F35F-2859-4868-A250-9877196A2A8B}"/>
+    <hyperlink ref="H24:H25" r:id="rId30" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{D5926397-0CC0-4EED-B446-ADD3939AFBF8}"/>
     <hyperlink ref="R3" r:id="rId31" xr:uid="{1F188A66-AA31-42D5-BF68-5F94EC7F5B80}"/>
-    <hyperlink ref="F14" r:id="rId32" xr:uid="{BBB5C12E-09F8-42A0-BC0B-98E2FE229F3F}"/>
-    <hyperlink ref="H14" r:id="rId33" display="Overnight cost, suggerito da Lorenzo Mazzocco (vedi messaggio discord su Coordinamento energia)" xr:uid="{7623CF7E-7357-466F-811C-79E8E0B20885}"/>
-    <hyperlink ref="F18" r:id="rId34" display="World Bank" xr:uid="{A46629F6-B5CF-4B20-92CC-DAAA37FA0295}"/>
-    <hyperlink ref="G18" r:id="rId35" xr:uid="{4C8330BE-8E6C-45DA-8011-98C7288331BF}"/>
-    <hyperlink ref="H18" r:id="rId36" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{DBA68ACF-849E-462B-8CC2-2BE6A9705126}"/>
-    <hyperlink ref="F19" r:id="rId37" display="World Bank" xr:uid="{E1E46D67-8566-4081-8026-9282FEEA7794}"/>
-    <hyperlink ref="F20" r:id="rId38" display="World Bank" xr:uid="{C2B4C806-3E78-4AEF-A359-42B49AF6C869}"/>
-    <hyperlink ref="G19" r:id="rId39" xr:uid="{A07DD3DB-85F5-450E-BE7A-F242BAF7D635}"/>
-    <hyperlink ref="G20" r:id="rId40" xr:uid="{CB5BF0A4-3E46-40DE-9A2B-D68DCB0772EB}"/>
-    <hyperlink ref="H19" r:id="rId41" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{2364EE2D-C0F7-4609-B6E2-FD4BE059C070}"/>
-    <hyperlink ref="H20" r:id="rId42" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{222C5FBD-1584-4E8E-8AE1-8423CB925839}"/>
+    <hyperlink ref="F22" r:id="rId32" xr:uid="{BBB5C12E-09F8-42A0-BC0B-98E2FE229F3F}"/>
+    <hyperlink ref="H22" r:id="rId33" display="Overnight cost, suggerito da Lorenzo Mazzocco (vedi messaggio discord su Coordinamento energia)" xr:uid="{7623CF7E-7357-466F-811C-79E8E0B20885}"/>
+    <hyperlink ref="F26" r:id="rId34" display="World Bank" xr:uid="{A46629F6-B5CF-4B20-92CC-DAAA37FA0295}"/>
+    <hyperlink ref="G26" r:id="rId35" xr:uid="{4C8330BE-8E6C-45DA-8011-98C7288331BF}"/>
+    <hyperlink ref="H26" r:id="rId36" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{DBA68ACF-849E-462B-8CC2-2BE6A9705126}"/>
+    <hyperlink ref="F27" r:id="rId37" display="World Bank" xr:uid="{E1E46D67-8566-4081-8026-9282FEEA7794}"/>
+    <hyperlink ref="F28" r:id="rId38" display="World Bank" xr:uid="{C2B4C806-3E78-4AEF-A359-42B49AF6C869}"/>
+    <hyperlink ref="G27" r:id="rId39" xr:uid="{A07DD3DB-85F5-450E-BE7A-F242BAF7D635}"/>
+    <hyperlink ref="G28" r:id="rId40" xr:uid="{CB5BF0A4-3E46-40DE-9A2B-D68DCB0772EB}"/>
+    <hyperlink ref="H27" r:id="rId41" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{2364EE2D-C0F7-4609-B6E2-FD4BE059C070}"/>
+    <hyperlink ref="H28" r:id="rId42" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{222C5FBD-1584-4E8E-8AE1-8423CB925839}"/>
+    <hyperlink ref="F14" r:id="rId43" display="World Bank" xr:uid="{E6B37642-D048-481C-9CC7-5A49E1FAF2CA}"/>
+    <hyperlink ref="F15" r:id="rId44" display="World Bank" xr:uid="{84A1BEF5-1A35-4339-BC8F-1422193D060B}"/>
+    <hyperlink ref="F16" r:id="rId45" display="World Bank" xr:uid="{F64E52A3-071D-493B-B9F5-54A99596FF8A}"/>
+    <hyperlink ref="F17" r:id="rId46" display="World Bank" xr:uid="{007C4746-D8D7-4BB4-9A98-094B413757E0}"/>
+    <hyperlink ref="F18" r:id="rId47" display="World Bank" xr:uid="{2ED50F93-82F0-4419-934B-859DBAF4AF86}"/>
+    <hyperlink ref="F19" r:id="rId48" display="World Bank" xr:uid="{4152C890-4CBC-4765-9676-DA66A17BA52D}"/>
+    <hyperlink ref="F20" r:id="rId49" display="World Bank" xr:uid="{36A7A00F-693D-4DAE-9AF0-675C47F8279D}"/>
+    <hyperlink ref="F21" r:id="rId50" display="World Bank" xr:uid="{3860649B-A612-480C-B0EF-543D2BC864C7}"/>
+    <hyperlink ref="G14" r:id="rId51" xr:uid="{FC002B2B-3217-4129-88DA-356B844CE48E}"/>
+    <hyperlink ref="G15" r:id="rId52" xr:uid="{94E9F270-83DE-4273-954E-96F713533C46}"/>
+    <hyperlink ref="G16" r:id="rId53" xr:uid="{487E5883-403D-40EC-91F6-69377FC88A21}"/>
+    <hyperlink ref="G17" r:id="rId54" xr:uid="{AEA5CDB1-5155-4166-A825-786CA9AB969B}"/>
+    <hyperlink ref="G18" r:id="rId55" xr:uid="{2C8D643E-A3EA-469A-BB23-74E3B07C68EF}"/>
+    <hyperlink ref="G19" r:id="rId56" xr:uid="{2550B267-0DEF-4867-BFB8-835C895322D8}"/>
+    <hyperlink ref="G20" r:id="rId57" xr:uid="{F41DC907-DAFD-4054-B9F6-FF5FB48AE9FA}"/>
+    <hyperlink ref="G21" r:id="rId58" xr:uid="{2EFD1AB9-F361-4E75-A928-2E6F74388126}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finished data processing/import. Added NuclearPlant and CoalPlant json files. Added new, centralized technology folder. Read_demand is not working yet
</commit_message>
<xml_diff>
--- a/dati_casoStudioItalia/altri_dati.xlsx
+++ b/dati_casoStudioItalia/altri_dati.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/gianvito_colucci_polito_it/Documents/Jobs/DRIN DRIN/Energy mix/DrinDrin---Mix-energetico/dati_casoStudioItalia/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DrinDrin\dati_casoStudioItalia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="778" documentId="8_{629DCDB6-94E5-432A-9179-03575796D74D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D131766D-960B-401D-97E4-990DB27333E4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3E9678-A73D-4A20-B42E-4F005D2E7DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B845255D-815F-49EA-8438-49CAB31B3547}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{B845255D-815F-49EA-8438-49CAB31B3547}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
-    <sheet name="raw_data_commodity" sheetId="2" r:id="rId2"/>
-    <sheet name="raw_data_techs" sheetId="3" r:id="rId3"/>
+    <sheet name="OPEX" sheetId="6" r:id="rId1"/>
+    <sheet name="CAPEX" sheetId="1" r:id="rId2"/>
+    <sheet name="Fuel_cost" sheetId="5" r:id="rId3"/>
+    <sheet name="Transmission_abroad" sheetId="4" r:id="rId4"/>
+    <sheet name="raw_data_commodity" sheetId="2" r:id="rId5"/>
+    <sheet name="raw_data_techs" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,10 +43,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Gianvito Colucci</author>
+    <author>Bertoni, L. (Luca)</author>
   </authors>
   <commentList>
-    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{5CF03D84-CFD5-4BC9-8BE2-A62E05876F5C}">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{52950CF3-9BD0-40D6-94D2-8E0C1D67B00B}">
       <text>
         <r>
           <rPr>
@@ -53,7 +56,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Gianvito Colucci:</t>
+          <t>Bertoni, L. (Luca):</t>
         </r>
         <r>
           <rPr>
@@ -63,11 +66,12 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-EUR/MW, da dividere per il tempo di carica/scarica del modello per passare a EUR/MWh</t>
+in MWh
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{9268CEBC-CA26-47CA-9A6F-B6483AED7888}">
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{6042687D-A9B5-4779-9A54-E22AF9FBB252}">
       <text>
         <r>
           <rPr>
@@ -77,7 +81,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Gianvito Colucci:</t>
+          <t>Bertoni, L. (Luca):</t>
         </r>
         <r>
           <rPr>
@@ -87,11 +91,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Ha senso inserire un capex? Secondo me la capacità esistente è già la massima sfruttabile</t>
+Tutti I tipi</t>
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{011B247D-6DEC-4E3E-B41E-D67D270E60E7}">
+    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{ACE5EF51-CB51-4DAB-B6B4-87E92D626050}">
       <text>
         <r>
           <rPr>
@@ -101,7 +105,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Gianvito Colucci:</t>
+          <t>Bertoni, L. (Luca):</t>
         </r>
         <r>
           <rPr>
@@ -111,7 +115,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Ha senso inserire un capex? Secondo me la capacità esistente è già la massima sfruttabile</t>
+in MWh
+</t>
         </r>
       </text>
     </comment>
@@ -298,10 +303,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="87">
-  <si>
-    <t>value</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="98">
   <si>
     <t>CAPEX solare</t>
   </si>
@@ -333,27 +335,6 @@
     <t>EUR/MWh</t>
   </si>
   <si>
-    <t>Trasmissione Francia</t>
-  </si>
-  <si>
-    <t>MW</t>
-  </si>
-  <si>
-    <t>Trasmissione Svizzera</t>
-  </si>
-  <si>
-    <t>Trasmissione Austria</t>
-  </si>
-  <si>
-    <t>Trasmissione Slovenia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prezzo import </t>
-  </si>
-  <si>
-    <t>Prezzo export</t>
-  </si>
-  <si>
     <t>costo combustibile gas</t>
   </si>
   <si>
@@ -468,12 +449,6 @@
     <t>Average annual value, 2024</t>
   </si>
   <si>
-    <t>CAPEX eolico onshore</t>
-  </si>
-  <si>
-    <t>CAPEX eolico offshore</t>
-  </si>
-  <si>
     <t>Average, 2020-2030</t>
   </si>
   <si>
@@ -543,22 +518,85 @@
     <t>World Nuclear Association, EIA, NREL</t>
   </si>
   <si>
-    <t>CAPEX idroelettrico</t>
-  </si>
-  <si>
-    <t>CAPEX PHS</t>
-  </si>
-  <si>
-    <t>CAPEX carbone</t>
-  </si>
-  <si>
-    <t>CAPEX gas</t>
-  </si>
-  <si>
-    <t>Ciclo combinato</t>
-  </si>
-  <si>
-    <t>Ciclo a vapore</t>
+    <t>CAPEX</t>
+  </si>
+  <si>
+    <t>Hydro_Reservoir</t>
+  </si>
+  <si>
+    <t>GasTurbine_simple</t>
+  </si>
+  <si>
+    <t>Photovoltaic</t>
+  </si>
+  <si>
+    <t>CoalPlant</t>
+  </si>
+  <si>
+    <t>Storage_Battery</t>
+  </si>
+  <si>
+    <t>PumpedHydro_Closed</t>
+  </si>
+  <si>
+    <t>NuclearPlant</t>
+  </si>
+  <si>
+    <t>electricity map</t>
+  </si>
+  <si>
+    <t>Include francia, svizzera, slovenia, austria</t>
+  </si>
+  <si>
+    <t>WindTurbine_Onshore_4000</t>
+  </si>
+  <si>
+    <t>OPEX</t>
+  </si>
+  <si>
+    <t>fraction of capex</t>
+  </si>
+  <si>
+    <t>fuel_cost</t>
+  </si>
+  <si>
+    <t>costo_combustibile_gas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">costo_combustibile_nucleare </t>
+  </si>
+  <si>
+    <t>costo_combustibile_carbone</t>
+  </si>
+  <si>
+    <t>capacity</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>CALA</t>
+  </si>
+  <si>
+    <t>CNOR</t>
+  </si>
+  <si>
+    <t>CSUD</t>
+  </si>
+  <si>
+    <t>NORD</t>
+  </si>
+  <si>
+    <t>SARD</t>
+  </si>
+  <si>
+    <t>SICI</t>
+  </si>
+  <si>
+    <t>SUD</t>
+  </si>
+  <si>
+    <t>emission_factor_t/MWh</t>
   </si>
 </sst>
 </file>
@@ -649,26 +687,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -685,7 +727,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -768,18 +810,21 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1116,11 +1161,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C372154-4B0A-49B9-8FF3-F49D60098BF7}">
-  <dimension ref="A1:E19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9398001-B177-42A1-9F09-DD1B7293885B}">
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1134,301 +1179,515 @@
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="23">
-        <v>27.538556570687646</v>
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="8">
+        <v>0.04</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" t="s">
-        <v>55</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="23">
-        <v>10.331146370574086</v>
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="8">
+        <v>0.04</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="23">
-        <v>4.8</v>
+        <v>78</v>
+      </c>
+      <c r="B4" s="8">
+        <v>0.04</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="E4" t="s">
-        <v>79</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>1</v>
+      <c r="A5" t="s">
+        <v>76</v>
       </c>
       <c r="B5" s="8">
-        <v>918280</v>
+        <v>0.04</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
-        <v>56</v>
+        <v>83</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>72</v>
       </c>
       <c r="B6" s="8">
-        <v>1063920</v>
+        <v>0.04</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
-        <v>57</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>73</v>
       </c>
       <c r="B7" s="8">
-        <v>3082860</v>
+        <v>0.04</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
-        <v>6</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>75</v>
       </c>
       <c r="B8" s="8">
-        <v>3154360</v>
+        <v>0.04</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" s="27" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="30">
-        <v>1005598.9652225529</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="8">
+        <v>0.04</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B12" s="34">
-        <v>2338600</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B13" s="34">
-        <v>825440</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="8"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="8"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="8"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="8"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="8"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="8"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{B66498B8-EE20-4806-A7DF-B085A43B81A8}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{B66BD1F3-C8A1-406D-BC7B-C4AD639B5C2B}"/>
-    <hyperlink ref="D8" r:id="rId3" xr:uid="{76843948-9A3E-4EB0-A540-24DF6B66F999}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C372154-4B0A-49B9-8FF3-F49D60098BF7}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="8">
+        <v>918280</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1063920</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="8">
+        <v>3154360</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="33">
+        <f>1005598.96522255*0.3</f>
+        <v>301679.68956676498</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="34">
+        <v>1</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="34">
+        <v>2</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="34">
+        <v>2</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="34">
+        <v>2</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{76843948-9A3E-4EB0-A540-24DF6B66F999}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F36F9B7-E410-4418-9AFE-4DC5A9893242}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="23">
+        <v>27.538556570687646</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="23">
+        <v>10.331146370574086</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="23">
+        <v>4.8</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{899EB925-18FE-4D0F-90A7-19454D63E70C}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{8C713812-7D41-41B1-95A2-AD8C3456DC0C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25E773EF-BD6E-41C4-818D-318BE958C680}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="8">
+        <v>10138</v>
+      </c>
+      <c r="C2" s="8">
+        <v>100</v>
+      </c>
+      <c r="D2">
+        <v>0.1</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="34">
+        <v>1</v>
+      </c>
+      <c r="C3" s="34">
+        <v>1</v>
+      </c>
+      <c r="D3" s="34">
+        <v>1</v>
+      </c>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="34">
+        <v>1</v>
+      </c>
+      <c r="C4" s="34">
+        <v>1</v>
+      </c>
+      <c r="D4" s="34">
+        <v>1</v>
+      </c>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="34">
+        <v>1</v>
+      </c>
+      <c r="C5" s="34">
+        <v>1</v>
+      </c>
+      <c r="D5" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="34">
+        <v>1</v>
+      </c>
+      <c r="C6" s="34">
+        <v>1</v>
+      </c>
+      <c r="D6" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="34">
+        <v>1</v>
+      </c>
+      <c r="C7" s="34">
+        <v>1</v>
+      </c>
+      <c r="D7" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="34">
+        <v>1</v>
+      </c>
+      <c r="C8" s="34">
+        <v>1</v>
+      </c>
+      <c r="D8" s="34">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42806216-DB6B-4ED6-9AA4-BC1B162122E7}">
   <dimension ref="A1:Y27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1450,35 +1709,35 @@
   <sheetData>
     <row r="1" spans="1:25" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B2" s="20">
         <v>2018</v>
@@ -1487,36 +1746,36 @@
         <v>7.5414094383199997</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G2" s="9">
         <f t="shared" ref="G2:G8" si="0">C2*$M$3/$M$4</f>
         <v>21.805545521741941</v>
       </c>
       <c r="H2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B3" s="20">
         <v>2019</v>
@@ -1525,38 +1784,38 @@
         <v>4.8274540271299999</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G3" s="9">
         <f t="shared" si="0"/>
         <v>13.958301747657082</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
       <c r="L3" s="15" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="M3" s="11">
         <v>0.85</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="W3" s="2"/>
       <c r="Y3" s="6"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B4" s="20">
         <v>2020</v>
@@ -1565,23 +1824,23 @@
         <v>3.3115669452400409</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G4" s="9">
         <f t="shared" si="0"/>
         <v>9.5752026677938797</v>
       </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="L4" s="15" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="M4" s="12">
         <v>0.29397099999999998</v>
@@ -1592,7 +1851,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B5" s="20">
         <v>2021</v>
@@ -1601,23 +1860,23 @@
         <v>14.731149861407678</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G5" s="9">
         <f t="shared" si="0"/>
         <v>42.594260597802254</v>
       </c>
       <c r="H5" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="L5" s="15" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="M5" s="14">
         <f>1.622*10^-6</f>
@@ -1628,7 +1887,7 @@
     </row>
     <row r="6" spans="1:25" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B6" s="20">
         <v>2022</v>
@@ -1637,35 +1896,35 @@
         <v>34.346664233461041</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G6" s="9">
         <f t="shared" si="0"/>
         <v>99.311376286919071</v>
       </c>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="M6" s="11">
         <v>6000</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="Y6" s="10"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B7" s="20">
         <v>2023</v>
@@ -1674,35 +1933,35 @@
         <v>11.492903809114813</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G7" s="9">
         <f t="shared" si="0"/>
         <v>33.23106101536407</v>
       </c>
       <c r="H7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="L7" s="15" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="M7" s="11">
         <v>0.82</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="Y7" s="10"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B8" s="20">
         <v>2024</v>
@@ -1711,35 +1970,35 @@
         <v>9.52416119251955</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G8" s="9">
         <f t="shared" si="0"/>
         <v>27.538556570687646</v>
       </c>
       <c r="H8" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="L8" s="15" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="M8" s="11">
         <v>0.88</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="Y8" s="10"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B9" s="20">
         <v>2018</v>
@@ -1748,27 +2007,27 @@
         <v>105.06823090515999</v>
       </c>
       <c r="D9" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E9" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="G9" s="9">
         <f t="shared" ref="G9:G15" si="1">C9*$M$3/$M$6/$M$5/1000</f>
         <v>9.1767361559171796</v>
       </c>
       <c r="H9" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="M9" s="13"/>
       <c r="Y9" s="10"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B10" s="20">
         <v>2019</v>
@@ -1777,27 +2036,27 @@
         <v>78.292956708220004</v>
       </c>
       <c r="D10" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="G10" s="9">
         <f t="shared" si="1"/>
         <v>6.8381641185765512</v>
       </c>
       <c r="H10" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="M10" s="13"/>
       <c r="Y10" s="10"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B11" s="20">
         <v>2020</v>
@@ -1806,27 +2065,27 @@
         <v>62.08886618998978</v>
       </c>
       <c r="D11" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="G11" s="9">
         <f t="shared" si="1"/>
         <v>5.4228869976871463</v>
       </c>
       <c r="H11" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="M11" s="13"/>
       <c r="Y11" s="10"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B12" s="20">
         <v>2021</v>
@@ -1835,27 +2094,27 @@
         <v>126.18829981718464</v>
       </c>
       <c r="D12" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E12" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="G12" s="9">
         <f t="shared" si="1"/>
         <v>11.021378426285136</v>
       </c>
       <c r="H12" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="M12" s="13"/>
       <c r="Y12" s="10"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B13" s="20">
         <v>2022</v>
@@ -1864,27 +2123,27 @@
         <v>293.6511990918093</v>
       </c>
       <c r="D13" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="G13" s="9">
         <f t="shared" si="1"/>
         <v>25.647710565971831</v>
       </c>
       <c r="H13" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="M13" s="13"/>
       <c r="Y13" s="10"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B14" s="20">
         <v>2023</v>
@@ -1893,27 +2152,27 @@
         <v>151.42784107508328</v>
       </c>
       <c r="D14" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E14" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="G14" s="9">
         <f t="shared" si="1"/>
         <v>13.225818425176818</v>
       </c>
       <c r="H14" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="M14" s="13"/>
       <c r="Y14" s="10"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B15" s="20">
         <v>2024</v>
@@ -1922,27 +2181,27 @@
         <v>118.28554879814943</v>
       </c>
       <c r="D15" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="G15" s="9">
         <f t="shared" si="1"/>
         <v>10.331146370574086</v>
       </c>
       <c r="H15" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="M15" s="13"/>
       <c r="Y15" s="10"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16" s="20">
         <v>2021</v>
@@ -1951,50 +2210,50 @@
         <v>0.46</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="G16" s="9">
         <f>C16*M7/100*1000</f>
         <v>3.7719999999999998</v>
       </c>
       <c r="H16" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="M16" s="13"/>
       <c r="Y16" s="4"/>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="32" t="s">
-        <v>77</v>
+        <v>1</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>67</v>
       </c>
       <c r="C17" s="21">
         <v>7</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="G17" s="9">
         <f>C17*M7</f>
         <v>5.7399999999999993</v>
       </c>
       <c r="H17" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="M17" s="13"/>
       <c r="Y17" s="5"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B18" s="20">
         <v>2021</v>
@@ -2003,17 +2262,17 @@
         <v>0.61</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="G18" s="9">
         <f>C18*M7/100*1000</f>
         <v>5.0019999999999998</v>
       </c>
       <c r="H18" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="M18" s="13"/>
       <c r="Y18" s="9"/>
@@ -2030,7 +2289,7 @@
       <c r="E21" s="24"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="E22" s="31"/>
+      <c r="E22" s="30"/>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="Q27" s="17"/>
@@ -2059,12 +2318,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F958822-C8DD-4CF0-BC79-5189EFFDF89D}">
-  <dimension ref="A1:T37"/>
+  <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3:R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2082,44 +2341,44 @@
     <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>47</v>
       </c>
       <c r="C2" s="8">
         <v>2020</v>
@@ -2128,13 +2387,13 @@
         <v>1333</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="24" t="s">
         <v>36</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="24" t="s">
-        <v>44</v>
       </c>
       <c r="H2" s="24"/>
       <c r="I2" s="23">
@@ -2142,24 +2401,24 @@
         <v>1173040</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C3" s="8">
         <v>2030</v>
@@ -2168,13 +2427,13 @@
         <v>754</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="24" t="s">
         <v>36</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="24" t="s">
-        <v>44</v>
       </c>
       <c r="H3" s="24"/>
       <c r="I3" s="23">
@@ -2182,24 +2441,24 @@
         <v>663520</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="P3" s="15" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="Q3" s="11">
         <v>0.88</v>
       </c>
       <c r="R3" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C4" s="8">
         <v>2020</v>
@@ -2208,13 +2467,13 @@
         <v>1462</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="24" t="s">
         <v>36</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" s="24" t="s">
-        <v>44</v>
       </c>
       <c r="H4" s="24"/>
       <c r="I4" s="23">
@@ -2222,15 +2481,15 @@
         <v>1286560</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C5" s="8">
         <v>2030</v>
@@ -2239,13 +2498,13 @@
         <v>956</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="24" t="s">
         <v>36</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>44</v>
       </c>
       <c r="H5" s="24"/>
       <c r="I5" s="23">
@@ -2253,15 +2512,15 @@
         <v>841280</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C6" s="8">
         <v>2020</v>
@@ -2270,13 +2529,13 @@
         <v>3739</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="24" t="s">
         <v>36</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" s="24" t="s">
-        <v>44</v>
       </c>
       <c r="H6" s="24"/>
       <c r="I6" s="23">
@@ -2284,15 +2543,15 @@
         <v>3290320</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C7" s="8">
         <v>2030</v>
@@ -2301,13 +2560,13 @@
         <v>2758</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="24" t="s">
         <v>36</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="24" t="s">
-        <v>44</v>
       </c>
       <c r="H7" s="24"/>
       <c r="I7" s="23">
@@ -2315,15 +2574,15 @@
         <v>2427040</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C8" s="8">
         <v>2020</v>
@@ -2332,13 +2591,13 @@
         <v>4049</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="24" t="s">
         <v>36</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G8" s="24" t="s">
-        <v>44</v>
       </c>
       <c r="H8" s="24"/>
       <c r="I8" s="23">
@@ -2346,15 +2605,15 @@
         <v>3563120</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C9" s="8">
         <v>2030</v>
@@ -2363,13 +2622,13 @@
         <v>3467</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="24" t="s">
         <v>36</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" s="24" t="s">
-        <v>44</v>
       </c>
       <c r="H9" s="24"/>
       <c r="I9" s="23">
@@ -2377,15 +2636,15 @@
         <v>3050960</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C10" s="8">
         <v>2035</v>
@@ -2394,31 +2653,31 @@
         <v>6160.0000000000009</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="H10" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10" s="23">
+        <f t="shared" ref="I10:I17" si="1">D10*$Q$3*10^3</f>
+        <v>5420800.0000000009</v>
+      </c>
+      <c r="J10" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="H10" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="I10" s="23">
-        <f t="shared" ref="I10:I25" si="1">D10*$Q$3*10^3</f>
-        <v>5420800.0000000009</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C11" s="8">
         <v>2050</v>
@@ -2427,31 +2686,31 @@
         <v>5500</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" s="24" t="s">
-        <v>44</v>
-      </c>
       <c r="H11" s="25" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="I11" s="23">
         <f t="shared" si="1"/>
         <v>4840000</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="C12" s="8">
         <v>2035</v>
@@ -2460,31 +2719,31 @@
         <v>6820.0000000000009</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G12" s="24" t="s">
-        <v>44</v>
-      </c>
       <c r="H12" s="25" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="I12" s="23">
         <f t="shared" si="1"/>
         <v>6001600.0000000009</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="C13" s="8">
         <v>2050</v>
@@ -2493,619 +2752,379 @@
         <v>6050.0000000000009</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G13" s="24" t="s">
-        <v>44</v>
-      </c>
       <c r="H13" s="25" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="I13" s="23">
         <f t="shared" si="1"/>
         <v>5324000.0000000009</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="B14" s="8"/>
+        <v>5</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="C14" s="8">
+        <v>2025</v>
+      </c>
+      <c r="D14" s="23">
+        <v>5350</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="I14" s="23">
+        <f>D14*$Q$3*10^3*0.67</f>
+        <v>3154360</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="8">
         <v>2020</v>
       </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="1" t="s">
+      <c r="D15" s="28">
+        <v>988.32170015695567</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="H15" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="I15" s="23">
+        <f t="shared" si="1"/>
+        <v>869723.09613812109</v>
+      </c>
+      <c r="J15" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="H14" s="25"/>
-      <c r="I14" s="23">
-        <f t="shared" ref="I14:I21" si="2">D14*$Q$3*10^3</f>
-        <v>0</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8">
+      <c r="R15" s="2"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+    </row>
+    <row r="16" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="8">
         <v>2030</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="1" t="s">
+      <c r="D16" s="28">
+        <v>681.62247956991291</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="H16" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="I16" s="23">
+        <f t="shared" si="1"/>
+        <v>599827.78202152334</v>
+      </c>
+      <c r="J16" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="H15" s="25"/>
-      <c r="I15" s="23">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8">
-        <v>2020</v>
-      </c>
-      <c r="D16" s="23"/>
-      <c r="E16" s="1" t="s">
+      <c r="R16" s="2"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+    </row>
+    <row r="17" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="8">
+        <v>2050</v>
+      </c>
+      <c r="D17" s="29">
+        <v>681.62247956991291</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="H17" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="I17" s="23">
+        <f t="shared" si="1"/>
+        <v>599827.78202152334</v>
+      </c>
+      <c r="J17" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G16" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="H16" s="25"/>
-      <c r="I16" s="23">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8">
-        <v>2030</v>
-      </c>
-      <c r="D17" s="23"/>
-      <c r="E17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G17" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="H17" s="25"/>
-      <c r="I17" s="23">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J17" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R17" s="2"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+    </row>
+    <row r="18" spans="1:20" ht="72" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>83</v>
+        <v>6</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
       <c r="C18" s="8">
         <v>2020</v>
       </c>
-      <c r="D18" s="23">
-        <v>3075</v>
+      <c r="D18" s="28">
+        <v>1727.2344448095646</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="H18" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="I18" s="23">
+        <f t="shared" ref="I18:I20" si="2">D18*$Q$3*10^3</f>
+        <v>1519966.3114324168</v>
+      </c>
+      <c r="J18" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G18" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="H18" s="25"/>
-      <c r="I18" s="23">
-        <f t="shared" si="2"/>
-        <v>2706000</v>
-      </c>
-      <c r="J18" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="S18" s="9"/>
+      <c r="T18" s="10"/>
+    </row>
+    <row r="19" spans="1:20" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>83</v>
+        <v>6</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
       <c r="C19" s="8">
         <v>2030</v>
       </c>
-      <c r="D19" s="23">
-        <v>2240</v>
+      <c r="D19" s="28">
+        <v>1173.7257628388072</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F19" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G19" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="H19" s="25"/>
+      <c r="H19" s="24" t="s">
+        <v>58</v>
+      </c>
       <c r="I19" s="23">
         <f t="shared" si="2"/>
-        <v>1971200</v>
+        <v>1032878.6712981503</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="K19" s="10">
-        <f>AVERAGE(I18:I19)</f>
-        <v>2338600</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="S19" s="9"/>
+      <c r="T19" s="10"/>
+    </row>
+    <row r="20" spans="1:20" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>84</v>
+        <v>6</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="C20" s="8">
-        <v>2020</v>
-      </c>
-      <c r="D20" s="23">
-        <v>1038</v>
+        <v>2050</v>
+      </c>
+      <c r="D20" s="29">
+        <v>1173.7257628388072</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G20" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="H20" s="25"/>
+      <c r="H20" s="24" t="s">
+        <v>58</v>
+      </c>
       <c r="I20" s="23">
         <f t="shared" si="2"/>
-        <v>913440</v>
+        <v>1032878.6712981503</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="K20" s="10">
-        <f>AVERAGE(I20:I21)</f>
-        <v>825440</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A21" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21" s="8">
-        <v>2030</v>
-      </c>
-      <c r="D21" s="23">
-        <v>838</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G21" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="H21" s="25"/>
-      <c r="I21" s="23">
-        <f t="shared" si="2"/>
-        <v>737440</v>
-      </c>
-      <c r="J21" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" s="8">
-        <v>2025</v>
-      </c>
-      <c r="D22" s="23">
-        <v>5350</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F22" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="G22" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="H22" s="24" t="s">
-        <v>61</v>
-      </c>
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
       <c r="I22" s="23">
-        <f>D22*$Q$3*10^3*0.67</f>
-        <v>3154360</v>
-      </c>
-      <c r="J22" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" ht="72" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="8">
-        <v>2020</v>
-      </c>
-      <c r="D23" s="28">
-        <v>988.32170015695567</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G23" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="H23" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="I23" s="23">
-        <f t="shared" si="1"/>
-        <v>869723.09613812109</v>
-      </c>
-      <c r="J23" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="R23" s="2"/>
-      <c r="S23" s="6"/>
-      <c r="T23" s="6"/>
-    </row>
-    <row r="24" spans="1:20" ht="72" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C24" s="8">
-        <v>2030</v>
-      </c>
-      <c r="D24" s="28">
-        <v>681.62247956991291</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G24" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="H24" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="I24" s="23">
-        <f t="shared" si="1"/>
-        <v>599827.78202152334</v>
-      </c>
-      <c r="J24" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="R24" s="2"/>
-      <c r="S24" s="4"/>
-      <c r="T24" s="4"/>
-    </row>
-    <row r="25" spans="1:20" ht="72" x14ac:dyDescent="0.3">
-      <c r="A25" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C25" s="8">
-        <v>2050</v>
-      </c>
-      <c r="D25" s="29">
-        <v>681.62247956991291</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G25" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="H25" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="I25" s="23">
-        <f t="shared" si="1"/>
-        <v>599827.78202152334</v>
-      </c>
-      <c r="J25" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="R25" s="2"/>
-      <c r="S25" s="5"/>
-      <c r="T25" s="5"/>
-    </row>
-    <row r="26" spans="1:20" ht="72" x14ac:dyDescent="0.3">
-      <c r="A26" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" s="8">
-        <v>2020</v>
-      </c>
-      <c r="D26" s="28">
-        <v>1727.2344448095646</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G26" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="H26" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="I26" s="23">
-        <f t="shared" ref="I26:I28" si="3">D26*$Q$3*10^3</f>
-        <v>1519966.3114324168</v>
-      </c>
-      <c r="J26" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="S26" s="9"/>
-      <c r="T26" s="10"/>
-    </row>
-    <row r="27" spans="1:20" ht="72" x14ac:dyDescent="0.3">
-      <c r="A27" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C27" s="8">
-        <v>2030</v>
-      </c>
-      <c r="D27" s="28">
-        <v>1173.7257628388072</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G27" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="H27" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="I27" s="23">
-        <f t="shared" si="3"/>
-        <v>1032878.6712981503</v>
-      </c>
-      <c r="J27" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="S27" s="9"/>
-      <c r="T27" s="10"/>
-    </row>
-    <row r="28" spans="1:20" ht="72" x14ac:dyDescent="0.3">
-      <c r="A28" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C28" s="8">
-        <v>2050</v>
-      </c>
-      <c r="D28" s="29">
-        <v>1173.7257628388072</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G28" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="H28" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="I28" s="23">
-        <f t="shared" si="3"/>
-        <v>1032878.6712981503</v>
-      </c>
-      <c r="J28" s="8" t="s">
-        <v>45</v>
-      </c>
+        <f>AVERAGE(I18,I19,I15,I16)</f>
+        <v>1005598.9652225529</v>
+      </c>
+      <c r="J22" s="8"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
-      <c r="D29" s="28"/>
+      <c r="D29" s="18"/>
       <c r="E29" s="1"/>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="23">
-        <f>AVERAGE(I26,I27,I23,I24)</f>
-        <v>1005598.9652225529</v>
-      </c>
-      <c r="J30" s="8"/>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3130,43 +3149,27 @@
     <hyperlink ref="F12" r:id="rId19" display="World Bank" xr:uid="{0EE4B772-3B1C-40C1-8489-D0631B2D4463}"/>
     <hyperlink ref="F13" r:id="rId20" display="World Bank" xr:uid="{C22641C2-FA38-48D9-BCB2-1FCE72A643D6}"/>
     <hyperlink ref="G10" r:id="rId21" xr:uid="{1BCFB97B-FADB-43D9-B44E-ADA05CA17A73}"/>
-    <hyperlink ref="F23" r:id="rId22" display="World Bank" xr:uid="{AF15079B-1809-4BD8-A648-4D62ABE8C206}"/>
-    <hyperlink ref="G23" r:id="rId23" xr:uid="{0CA73A59-1222-47DA-A59D-000D8B582034}"/>
-    <hyperlink ref="F24" r:id="rId24" display="World Bank" xr:uid="{199C7D2F-21A1-4692-9440-4CC169B6F2F2}"/>
-    <hyperlink ref="G24" r:id="rId25" xr:uid="{CECC446B-999A-4D89-A0D6-D3177C929A3D}"/>
-    <hyperlink ref="F25" r:id="rId26" display="World Bank" xr:uid="{8716B52B-0C43-4E99-8CCE-17C58FE13622}"/>
-    <hyperlink ref="G25" r:id="rId27" xr:uid="{85050209-E008-45C2-8A24-F79F70751A59}"/>
+    <hyperlink ref="F15" r:id="rId22" display="World Bank" xr:uid="{AF15079B-1809-4BD8-A648-4D62ABE8C206}"/>
+    <hyperlink ref="G15" r:id="rId23" xr:uid="{0CA73A59-1222-47DA-A59D-000D8B582034}"/>
+    <hyperlink ref="F16" r:id="rId24" display="World Bank" xr:uid="{199C7D2F-21A1-4692-9440-4CC169B6F2F2}"/>
+    <hyperlink ref="G16" r:id="rId25" xr:uid="{CECC446B-999A-4D89-A0D6-D3177C929A3D}"/>
+    <hyperlink ref="F17" r:id="rId26" display="World Bank" xr:uid="{8716B52B-0C43-4E99-8CCE-17C58FE13622}"/>
+    <hyperlink ref="G17" r:id="rId27" xr:uid="{85050209-E008-45C2-8A24-F79F70751A59}"/>
     <hyperlink ref="G11:G13" r:id="rId28" display="Dati elaborati da NREL" xr:uid="{8CAF9D49-1D95-457A-AD06-EF2B25EC7C48}"/>
-    <hyperlink ref="H23" r:id="rId29" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{BD06F35F-2859-4868-A250-9877196A2A8B}"/>
-    <hyperlink ref="H24:H25" r:id="rId30" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{D5926397-0CC0-4EED-B446-ADD3939AFBF8}"/>
+    <hyperlink ref="H15" r:id="rId29" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{BD06F35F-2859-4868-A250-9877196A2A8B}"/>
+    <hyperlink ref="H16:H17" r:id="rId30" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{D5926397-0CC0-4EED-B446-ADD3939AFBF8}"/>
     <hyperlink ref="R3" r:id="rId31" xr:uid="{1F188A66-AA31-42D5-BF68-5F94EC7F5B80}"/>
-    <hyperlink ref="F22" r:id="rId32" xr:uid="{BBB5C12E-09F8-42A0-BC0B-98E2FE229F3F}"/>
-    <hyperlink ref="H22" r:id="rId33" display="Overnight cost, suggerito da Lorenzo Mazzocco (vedi messaggio discord su Coordinamento energia)" xr:uid="{7623CF7E-7357-466F-811C-79E8E0B20885}"/>
-    <hyperlink ref="F26" r:id="rId34" display="World Bank" xr:uid="{A46629F6-B5CF-4B20-92CC-DAAA37FA0295}"/>
-    <hyperlink ref="G26" r:id="rId35" xr:uid="{4C8330BE-8E6C-45DA-8011-98C7288331BF}"/>
-    <hyperlink ref="H26" r:id="rId36" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{DBA68ACF-849E-462B-8CC2-2BE6A9705126}"/>
-    <hyperlink ref="F27" r:id="rId37" display="World Bank" xr:uid="{E1E46D67-8566-4081-8026-9282FEEA7794}"/>
-    <hyperlink ref="F28" r:id="rId38" display="World Bank" xr:uid="{C2B4C806-3E78-4AEF-A359-42B49AF6C869}"/>
-    <hyperlink ref="G27" r:id="rId39" xr:uid="{A07DD3DB-85F5-450E-BE7A-F242BAF7D635}"/>
-    <hyperlink ref="G28" r:id="rId40" xr:uid="{CB5BF0A4-3E46-40DE-9A2B-D68DCB0772EB}"/>
-    <hyperlink ref="H27" r:id="rId41" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{2364EE2D-C0F7-4609-B6E2-FD4BE059C070}"/>
-    <hyperlink ref="H28" r:id="rId42" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{222C5FBD-1584-4E8E-8AE1-8423CB925839}"/>
-    <hyperlink ref="F14" r:id="rId43" display="World Bank" xr:uid="{E6B37642-D048-481C-9CC7-5A49E1FAF2CA}"/>
-    <hyperlink ref="F15" r:id="rId44" display="World Bank" xr:uid="{84A1BEF5-1A35-4339-BC8F-1422193D060B}"/>
-    <hyperlink ref="F16" r:id="rId45" display="World Bank" xr:uid="{F64E52A3-071D-493B-B9F5-54A99596FF8A}"/>
-    <hyperlink ref="F17" r:id="rId46" display="World Bank" xr:uid="{007C4746-D8D7-4BB4-9A98-094B413757E0}"/>
-    <hyperlink ref="F18" r:id="rId47" display="World Bank" xr:uid="{2ED50F93-82F0-4419-934B-859DBAF4AF86}"/>
-    <hyperlink ref="F19" r:id="rId48" display="World Bank" xr:uid="{4152C890-4CBC-4765-9676-DA66A17BA52D}"/>
-    <hyperlink ref="F20" r:id="rId49" display="World Bank" xr:uid="{36A7A00F-693D-4DAE-9AF0-675C47F8279D}"/>
-    <hyperlink ref="F21" r:id="rId50" display="World Bank" xr:uid="{3860649B-A612-480C-B0EF-543D2BC864C7}"/>
-    <hyperlink ref="G14" r:id="rId51" xr:uid="{FC002B2B-3217-4129-88DA-356B844CE48E}"/>
-    <hyperlink ref="G15" r:id="rId52" xr:uid="{94E9F270-83DE-4273-954E-96F713533C46}"/>
-    <hyperlink ref="G16" r:id="rId53" xr:uid="{487E5883-403D-40EC-91F6-69377FC88A21}"/>
-    <hyperlink ref="G17" r:id="rId54" xr:uid="{AEA5CDB1-5155-4166-A825-786CA9AB969B}"/>
-    <hyperlink ref="G18" r:id="rId55" xr:uid="{2C8D643E-A3EA-469A-BB23-74E3B07C68EF}"/>
-    <hyperlink ref="G19" r:id="rId56" xr:uid="{2550B267-0DEF-4867-BFB8-835C895322D8}"/>
-    <hyperlink ref="G20" r:id="rId57" xr:uid="{F41DC907-DAFD-4054-B9F6-FF5FB48AE9FA}"/>
-    <hyperlink ref="G21" r:id="rId58" xr:uid="{2EFD1AB9-F361-4E75-A928-2E6F74388126}"/>
+    <hyperlink ref="F14" r:id="rId32" xr:uid="{BBB5C12E-09F8-42A0-BC0B-98E2FE229F3F}"/>
+    <hyperlink ref="H14" r:id="rId33" display="Overnight cost, suggerito da Lorenzo Mazzocco (vedi messaggio discord su Coordinamento energia)" xr:uid="{7623CF7E-7357-466F-811C-79E8E0B20885}"/>
+    <hyperlink ref="F18" r:id="rId34" display="World Bank" xr:uid="{A46629F6-B5CF-4B20-92CC-DAAA37FA0295}"/>
+    <hyperlink ref="G18" r:id="rId35" xr:uid="{4C8330BE-8E6C-45DA-8011-98C7288331BF}"/>
+    <hyperlink ref="H18" r:id="rId36" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{DBA68ACF-849E-462B-8CC2-2BE6A9705126}"/>
+    <hyperlink ref="F19" r:id="rId37" display="World Bank" xr:uid="{E1E46D67-8566-4081-8026-9282FEEA7794}"/>
+    <hyperlink ref="F20" r:id="rId38" display="World Bank" xr:uid="{C2B4C806-3E78-4AEF-A359-42B49AF6C869}"/>
+    <hyperlink ref="G19" r:id="rId39" xr:uid="{A07DD3DB-85F5-450E-BE7A-F242BAF7D635}"/>
+    <hyperlink ref="G20" r:id="rId40" xr:uid="{CB5BF0A4-3E46-40DE-9A2B-D68DCB0772EB}"/>
+    <hyperlink ref="H19" r:id="rId41" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{2364EE2D-C0F7-4609-B6E2-FD4BE059C070}"/>
+    <hyperlink ref="H20" r:id="rId42" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{222C5FBD-1584-4E8E-8AE1-8423CB925839}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added hydro_inflows per node, added climate data
</commit_message>
<xml_diff>
--- a/dati_casoStudioItalia/altri_dati.xlsx
+++ b/dati_casoStudioItalia/altri_dati.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DrinDrin\dati_casoStudioItalia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3E9678-A73D-4A20-B42E-4F005D2E7DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C547F90F-F897-44F6-83BD-390C2A939836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{B845255D-815F-49EA-8438-49CAB31B3547}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{B845255D-815F-49EA-8438-49CAB31B3547}"/>
   </bookViews>
   <sheets>
     <sheet name="OPEX" sheetId="6" r:id="rId1"/>
@@ -1296,8 +1296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C372154-4B0A-49B9-8FF3-F49D60098BF7}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1397,7 +1397,7 @@
         <v>72</v>
       </c>
       <c r="B6" s="34">
-        <v>1</v>
+        <v>1000000</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>7</v>
@@ -1408,7 +1408,7 @@
         <v>73</v>
       </c>
       <c r="B7" s="34">
-        <v>2</v>
+        <v>1000000</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>7</v>
@@ -1419,7 +1419,7 @@
         <v>75</v>
       </c>
       <c r="B8" s="34">
-        <v>2</v>
+        <v>1000000</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>7</v>
@@ -1430,7 +1430,7 @@
         <v>77</v>
       </c>
       <c r="B9" s="34">
-        <v>2</v>
+        <v>1000000</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>9</v>
@@ -1541,7 +1541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25E773EF-BD6E-41C4-818D-318BE958C680}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update costi techs (Danish Energy Agency)
</commit_message>
<xml_diff>
--- a/dati_casoStudioItalia/altri_dati.xlsx
+++ b/dati_casoStudioItalia/altri_dati.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DrinDrin\dati_casoStudioItalia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/gianvito_colucci_polito_it/Documents/Jobs/DRIN DRIN/Energy mix/DrinDrin---Mix-energetico/dati_casoStudioItalia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3E9678-A73D-4A20-B42E-4F005D2E7DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="225" documentId="13_ncr:1_{3F3E9678-A73D-4A20-B42E-4F005D2E7DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2BB85D4-0850-4FF1-AF62-92DB718E3833}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{B845255D-815F-49EA-8438-49CAB31B3547}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="5" xr2:uid="{B845255D-815F-49EA-8438-49CAB31B3547}"/>
   </bookViews>
   <sheets>
     <sheet name="OPEX" sheetId="6" r:id="rId1"/>
@@ -46,31 +46,6 @@
     <author>Bertoni, L. (Luca)</author>
   </authors>
   <commentList>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{52950CF3-9BD0-40D6-94D2-8E0C1D67B00B}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Bertoni, L. (Luca):</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-in MWh
-</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="A7" authorId="0" shapeId="0" xr:uid="{6042687D-A9B5-4779-9A54-E22AF9FBB252}">
       <text>
         <r>
@@ -303,7 +278,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="120">
   <si>
     <t>CAPEX solare</t>
   </si>
@@ -449,9 +424,6 @@
     <t>Average annual value, 2024</t>
   </si>
   <si>
-    <t>Average, 2020-2030</t>
-  </si>
-  <si>
     <t>(M$2025/GW)</t>
   </si>
   <si>
@@ -482,9 +454,6 @@
     <t>Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno "storage duration" di 4 ore. Per ulteriori info, vedere questo paper</t>
   </si>
   <si>
-    <t>Average 2h-4h, 2020-2030</t>
-  </si>
-  <si>
     <t>(c$2021/kWh)</t>
   </si>
   <si>
@@ -597,6 +566,78 @@
   </si>
   <si>
     <t>emission_factor_t/MWh</t>
+  </si>
+  <si>
+    <t>CAPEX idroelettrico</t>
+  </si>
+  <si>
+    <t>CAPEX PHS</t>
+  </si>
+  <si>
+    <t>CAPEX carbone</t>
+  </si>
+  <si>
+    <t>Ciclo a vapore</t>
+  </si>
+  <si>
+    <t>CAPEX gas</t>
+  </si>
+  <si>
+    <t>Ciclo combinato</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Utility</t>
+  </si>
+  <si>
+    <t>Mixed investment costs based on average of 50% 'solar-rooftop' and 50% 'solar-utility'</t>
+  </si>
+  <si>
+    <t>PyPSA/technology-data</t>
+  </si>
+  <si>
+    <t>(M$2015/GW)</t>
+  </si>
+  <si>
+    <t>€2020/€2015</t>
+  </si>
+  <si>
+    <t>Durata dovrebbe essere di 2 h</t>
+  </si>
+  <si>
+    <t>2 h - utility</t>
+  </si>
+  <si>
+    <t>2 h - home</t>
+  </si>
+  <si>
+    <t>(M€2015/GW)</t>
+  </si>
+  <si>
+    <t>Gas turbine, simple cycle</t>
+  </si>
+  <si>
+    <t>(M€2010/GW)</t>
+  </si>
+  <si>
+    <t>€2010/€2015</t>
+  </si>
+  <si>
+    <t>2025-Mixed investment costs based on average of 50% 'solar-rooftop' and 50% 'solar-utility'</t>
+  </si>
+  <si>
+    <t>2025, 2 h, Average utility-home</t>
+  </si>
+  <si>
+    <t>2025, Gas turbine, simple cycle</t>
+  </si>
+  <si>
+    <t>Dati elaborati da Danish Energy Agency</t>
+  </si>
+  <si>
+    <t>(€2015/MWh)</t>
   </si>
 </sst>
 </file>
@@ -607,7 +648,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0E+00"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -698,6 +739,51 @@
       <sz val="11"/>
       <name val="Aptos Narrow"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -727,7 +813,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -823,8 +909,71 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1165,7 +1314,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1179,7 +1328,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -1193,98 +1342,98 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B2" s="8">
         <v>0.04</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B3" s="8">
         <v>0.04</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B4" s="8">
         <v>0.04</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B5" s="8">
         <v>0.04</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B6" s="8">
         <v>0.04</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B7" s="8">
         <v>0.04</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B8" s="8">
         <v>0.04</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B9" s="8">
         <v>0.04</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1297,7 +1446,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E9"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1311,7 +1460,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -1323,43 +1472,43 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="8">
-        <v>918280</v>
+        <v>72</v>
+      </c>
+      <c r="B2" s="23">
+        <v>676570.29999999993</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+      <c r="E2" s="50" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B3" s="8">
-        <v>1063920</v>
+        <v>1208275.5560000001</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>48</v>
+        <v>105</v>
+      </c>
+      <c r="E3" s="27">
+        <v>2025</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B4" s="8">
         <v>3154360</v>
@@ -1368,80 +1517,111 @@
         <v>7</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" s="33">
-        <f>1005598.96522255*0.3</f>
-        <v>301679.68956676498</v>
+        <v>74</v>
+      </c>
+      <c r="B5" s="10">
+        <f>506759.606*0.3</f>
+        <v>152027.8818</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" s="34">
-        <v>1</v>
+        <v>70</v>
+      </c>
+      <c r="B6" s="49">
+        <v>2593292.1779999998</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" s="51">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" s="34">
-        <v>2</v>
+        <v>71</v>
+      </c>
+      <c r="B7" s="33">
+        <v>644986.04399999999</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>75</v>
-      </c>
-      <c r="B8" s="34">
-        <v>2</v>
+        <v>73</v>
+      </c>
+      <c r="B8" s="33">
+        <v>2109090.4800000004</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D8" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" s="27">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>77</v>
-      </c>
-      <c r="B9" s="34">
-        <v>2</v>
+        <v>75</v>
+      </c>
+      <c r="B9" s="56">
+        <v>60498.506250000006</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>9</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" s="51">
+        <v>2025</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{76843948-9A3E-4EB0-A540-24DF6B66F999}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{D3DAE58A-78C9-42A3-AACE-003B92F3B755}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{4F66A19D-E563-4CE0-A0F8-405FBE5A76EE}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{27416DF2-25A2-40A4-ADBE-E01677AB7CAF}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{0EC7236B-99A1-46EF-8EA3-6832779019E9}"/>
+    <hyperlink ref="D8" r:id="rId6" xr:uid="{34FFE429-8ADC-4F03-A78F-036552A631F1}"/>
+    <hyperlink ref="D6" r:id="rId7" xr:uid="{E8D8F775-B077-49C3-91F8-A7497013BEB0}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{4A9E0CE3-D16C-464A-84CE-CA642CBCF8D2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -1464,7 +1644,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -1478,7 +1658,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B2" s="23">
         <v>27.538556570687646</v>
@@ -1495,7 +1675,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B3" s="23">
         <v>10.331146370574086</v>
@@ -1512,7 +1692,7 @@
     </row>
     <row r="4" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B4" s="23">
         <v>4.8</v>
@@ -1521,10 +1701,10 @@
         <v>2</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1541,7 +1721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25E773EF-BD6E-41C4-818D-318BE958C680}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -1556,13 +1736,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E1" t="s">
         <v>8</v>
@@ -1573,7 +1753,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B2" s="8">
         <v>10138</v>
@@ -1585,15 +1765,15 @@
         <v>0.1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="35" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B3" s="34">
         <v>1</v>
@@ -1608,7 +1788,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="35" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B4" s="34">
         <v>1</v>
@@ -1623,7 +1803,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="35" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B5" s="34">
         <v>1</v>
@@ -1637,7 +1817,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="35" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B6" s="34">
         <v>1</v>
@@ -1651,7 +1831,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="35" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B7" s="34">
         <v>1</v>
@@ -1665,7 +1845,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="35" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B8" s="34">
         <v>1</v>
@@ -1686,7 +1866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42806216-DB6B-4ED6-9AA4-BC1B162122E7}">
   <dimension ref="A1:Y27"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16:G18"/>
     </sheetView>
   </sheetViews>
@@ -1949,7 +2129,7 @@
         <v>26</v>
       </c>
       <c r="L7" s="15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M7" s="11">
         <v>0.82</v>
@@ -2210,10 +2390,10 @@
         <v>0.46</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G16" s="9">
         <f>C16*M7/100*1000</f>
@@ -2230,16 +2410,16 @@
         <v>1</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C17" s="21">
         <v>7</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G17" s="9">
         <f>C17*M7</f>
@@ -2262,10 +2442,10 @@
         <v>0.61</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G18" s="9">
         <f>C18*M7/100*1000</f>
@@ -2320,10 +2500,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F958822-C8DD-4CF0-BC79-5189EFFDF89D}">
-  <dimension ref="A1:T29"/>
+  <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3:R3"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2341,7 +2521,7 @@
     <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -2373,7 +2553,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -2413,7 +2593,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
@@ -2437,7 +2617,7 @@
       </c>
       <c r="H3" s="24"/>
       <c r="I3" s="23">
-        <f t="shared" ref="I3:I8" si="0">D3*$Q$3*10^3</f>
+        <f t="shared" ref="I3:I12" si="0">D3*$Q$3*10^3</f>
         <v>663520</v>
       </c>
       <c r="J3" s="8" t="s">
@@ -2453,80 +2633,100 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="8">
-        <v>2020</v>
-      </c>
-      <c r="D4" s="23">
-        <v>1462</v>
-      </c>
-      <c r="E4" s="1" t="s">
+    <row r="4" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="38">
+        <v>2025</v>
+      </c>
+      <c r="D4" s="37">
+        <v>676.57029999999997</v>
+      </c>
+      <c r="E4" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" s="24"/>
-      <c r="I4" s="23">
-        <f t="shared" si="0"/>
-        <v>1286560</v>
-      </c>
-      <c r="J4" s="8" t="s">
+      <c r="F4" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="H4" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="I4" s="36">
+        <f>D4*10^3</f>
+        <v>676570.29999999993</v>
+      </c>
+      <c r="J4" s="38" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="P4" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q4" s="11">
+        <v>1.06</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>40</v>
+        <v>103</v>
       </c>
       <c r="C5" s="8">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="D5" s="23">
-        <v>956</v>
+        <v>473.11559999999997</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>36</v>
+        <v>105</v>
+      </c>
+      <c r="G5" s="41" t="s">
+        <v>118</v>
       </c>
       <c r="H5" s="24"/>
       <c r="I5" s="23">
-        <f t="shared" si="0"/>
-        <v>841280</v>
+        <f>D5*10^3</f>
+        <v>473115.6</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="P5" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q5" s="11">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="8">
         <v>2020</v>
       </c>
       <c r="D6" s="23">
-        <v>3739</v>
+        <v>1462</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>28</v>
@@ -2540,24 +2740,24 @@
       <c r="H6" s="24"/>
       <c r="I6" s="23">
         <f t="shared" si="0"/>
-        <v>3290320</v>
+        <v>1286560</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="8">
         <v>2030</v>
       </c>
       <c r="D7" s="23">
-        <v>2758</v>
+        <v>956</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>28</v>
@@ -2571,560 +2771,967 @@
       <c r="H7" s="24"/>
       <c r="I7" s="23">
         <f t="shared" si="0"/>
-        <v>2427040</v>
+        <v>841280</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="38">
+        <v>2025</v>
+      </c>
+      <c r="D8" s="36">
+        <v>1139.8825999999999</v>
+      </c>
+      <c r="E8" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="G8" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="H8" s="42"/>
+      <c r="I8" s="43">
+        <f>D8*$Q$4*10^3</f>
+        <v>1208275.5560000001</v>
+      </c>
+      <c r="J8" s="38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="8">
+        <v>2020</v>
+      </c>
+      <c r="D9" s="23">
+        <v>3739</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="44"/>
+      <c r="I9" s="45">
+        <f t="shared" si="0"/>
+        <v>3290320</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="8">
+        <v>2030</v>
+      </c>
+      <c r="D10" s="23">
+        <v>2758</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="44"/>
+      <c r="I10" s="45">
+        <f t="shared" si="0"/>
+        <v>2427040</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="33">
+        <v>2025</v>
+      </c>
+      <c r="D11" s="52">
+        <v>1769.1170999999999</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="53" t="s">
+        <v>105</v>
+      </c>
+      <c r="G11" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="H11" s="55"/>
+      <c r="I11" s="45">
+        <f>D11*10^3</f>
+        <v>1769117.0999999999</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C12" s="8">
         <v>2020</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D12" s="23">
         <v>4049</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F12" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G12" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="H8" s="24"/>
-      <c r="I8" s="23">
+      <c r="H12" s="24"/>
+      <c r="I12" s="23">
         <f t="shared" si="0"/>
         <v>3563120</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="J12" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B13" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C13" s="8">
         <v>2030</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D13" s="23">
         <v>3467</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F13" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="24" t="s">
+      <c r="G13" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="24"/>
-      <c r="I9" s="23">
-        <f>D9*$Q$3*10^3</f>
+      <c r="H13" s="24"/>
+      <c r="I13" s="23">
+        <f>D13*$Q$3*10^3</f>
         <v>3050960</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="J13" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" s="8">
+      <c r="B14" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="8">
         <v>2035</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D14" s="23">
         <v>6160.0000000000009</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F14" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="24" t="s">
+      <c r="G14" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="25" t="s">
+      <c r="H14" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="I10" s="23">
-        <f t="shared" ref="I10:I17" si="1">D10*$Q$3*10^3</f>
+      <c r="I14" s="23">
+        <f t="shared" ref="I14:I29" si="1">D14*$Q$3*10^3</f>
         <v>5420800.0000000009</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="J14" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" s="8">
+      <c r="B15" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="8">
         <v>2050</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D15" s="23">
         <v>5500</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F15" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="24" t="s">
+      <c r="G15" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="25" t="s">
+      <c r="H15" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="I11" s="23">
+      <c r="I15" s="23">
         <f t="shared" si="1"/>
         <v>4840000</v>
       </c>
-      <c r="J11" s="8" t="s">
+      <c r="J15" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="8">
+      <c r="B16" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="8">
         <v>2035</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D16" s="23">
         <v>6820.0000000000009</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F16" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="24" t="s">
+      <c r="G16" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="H12" s="25" t="s">
+      <c r="H16" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="I12" s="23">
+      <c r="I16" s="23">
         <f t="shared" si="1"/>
         <v>6001600.0000000009</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="J16" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="8">
+      <c r="B17" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="8">
         <v>2050</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D17" s="23">
         <v>6050.0000000000009</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F17" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="24" t="s">
+      <c r="G17" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="H13" s="25" t="s">
+      <c r="H17" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="I13" s="23">
+      <c r="I17" s="23">
         <f t="shared" si="1"/>
         <v>5324000.0000000009</v>
       </c>
-      <c r="J13" s="8" t="s">
+      <c r="J17" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+    <row r="18" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38">
+        <v>2025</v>
+      </c>
+      <c r="D18" s="36">
+        <v>2274.8177000000001</v>
+      </c>
+      <c r="E18" s="39" t="s">
+        <v>113</v>
+      </c>
+      <c r="F18" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="G18" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="H18" s="48"/>
+      <c r="I18" s="36">
+        <f>D18*$Q$5*10^3</f>
+        <v>2593292.1779999998</v>
+      </c>
+      <c r="J18" s="38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38">
+        <v>2025</v>
+      </c>
+      <c r="D19" s="36">
+        <v>57074.0625</v>
+      </c>
+      <c r="E19" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="F19" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="G19" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="H19" s="48"/>
+      <c r="I19" s="36">
+        <f>D19*$Q$4</f>
+        <v>60498.506250000006</v>
+      </c>
+      <c r="J19" s="38" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" s="8">
+        <v>2020</v>
+      </c>
+      <c r="D20" s="23">
+        <v>3075</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="H20" s="25"/>
+      <c r="I20" s="23">
+        <f t="shared" si="1"/>
+        <v>2706000</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" s="8">
+        <v>2030</v>
+      </c>
+      <c r="D21" s="23">
+        <v>2240</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="H21" s="25"/>
+      <c r="I21" s="23">
+        <f t="shared" si="1"/>
+        <v>1971200</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" s="38"/>
+      <c r="C22" s="38">
+        <v>2025</v>
+      </c>
+      <c r="D22" s="36">
+        <v>1989.7080000000001</v>
+      </c>
+      <c r="E22" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="F22" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="G22" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="H22" s="48"/>
+      <c r="I22" s="36">
+        <f>D22*$Q$4*10^3</f>
+        <v>2109090.4800000004</v>
+      </c>
+      <c r="J22" s="38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" s="8">
+        <v>2020</v>
+      </c>
+      <c r="D23" s="23">
+        <v>1038</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="H23" s="25"/>
+      <c r="I23" s="23">
+        <f t="shared" si="1"/>
+        <v>913440</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" s="8">
+        <v>2030</v>
+      </c>
+      <c r="D24" s="23">
+        <v>838</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="H24" s="25"/>
+      <c r="I24" s="23">
+        <f t="shared" si="1"/>
+        <v>737440</v>
+      </c>
+      <c r="J24" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="C25" s="38">
+        <v>2025</v>
+      </c>
+      <c r="D25" s="36">
+        <v>608.47739999999999</v>
+      </c>
+      <c r="E25" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="F25" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="G25" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="H25" s="48"/>
+      <c r="I25" s="36">
+        <f>D25*$Q$4*10^3</f>
+        <v>644986.04399999999</v>
+      </c>
+      <c r="J25" s="38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="8">
+      <c r="B26" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="8">
         <v>2025</v>
       </c>
-      <c r="D14" s="23">
+      <c r="D26" s="23">
         <v>5350</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F26" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="26" t="s">
+      <c r="G26" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="H26" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="G14" s="25" t="s">
+      <c r="I26" s="23">
+        <f>D26*$Q$3*10^3*0.67</f>
+        <v>3154360</v>
+      </c>
+      <c r="J26" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="H14" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="I14" s="23">
-        <f>D14*$Q$3*10^3*0.67</f>
-        <v>3154360</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" ht="72" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="8">
+      <c r="C27" s="8">
         <v>2020</v>
       </c>
-      <c r="D15" s="28">
+      <c r="D27" s="28">
         <v>988.32170015695567</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F27" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="24" t="s">
+      <c r="G27" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="H15" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="I15" s="23">
+      <c r="H27" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="I27" s="23">
         <f t="shared" si="1"/>
         <v>869723.09613812109</v>
       </c>
-      <c r="J15" s="8" t="s">
+      <c r="J27" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="R15" s="2"/>
-      <c r="S15" s="6"/>
-      <c r="T15" s="6"/>
-    </row>
-    <row r="16" spans="1:20" ht="72" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
+      <c r="R27" s="2"/>
+      <c r="S27" s="6"/>
+      <c r="T27" s="6"/>
+    </row>
+    <row r="28" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+      <c r="A28" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="8">
+      <c r="B28" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="8">
         <v>2030</v>
       </c>
-      <c r="D16" s="28">
+      <c r="D28" s="28">
         <v>681.62247956991291</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F28" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G16" s="24" t="s">
+      <c r="G28" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="H16" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="I16" s="23">
+      <c r="H28" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="I28" s="23">
         <f t="shared" si="1"/>
         <v>599827.78202152334</v>
       </c>
-      <c r="J16" s="8" t="s">
+      <c r="J28" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="R16" s="2"/>
-      <c r="S16" s="4"/>
-      <c r="T16" s="4"/>
-    </row>
-    <row r="17" spans="1:20" ht="72" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
+      <c r="R28" s="2"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="4"/>
+    </row>
+    <row r="29" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+      <c r="A29" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" s="8">
+      <c r="B29" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="8">
         <v>2050</v>
       </c>
-      <c r="D17" s="29">
+      <c r="D29" s="29">
         <v>681.62247956991291</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F29" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="24" t="s">
+      <c r="G29" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="H17" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="I17" s="23">
+      <c r="H29" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="I29" s="23">
         <f t="shared" si="1"/>
         <v>599827.78202152334</v>
       </c>
-      <c r="J17" s="8" t="s">
+      <c r="J29" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="R17" s="2"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
-    </row>
-    <row r="18" spans="1:20" ht="72" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
+      <c r="R29" s="2"/>
+      <c r="S29" s="5"/>
+      <c r="T29" s="5"/>
+    </row>
+    <row r="30" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+      <c r="A30" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="8">
+      <c r="B30" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="8">
         <v>2020</v>
       </c>
-      <c r="D18" s="28">
+      <c r="D30" s="28">
         <v>1727.2344448095646</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F30" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G18" s="24" t="s">
+      <c r="G30" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="H18" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="I18" s="23">
-        <f t="shared" ref="I18:I20" si="2">D18*$Q$3*10^3</f>
+      <c r="H30" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="I30" s="23">
+        <f t="shared" ref="I30:I32" si="2">D30*$Q$3*10^3</f>
         <v>1519966.3114324168</v>
       </c>
-      <c r="J18" s="8" t="s">
+      <c r="J30" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="S18" s="9"/>
-      <c r="T18" s="10"/>
-    </row>
-    <row r="19" spans="1:20" ht="72" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
+      <c r="S30" s="9"/>
+      <c r="T30" s="10"/>
+    </row>
+    <row r="31" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+      <c r="A31" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="8">
+      <c r="B31" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="8">
         <v>2030</v>
       </c>
-      <c r="D19" s="28">
+      <c r="D31" s="28">
         <v>1173.7257628388072</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F31" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G19" s="24" t="s">
+      <c r="G31" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="H19" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="I19" s="23">
+      <c r="H31" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="I31" s="23">
         <f t="shared" si="2"/>
         <v>1032878.6712981503</v>
       </c>
-      <c r="J19" s="8" t="s">
+      <c r="J31" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="S19" s="9"/>
-      <c r="T19" s="10"/>
-    </row>
-    <row r="20" spans="1:20" ht="72" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
+      <c r="S31" s="9"/>
+      <c r="T31" s="10"/>
+    </row>
+    <row r="32" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+      <c r="A32" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="8">
+      <c r="B32" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="8">
         <v>2050</v>
       </c>
-      <c r="D20" s="29">
+      <c r="D32" s="29">
         <v>1173.7257628388072</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F32" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="24" t="s">
+      <c r="G32" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="H20" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="I20" s="23">
+      <c r="H32" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="I32" s="23">
         <f t="shared" si="2"/>
         <v>1032878.6712981503</v>
       </c>
-      <c r="J20" s="8" t="s">
+      <c r="J32" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="23">
-        <f>AVERAGE(I18,I19,I15,I16)</f>
-        <v>1005598.9652225529</v>
-      </c>
-      <c r="J22" s="8"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
+    <row r="33" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" s="38">
+        <v>2025</v>
+      </c>
+      <c r="D33" s="46">
+        <f>197.8874*2</f>
+        <v>395.77480000000003</v>
+      </c>
+      <c r="E33" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="F33" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="G33" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="H33" s="47" t="s">
+        <v>108</v>
+      </c>
+      <c r="I33" s="36">
+        <f>D33*$Q$4*10^3</f>
+        <v>419521.288</v>
+      </c>
+      <c r="J33" s="38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" s="38">
+        <v>2025</v>
+      </c>
+      <c r="D34" s="36">
+        <f>280.1877*2</f>
+        <v>560.37540000000001</v>
+      </c>
+      <c r="E34" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="F34" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="G34" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="H34" s="47" t="s">
+        <v>108</v>
+      </c>
+      <c r="I34" s="36">
+        <f>D34*$Q$4*10^3</f>
+        <v>593997.924</v>
+      </c>
+      <c r="J34" s="38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="8"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="23"/>
+      <c r="J37" s="8"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="8"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="8"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3132,44 +3739,65 @@
     <hyperlink ref="G2" r:id="rId2" xr:uid="{E134E359-0624-4ADD-AE0D-E6195FFD25A4}"/>
     <hyperlink ref="F3" r:id="rId3" display="World Bank" xr:uid="{11649A99-BBF5-429D-92C0-B1AB39DFCDAB}"/>
     <hyperlink ref="G3" r:id="rId4" xr:uid="{63198A70-1594-447D-BF39-AD7C3371EF67}"/>
-    <hyperlink ref="F4" r:id="rId5" display="World Bank" xr:uid="{234A250E-341C-41EF-9E6C-5F70C9AD1AA2}"/>
-    <hyperlink ref="F5" r:id="rId6" display="World Bank" xr:uid="{24ED7D87-6BA0-4591-B8FB-8DBFC7C67291}"/>
-    <hyperlink ref="F6" r:id="rId7" display="World Bank" xr:uid="{4E4A5E32-C5B0-4B55-BC1D-A8BCB8AB3343}"/>
-    <hyperlink ref="F7" r:id="rId8" display="World Bank" xr:uid="{34A735C2-398A-4AF0-AC92-CDE49E221E44}"/>
-    <hyperlink ref="F8" r:id="rId9" display="World Bank" xr:uid="{D82100BF-E290-4C7F-83FE-7ACF88644A48}"/>
-    <hyperlink ref="F9" r:id="rId10" display="World Bank" xr:uid="{F0A57130-2B16-425F-838B-37D425B23764}"/>
-    <hyperlink ref="G4" r:id="rId11" xr:uid="{74C7DDA8-7917-4F78-B0B5-A38959B43587}"/>
-    <hyperlink ref="G5" r:id="rId12" xr:uid="{EA35BC2E-0439-4BB5-8635-24C6E1A59507}"/>
-    <hyperlink ref="G6" r:id="rId13" xr:uid="{CB8B6EC7-D21F-4093-AE53-04FF92EE23C3}"/>
-    <hyperlink ref="G7" r:id="rId14" xr:uid="{4BC76F65-9AF5-43B2-95D0-0E17535DD882}"/>
-    <hyperlink ref="G8" r:id="rId15" xr:uid="{254A0ED1-9B59-4B3A-800D-0B7D5611C9F8}"/>
-    <hyperlink ref="G9" r:id="rId16" xr:uid="{53F61002-38D5-4F86-850D-731FF68607AC}"/>
-    <hyperlink ref="F10" r:id="rId17" display="World Bank" xr:uid="{F0DC3470-B776-4B2D-B27E-08A0A05751B0}"/>
-    <hyperlink ref="F11" r:id="rId18" display="World Bank" xr:uid="{69B713EC-CE42-44B4-85A8-A3466168667C}"/>
-    <hyperlink ref="F12" r:id="rId19" display="World Bank" xr:uid="{0EE4B772-3B1C-40C1-8489-D0631B2D4463}"/>
-    <hyperlink ref="F13" r:id="rId20" display="World Bank" xr:uid="{C22641C2-FA38-48D9-BCB2-1FCE72A643D6}"/>
-    <hyperlink ref="G10" r:id="rId21" xr:uid="{1BCFB97B-FADB-43D9-B44E-ADA05CA17A73}"/>
-    <hyperlink ref="F15" r:id="rId22" display="World Bank" xr:uid="{AF15079B-1809-4BD8-A648-4D62ABE8C206}"/>
-    <hyperlink ref="G15" r:id="rId23" xr:uid="{0CA73A59-1222-47DA-A59D-000D8B582034}"/>
-    <hyperlink ref="F16" r:id="rId24" display="World Bank" xr:uid="{199C7D2F-21A1-4692-9440-4CC169B6F2F2}"/>
-    <hyperlink ref="G16" r:id="rId25" xr:uid="{CECC446B-999A-4D89-A0D6-D3177C929A3D}"/>
-    <hyperlink ref="F17" r:id="rId26" display="World Bank" xr:uid="{8716B52B-0C43-4E99-8CCE-17C58FE13622}"/>
-    <hyperlink ref="G17" r:id="rId27" xr:uid="{85050209-E008-45C2-8A24-F79F70751A59}"/>
-    <hyperlink ref="G11:G13" r:id="rId28" display="Dati elaborati da NREL" xr:uid="{8CAF9D49-1D95-457A-AD06-EF2B25EC7C48}"/>
-    <hyperlink ref="H15" r:id="rId29" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{BD06F35F-2859-4868-A250-9877196A2A8B}"/>
-    <hyperlink ref="H16:H17" r:id="rId30" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{D5926397-0CC0-4EED-B446-ADD3939AFBF8}"/>
+    <hyperlink ref="F6" r:id="rId5" display="World Bank" xr:uid="{234A250E-341C-41EF-9E6C-5F70C9AD1AA2}"/>
+    <hyperlink ref="F7" r:id="rId6" display="World Bank" xr:uid="{24ED7D87-6BA0-4591-B8FB-8DBFC7C67291}"/>
+    <hyperlink ref="F9" r:id="rId7" display="World Bank" xr:uid="{4E4A5E32-C5B0-4B55-BC1D-A8BCB8AB3343}"/>
+    <hyperlink ref="F10" r:id="rId8" display="World Bank" xr:uid="{34A735C2-398A-4AF0-AC92-CDE49E221E44}"/>
+    <hyperlink ref="F12" r:id="rId9" display="World Bank" xr:uid="{D82100BF-E290-4C7F-83FE-7ACF88644A48}"/>
+    <hyperlink ref="F13" r:id="rId10" display="World Bank" xr:uid="{F0A57130-2B16-425F-838B-37D425B23764}"/>
+    <hyperlink ref="G6" r:id="rId11" xr:uid="{74C7DDA8-7917-4F78-B0B5-A38959B43587}"/>
+    <hyperlink ref="G7" r:id="rId12" xr:uid="{EA35BC2E-0439-4BB5-8635-24C6E1A59507}"/>
+    <hyperlink ref="G9" r:id="rId13" xr:uid="{CB8B6EC7-D21F-4093-AE53-04FF92EE23C3}"/>
+    <hyperlink ref="G10" r:id="rId14" xr:uid="{4BC76F65-9AF5-43B2-95D0-0E17535DD882}"/>
+    <hyperlink ref="G12" r:id="rId15" xr:uid="{254A0ED1-9B59-4B3A-800D-0B7D5611C9F8}"/>
+    <hyperlink ref="G13" r:id="rId16" xr:uid="{53F61002-38D5-4F86-850D-731FF68607AC}"/>
+    <hyperlink ref="F14" r:id="rId17" display="World Bank" xr:uid="{F0DC3470-B776-4B2D-B27E-08A0A05751B0}"/>
+    <hyperlink ref="F15" r:id="rId18" display="World Bank" xr:uid="{69B713EC-CE42-44B4-85A8-A3466168667C}"/>
+    <hyperlink ref="F16" r:id="rId19" display="World Bank" xr:uid="{0EE4B772-3B1C-40C1-8489-D0631B2D4463}"/>
+    <hyperlink ref="F17" r:id="rId20" display="World Bank" xr:uid="{C22641C2-FA38-48D9-BCB2-1FCE72A643D6}"/>
+    <hyperlink ref="G14" r:id="rId21" xr:uid="{1BCFB97B-FADB-43D9-B44E-ADA05CA17A73}"/>
+    <hyperlink ref="F27" r:id="rId22" display="World Bank" xr:uid="{AF15079B-1809-4BD8-A648-4D62ABE8C206}"/>
+    <hyperlink ref="G27" r:id="rId23" xr:uid="{0CA73A59-1222-47DA-A59D-000D8B582034}"/>
+    <hyperlink ref="F28" r:id="rId24" display="World Bank" xr:uid="{199C7D2F-21A1-4692-9440-4CC169B6F2F2}"/>
+    <hyperlink ref="G28" r:id="rId25" xr:uid="{CECC446B-999A-4D89-A0D6-D3177C929A3D}"/>
+    <hyperlink ref="F29" r:id="rId26" display="World Bank" xr:uid="{8716B52B-0C43-4E99-8CCE-17C58FE13622}"/>
+    <hyperlink ref="G29" r:id="rId27" xr:uid="{85050209-E008-45C2-8A24-F79F70751A59}"/>
+    <hyperlink ref="G15:G17" r:id="rId28" display="Dati elaborati da NREL" xr:uid="{8CAF9D49-1D95-457A-AD06-EF2B25EC7C48}"/>
+    <hyperlink ref="H27" r:id="rId29" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{BD06F35F-2859-4868-A250-9877196A2A8B}"/>
+    <hyperlink ref="H28:H29" r:id="rId30" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{D5926397-0CC0-4EED-B446-ADD3939AFBF8}"/>
     <hyperlink ref="R3" r:id="rId31" xr:uid="{1F188A66-AA31-42D5-BF68-5F94EC7F5B80}"/>
-    <hyperlink ref="F14" r:id="rId32" xr:uid="{BBB5C12E-09F8-42A0-BC0B-98E2FE229F3F}"/>
-    <hyperlink ref="H14" r:id="rId33" display="Overnight cost, suggerito da Lorenzo Mazzocco (vedi messaggio discord su Coordinamento energia)" xr:uid="{7623CF7E-7357-466F-811C-79E8E0B20885}"/>
-    <hyperlink ref="F18" r:id="rId34" display="World Bank" xr:uid="{A46629F6-B5CF-4B20-92CC-DAAA37FA0295}"/>
-    <hyperlink ref="G18" r:id="rId35" xr:uid="{4C8330BE-8E6C-45DA-8011-98C7288331BF}"/>
-    <hyperlink ref="H18" r:id="rId36" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{DBA68ACF-849E-462B-8CC2-2BE6A9705126}"/>
-    <hyperlink ref="F19" r:id="rId37" display="World Bank" xr:uid="{E1E46D67-8566-4081-8026-9282FEEA7794}"/>
-    <hyperlink ref="F20" r:id="rId38" display="World Bank" xr:uid="{C2B4C806-3E78-4AEF-A359-42B49AF6C869}"/>
-    <hyperlink ref="G19" r:id="rId39" xr:uid="{A07DD3DB-85F5-450E-BE7A-F242BAF7D635}"/>
-    <hyperlink ref="G20" r:id="rId40" xr:uid="{CB5BF0A4-3E46-40DE-9A2B-D68DCB0772EB}"/>
-    <hyperlink ref="H19" r:id="rId41" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{2364EE2D-C0F7-4609-B6E2-FD4BE059C070}"/>
-    <hyperlink ref="H20" r:id="rId42" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{222C5FBD-1584-4E8E-8AE1-8423CB925839}"/>
+    <hyperlink ref="F26" r:id="rId32" xr:uid="{BBB5C12E-09F8-42A0-BC0B-98E2FE229F3F}"/>
+    <hyperlink ref="H26" r:id="rId33" display="Overnight cost, suggerito da Lorenzo Mazzocco (vedi messaggio discord su Coordinamento energia)" xr:uid="{7623CF7E-7357-466F-811C-79E8E0B20885}"/>
+    <hyperlink ref="F30" r:id="rId34" display="World Bank" xr:uid="{A46629F6-B5CF-4B20-92CC-DAAA37FA0295}"/>
+    <hyperlink ref="G30" r:id="rId35" xr:uid="{4C8330BE-8E6C-45DA-8011-98C7288331BF}"/>
+    <hyperlink ref="H30" r:id="rId36" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{DBA68ACF-849E-462B-8CC2-2BE6A9705126}"/>
+    <hyperlink ref="F31" r:id="rId37" display="World Bank" xr:uid="{E1E46D67-8566-4081-8026-9282FEEA7794}"/>
+    <hyperlink ref="F32" r:id="rId38" display="World Bank" xr:uid="{C2B4C806-3E78-4AEF-A359-42B49AF6C869}"/>
+    <hyperlink ref="G31" r:id="rId39" xr:uid="{A07DD3DB-85F5-450E-BE7A-F242BAF7D635}"/>
+    <hyperlink ref="G32" r:id="rId40" xr:uid="{CB5BF0A4-3E46-40DE-9A2B-D68DCB0772EB}"/>
+    <hyperlink ref="H31" r:id="rId41" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{2364EE2D-C0F7-4609-B6E2-FD4BE059C070}"/>
+    <hyperlink ref="H32" r:id="rId42" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 6 ore. Per ulteriori info, vedere questo paper" xr:uid="{222C5FBD-1584-4E8E-8AE1-8423CB925839}"/>
+    <hyperlink ref="F20" r:id="rId43" display="World Bank" xr:uid="{144D646C-64DA-4184-9A12-DF7E1E799F17}"/>
+    <hyperlink ref="F21" r:id="rId44" display="World Bank" xr:uid="{86B096A8-BD30-4A89-9511-4059F8B3510E}"/>
+    <hyperlink ref="F23" r:id="rId45" display="World Bank" xr:uid="{696DD738-19D1-49F7-821B-56F8741182FD}"/>
+    <hyperlink ref="F24" r:id="rId46" display="World Bank" xr:uid="{3F2E4AE5-7757-40CD-A4F2-FA7451812D44}"/>
+    <hyperlink ref="G20" r:id="rId47" xr:uid="{37F5A6B5-EA7A-4E73-94DB-B4337F3B0C99}"/>
+    <hyperlink ref="G21" r:id="rId48" xr:uid="{274258D8-A309-4E31-88E8-4833EABC0CC8}"/>
+    <hyperlink ref="G23" r:id="rId49" xr:uid="{2BB0C756-C471-4708-B185-478B09E72710}"/>
+    <hyperlink ref="G24" r:id="rId50" xr:uid="{AC21D000-7C67-4597-A906-E0770FCED92C}"/>
+    <hyperlink ref="F4" r:id="rId51" xr:uid="{5D87E73B-1C45-44A9-9647-A816E1E5D102}"/>
+    <hyperlink ref="F5" r:id="rId52" xr:uid="{408D8586-4629-4006-A3A2-7382E5D36BD5}"/>
+    <hyperlink ref="F8" r:id="rId53" xr:uid="{135DDF62-C78C-42D0-8DC1-BDC7CBA22057}"/>
+    <hyperlink ref="F11" r:id="rId54" xr:uid="{FAF0EBAC-6E4A-490E-ABCA-3BFB19EB8D02}"/>
+    <hyperlink ref="H33" r:id="rId55" display="Durata dovrebbe essere di 2 h: vedere qui" xr:uid="{B7A9E32B-551D-453A-8ED3-733E625E714B}"/>
+    <hyperlink ref="F33" r:id="rId56" xr:uid="{78D3F3E0-DB9E-4087-B3AA-EB1E4D8B75BD}"/>
+    <hyperlink ref="H34" r:id="rId57" display="Durata dovrebbe essere di 2 h: vedere qui" xr:uid="{69359E17-3C66-48A7-8D80-D0D7D9FF3A61}"/>
+    <hyperlink ref="F34" r:id="rId58" xr:uid="{E844BEE8-4326-4848-9E13-EB17B475936B}"/>
+    <hyperlink ref="F25" r:id="rId59" xr:uid="{D488514D-CADA-463C-9D03-C37D102A130D}"/>
+    <hyperlink ref="F22" r:id="rId60" xr:uid="{F859514D-03DA-48AE-96D8-520E95C75762}"/>
+    <hyperlink ref="F18" r:id="rId61" xr:uid="{984B3FF9-23B1-40E7-A54B-5D874E8C0662}"/>
+    <hyperlink ref="F19" r:id="rId62" xr:uid="{14B54904-1E44-4343-A082-0DA88FF5D482}"/>
+    <hyperlink ref="R4:R5" r:id="rId63" display="Harmonised Index of Consumer Prices (HICP)" xr:uid="{5A3EEAB6-3263-4BE6-A4B6-04F42A57A8AA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Aggiornato PumpedHydro_Closed.json per avere la corretta potenza in assorbimento/scarica. Corretto capacita' di stoccaggio in generazione_domanda_per_zona_v02
</commit_message>
<xml_diff>
--- a/dati_casoStudioItalia/altri_dati.xlsx
+++ b/dati_casoStudioItalia/altri_dati.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/gianvito_colucci_polito_it/Documents/Jobs/DRIN DRIN/Energy mix/DrinDrin---Mix-energetico/dati_casoStudioItalia/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DrinDrin\dati_casoStudioItalia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="225" documentId="13_ncr:1_{3F3E9678-A73D-4A20-B42E-4F005D2E7DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2BB85D4-0850-4FF1-AF62-92DB718E3833}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACAA9509-AF48-41A4-8FDF-C19F1B242289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="5" xr2:uid="{B845255D-815F-49EA-8438-49CAB31B3547}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{B845255D-815F-49EA-8438-49CAB31B3547}"/>
   </bookViews>
   <sheets>
     <sheet name="OPEX" sheetId="6" r:id="rId1"/>
@@ -1445,8 +1445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C372154-4B0A-49B9-8FF3-F49D60098BF7}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2502,7 +2502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F958822-C8DD-4CF0-BC79-5189EFFDF89D}">
   <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Riformulato import_networ, aggiunto discount_rate per tecnologia
</commit_message>
<xml_diff>
--- a/dati_casoStudioItalia/altri_dati.xlsx
+++ b/dati_casoStudioItalia/altri_dati.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DrinDrin\dati_casoStudioItalia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACAA9509-AF48-41A4-8FDF-C19F1B242289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C938171-31FE-4B0E-BFCE-241857C15E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{B845255D-815F-49EA-8438-49CAB31B3547}"/>
+    <workbookView xWindow="-2964" yWindow="-17388" windowWidth="30936" windowHeight="16896" xr2:uid="{B845255D-815F-49EA-8438-49CAB31B3547}"/>
   </bookViews>
   <sheets>
-    <sheet name="OPEX" sheetId="6" r:id="rId1"/>
-    <sheet name="CAPEX" sheetId="1" r:id="rId2"/>
-    <sheet name="Fuel_cost" sheetId="5" r:id="rId3"/>
-    <sheet name="Transmission_abroad" sheetId="4" r:id="rId4"/>
-    <sheet name="raw_data_commodity" sheetId="2" r:id="rId5"/>
-    <sheet name="raw_data_techs" sheetId="3" r:id="rId6"/>
+    <sheet name="discount_rate" sheetId="7" r:id="rId1"/>
+    <sheet name="OPEX" sheetId="6" r:id="rId2"/>
+    <sheet name="CAPEX" sheetId="1" r:id="rId3"/>
+    <sheet name="Fuel_cost" sheetId="5" r:id="rId4"/>
+    <sheet name="Transmission_abroad" sheetId="4" r:id="rId5"/>
+    <sheet name="raw_data_commodity" sheetId="2" r:id="rId6"/>
+    <sheet name="raw_data_techs" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -278,7 +279,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="121">
   <si>
     <t>CAPEX solare</t>
   </si>
@@ -638,6 +639,9 @@
   </si>
   <si>
     <t>(€2015/MWh)</t>
+  </si>
+  <si>
+    <t>discount_rate</t>
   </si>
 </sst>
 </file>
@@ -1310,6 +1314,138 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{923C661C-C997-4238-A47F-A35B6AA9581D}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="27"/>
+    </row>
+    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9398001-B177-42A1-9F09-DD1B7293885B}">
   <dimension ref="A1:E9"/>
   <sheetViews>
@@ -1441,11 +1577,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C372154-4B0A-49B9-8FF3-F49D60098BF7}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -1625,7 +1761,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F36F9B7-E410-4418-9AFE-4DC5A9893242}">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -1717,7 +1853,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25E773EF-BD6E-41C4-818D-318BE958C680}">
   <dimension ref="A1:F8"/>
   <sheetViews>
@@ -1862,7 +1998,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42806216-DB6B-4ED6-9AA4-BC1B162122E7}">
   <dimension ref="A1:Y27"/>
   <sheetViews>
@@ -2498,7 +2634,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F958822-C8DD-4CF0-BC79-5189EFFDF89D}">
   <dimension ref="A1:T41"/>
   <sheetViews>

</xml_diff>

<commit_message>
Dati: discount rate e FIXOM
</commit_message>
<xml_diff>
--- a/dati_casoStudioItalia/altri_dati.xlsx
+++ b/dati_casoStudioItalia/altri_dati.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DrinDrin\dati_casoStudioItalia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gianvito.colucci\OneDrive - Politecnico di Torino\Jobs\DRIN DRIN\Energy mix\DrinDrin---Mix-energetico\dati_casoStudioItalia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C938171-31FE-4B0E-BFCE-241857C15E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8C6BD1-24ED-46C2-A2CB-EB83EE27F5C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2964" yWindow="-17388" windowWidth="30936" windowHeight="16896" xr2:uid="{B845255D-815F-49EA-8438-49CAB31B3547}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="797" firstSheet="5" activeTab="6" xr2:uid="{B845255D-815F-49EA-8438-49CAB31B3547}"/>
   </bookViews>
   <sheets>
     <sheet name="discount_rate" sheetId="7" r:id="rId1"/>
@@ -279,7 +279,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="122">
   <si>
     <t>CAPEX solare</t>
   </si>
@@ -642,15 +642,19 @@
   </si>
   <si>
     <t>discount_rate</t>
+  </si>
+  <si>
+    <t>Paper di supporto</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0E+00"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -817,7 +821,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -888,9 +892,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -937,15 +938,9 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -955,9 +950,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -976,8 +968,14 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1317,15 +1315,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{923C661C-C997-4238-A47F-A35B6AA9581D}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.88671875" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35.77734375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1349,62 +1347,80 @@
         <v>72</v>
       </c>
       <c r="B2" s="8">
-        <v>7.0000000000000007E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="8"/>
+      <c r="D2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>79</v>
       </c>
       <c r="B3" s="8">
-        <v>7.0000000000000007E-2</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="8"/>
+      <c r="D3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>76</v>
       </c>
       <c r="B4" s="8">
-        <v>7.0000000000000007E-2</v>
+        <v>0.1</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="27"/>
+      <c r="D4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>74</v>
       </c>
       <c r="B5" s="8">
-        <v>7.0000000000000007E-2</v>
+        <v>0.08</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="8"/>
+      <c r="D5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>70</v>
       </c>
       <c r="B6" s="8">
-        <v>7.0000000000000007E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>81</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1412,10 +1428,16 @@
         <v>71</v>
       </c>
       <c r="B7" s="8">
-        <v>7.0000000000000007E-2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>81</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1423,10 +1445,16 @@
         <v>73</v>
       </c>
       <c r="B8" s="8">
-        <v>7.0000000000000007E-2</v>
+        <v>6.2E-2</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>81</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1434,151 +1462,30 @@
         <v>75</v>
       </c>
       <c r="B9" s="8">
-        <v>7.0000000000000007E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>81</v>
       </c>
+      <c r="D9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>121</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="World Bank" xr:uid="{325A9913-111A-4B4C-A5B3-6737C44DB97B}"/>
+    <hyperlink ref="D3:D9" r:id="rId2" display="World Bank" xr:uid="{F3F18F13-983F-41F1-9B38-27EAD29EB214}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{F506094E-FA0C-4C64-8DA9-24EF0CE90647}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9398001-B177-42A1-9F09-DD1B7293885B}">
-  <dimension ref="A1:E9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="32.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="8">
-        <v>0.04</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="8"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" s="8">
-        <v>0.04</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="8"/>
-    </row>
-    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="8">
-        <v>0.04</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="27"/>
-    </row>
-    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5" s="8">
-        <v>0.04</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="8"/>
-    </row>
-    <row r="6" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6" s="8">
-        <v>0.04</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="8">
-        <v>0.04</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>73</v>
-      </c>
-      <c r="B8" s="8">
-        <v>0.04</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>75</v>
-      </c>
-      <c r="B9" s="8">
-        <v>0.04</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C372154-4B0A-49B9-8FF3-F49D60098BF7}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1596,7 +1503,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -1612,16 +1519,17 @@
       <c r="A2" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="23">
-        <v>676570.29999999993</v>
+      <c r="B2" s="52">
+        <f>1.7275/100</f>
+        <v>1.7274999999999999E-2</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>7</v>
+        <v>81</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E2" s="50" t="s">
+      <c r="E2" s="46" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1629,16 +1537,17 @@
       <c r="A3" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="8">
-        <v>1208275.5560000001</v>
+      <c r="B3" s="52">
+        <f>1.2347/100</f>
+        <v>1.2346999999999999E-2</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>7</v>
+        <v>81</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E3" s="27">
+      <c r="E3" s="26">
         <v>2025</v>
       </c>
     </row>
@@ -1646,6 +1555,178 @@
       <c r="A4" s="8" t="s">
         <v>76</v>
       </c>
+      <c r="B4" s="52"/>
+      <c r="C4" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="26"/>
+    </row>
+    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="52"/>
+      <c r="C5" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="26"/>
+    </row>
+    <row r="6" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="52">
+        <f>1/100</f>
+        <v>0.01</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" s="47">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="52">
+        <f>3.313/100</f>
+        <v>3.313E-2</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="52">
+        <f>1.6316/100</f>
+        <v>1.6316000000000001E-2</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" s="26">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="52">
+        <f>0.43/100</f>
+        <v>4.3E-3</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" s="47">
+        <v>2025</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{45FFE6C8-BB08-4880-94D9-EDA810A88275}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{218A3F33-E049-447D-A203-05D8EF114C08}"/>
+    <hyperlink ref="D7" r:id="rId3" xr:uid="{303CBD72-DF1C-479C-A96E-85F23E49E626}"/>
+    <hyperlink ref="D8" r:id="rId4" xr:uid="{35012D9B-0404-4C14-AD2C-45339E554D22}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{F10656D8-D406-484F-9D16-6B079A7CA6A3}"/>
+    <hyperlink ref="D9" r:id="rId6" xr:uid="{A02F5EEA-4641-4413-B905-FCFAE765F982}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C372154-4B0A-49B9-8FF3-F49D60098BF7}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="23">
+        <v>676570.29999999993</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" s="46" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1208275.5560000001</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" s="26">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>76</v>
+      </c>
       <c r="B4" s="8">
         <v>3154360</v>
       </c>
@@ -1655,7 +1736,7 @@
       <c r="D4" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="26" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1673,7 +1754,7 @@
       <c r="D5" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="26" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1681,7 +1762,7 @@
       <c r="A6" t="s">
         <v>70</v>
       </c>
-      <c r="B6" s="49">
+      <c r="B6" s="8">
         <v>2593292.1779999998</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -1690,7 +1771,7 @@
       <c r="D6" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E6" s="51">
+      <c r="E6" s="47">
         <v>2025</v>
       </c>
     </row>
@@ -1698,7 +1779,7 @@
       <c r="A7" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="33">
+      <c r="B7" s="32">
         <v>644986.04399999999</v>
       </c>
       <c r="C7" s="8" t="s">
@@ -1707,7 +1788,7 @@
       <c r="D7" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="26" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1715,7 +1796,7 @@
       <c r="A8" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="33">
+      <c r="B8" s="32">
         <v>2109090.4800000004</v>
       </c>
       <c r="C8" s="8" t="s">
@@ -1724,7 +1805,7 @@
       <c r="D8" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="26">
         <v>2025</v>
       </c>
     </row>
@@ -1732,7 +1813,7 @@
       <c r="A9" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="56">
+      <c r="B9" s="18">
         <v>60498.506250000006</v>
       </c>
       <c r="C9" s="8" t="s">
@@ -1741,7 +1822,7 @@
       <c r="D9" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E9" s="51">
+      <c r="E9" s="47">
         <v>2025</v>
       </c>
     </row>
@@ -1836,7 +1917,7 @@
       <c r="C4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="31" t="s">
         <v>68</v>
       </c>
       <c r="E4" t="s">
@@ -1888,7 +1969,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="34" t="s">
         <v>91</v>
       </c>
       <c r="B2" s="8">
@@ -1908,88 +1989,88 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="34">
+      <c r="B3" s="33">
         <v>1</v>
       </c>
-      <c r="C3" s="34">
+      <c r="C3" s="33">
         <v>1</v>
       </c>
-      <c r="D3" s="34">
+      <c r="D3" s="33">
         <v>1</v>
       </c>
       <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="B4" s="34">
+      <c r="B4" s="33">
         <v>1</v>
       </c>
-      <c r="C4" s="34">
+      <c r="C4" s="33">
         <v>1</v>
       </c>
-      <c r="D4" s="34">
+      <c r="D4" s="33">
         <v>1</v>
       </c>
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="B5" s="34">
+      <c r="B5" s="33">
         <v>1</v>
       </c>
-      <c r="C5" s="34">
+      <c r="C5" s="33">
         <v>1</v>
       </c>
-      <c r="D5" s="34">
+      <c r="D5" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="B6" s="34">
+      <c r="B6" s="33">
         <v>1</v>
       </c>
-      <c r="C6" s="34">
+      <c r="C6" s="33">
         <v>1</v>
       </c>
-      <c r="D6" s="34">
+      <c r="D6" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="34">
+      <c r="B7" s="33">
         <v>1</v>
       </c>
-      <c r="C7" s="34">
+      <c r="C7" s="33">
         <v>1</v>
       </c>
-      <c r="D7" s="34">
+      <c r="D7" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="34">
+      <c r="B8" s="33">
         <v>1</v>
       </c>
-      <c r="C8" s="34">
+      <c r="C8" s="33">
         <v>1</v>
       </c>
-      <c r="D8" s="34">
+      <c r="D8" s="33">
         <v>1</v>
       </c>
     </row>
@@ -2545,7 +2626,7 @@
       <c r="A17" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="30" t="s">
         <v>65</v>
       </c>
       <c r="C17" s="21">
@@ -2605,7 +2686,7 @@
       <c r="E21" s="24"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="E22" s="30"/>
+      <c r="E22" s="29"/>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="Q27" s="17"/>
@@ -2638,8 +2719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F958822-C8DD-4CF0-BC79-5189EFFDF89D}">
   <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2770,35 +2851,35 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="C4" s="38">
+      <c r="C4" s="37">
         <v>2025</v>
       </c>
-      <c r="D4" s="37">
+      <c r="D4" s="36">
         <v>676.57029999999997</v>
       </c>
-      <c r="E4" s="39" t="s">
+      <c r="E4" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="40" t="s">
+      <c r="F4" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="G4" s="41" t="s">
+      <c r="G4" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="H4" s="41" t="s">
+      <c r="H4" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="I4" s="36">
+      <c r="I4" s="35">
         <f>D4*10^3</f>
         <v>676570.29999999993</v>
       </c>
-      <c r="J4" s="38" t="s">
+      <c r="J4" s="37" t="s">
         <v>37</v>
       </c>
       <c r="P4" s="15" t="s">
@@ -2830,7 +2911,7 @@
       <c r="F5" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="G5" s="41" t="s">
+      <c r="G5" s="40" t="s">
         <v>118</v>
       </c>
       <c r="H5" s="24"/>
@@ -2914,33 +2995,33 @@
       </c>
     </row>
     <row r="8" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="38">
+      <c r="C8" s="37">
         <v>2025</v>
       </c>
-      <c r="D8" s="36">
+      <c r="D8" s="35">
         <v>1139.8825999999999</v>
       </c>
-      <c r="E8" s="39" t="s">
+      <c r="E8" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="F8" s="40" t="s">
+      <c r="F8" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="G8" s="41" t="s">
+      <c r="G8" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="H8" s="42"/>
-      <c r="I8" s="43">
+      <c r="H8" s="41"/>
+      <c r="I8" s="35">
         <f>D8*$Q$4*10^3</f>
         <v>1208275.5560000001</v>
       </c>
-      <c r="J8" s="38" t="s">
+      <c r="J8" s="37" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2966,8 +3047,8 @@
       <c r="G9" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="44"/>
-      <c r="I9" s="45">
+      <c r="H9" s="42"/>
+      <c r="I9" s="23">
         <f t="shared" si="0"/>
         <v>3290320</v>
       </c>
@@ -2997,8 +3078,8 @@
       <c r="G10" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="44"/>
-      <c r="I10" s="45">
+      <c r="H10" s="42"/>
+      <c r="I10" s="23">
         <f t="shared" si="0"/>
         <v>2427040</v>
       </c>
@@ -3007,29 +3088,29 @@
       </c>
     </row>
     <row r="11" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="33">
+      <c r="C11" s="32">
         <v>2025</v>
       </c>
-      <c r="D11" s="52">
+      <c r="D11" s="48">
         <v>1769.1170999999999</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="53" t="s">
+      <c r="F11" s="49" t="s">
         <v>105</v>
       </c>
-      <c r="G11" s="54" t="s">
+      <c r="G11" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="H11" s="55"/>
-      <c r="I11" s="45">
+      <c r="H11" s="51"/>
+      <c r="I11" s="23">
         <f>D11*10^3</f>
         <v>1769117.0999999999</v>
       </c>
@@ -3232,60 +3313,60 @@
       </c>
     </row>
     <row r="18" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="38" t="s">
+      <c r="A18" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="B18" s="38"/>
-      <c r="C18" s="38">
+      <c r="B18" s="37"/>
+      <c r="C18" s="37">
         <v>2025</v>
       </c>
-      <c r="D18" s="36">
+      <c r="D18" s="35">
         <v>2274.8177000000001</v>
       </c>
-      <c r="E18" s="39" t="s">
+      <c r="E18" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="F18" s="40" t="s">
+      <c r="F18" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="G18" s="41" t="s">
+      <c r="G18" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="H18" s="48"/>
-      <c r="I18" s="36">
+      <c r="H18" s="45"/>
+      <c r="I18" s="35">
         <f>D18*$Q$5*10^3</f>
         <v>2593292.1779999998</v>
       </c>
-      <c r="J18" s="38" t="s">
+      <c r="J18" s="37" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="38" t="s">
+      <c r="A19" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="B19" s="38"/>
-      <c r="C19" s="38">
+      <c r="B19" s="37"/>
+      <c r="C19" s="37">
         <v>2025</v>
       </c>
-      <c r="D19" s="36">
+      <c r="D19" s="35">
         <v>57074.0625</v>
       </c>
-      <c r="E19" s="39" t="s">
+      <c r="E19" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="F19" s="40" t="s">
+      <c r="F19" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="G19" s="41" t="s">
+      <c r="G19" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="H19" s="48"/>
-      <c r="I19" s="36">
+      <c r="H19" s="45"/>
+      <c r="I19" s="35">
         <f>D19*$Q$4</f>
         <v>60498.506250000006</v>
       </c>
-      <c r="J19" s="38" t="s">
+      <c r="J19" s="37" t="s">
         <v>26</v>
       </c>
     </row>
@@ -3352,31 +3433,31 @@
       </c>
     </row>
     <row r="22" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="38" t="s">
+      <c r="A22" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="B22" s="38"/>
-      <c r="C22" s="38">
+      <c r="B22" s="37"/>
+      <c r="C22" s="37">
         <v>2025</v>
       </c>
-      <c r="D22" s="36">
+      <c r="D22" s="35">
         <v>1989.7080000000001</v>
       </c>
-      <c r="E22" s="39" t="s">
+      <c r="E22" s="38" t="s">
         <v>111</v>
       </c>
-      <c r="F22" s="40" t="s">
+      <c r="F22" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="G22" s="41" t="s">
+      <c r="G22" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="H22" s="48"/>
-      <c r="I22" s="36">
+      <c r="H22" s="45"/>
+      <c r="I22" s="35">
         <f>D22*$Q$4*10^3</f>
         <v>2109090.4800000004</v>
       </c>
-      <c r="J22" s="38" t="s">
+      <c r="J22" s="37" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3443,66 +3524,66 @@
       </c>
     </row>
     <row r="25" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="38" t="s">
+      <c r="A25" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="B25" s="38" t="s">
+      <c r="B25" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="C25" s="38">
+      <c r="C25" s="37">
         <v>2025</v>
       </c>
-      <c r="D25" s="36">
+      <c r="D25" s="35">
         <v>608.47739999999999</v>
       </c>
-      <c r="E25" s="39" t="s">
+      <c r="E25" s="38" t="s">
         <v>111</v>
       </c>
-      <c r="F25" s="40" t="s">
+      <c r="F25" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="G25" s="41" t="s">
+      <c r="G25" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="H25" s="48"/>
-      <c r="I25" s="36">
+      <c r="H25" s="45"/>
+      <c r="I25" s="35">
         <f>D25*$Q$4*10^3</f>
         <v>644986.04399999999</v>
       </c>
-      <c r="J25" s="38" t="s">
+      <c r="J25" s="37" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26" s="37">
         <v>2025</v>
       </c>
-      <c r="D26" s="23">
+      <c r="D26" s="35">
         <v>5350</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="F26" s="26" t="s">
+      <c r="F26" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="G26" s="25" t="s">
+      <c r="G26" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="H26" s="24" t="s">
+      <c r="H26" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="I26" s="23">
+      <c r="I26" s="35">
         <f>D26*$Q$3*10^3*0.67</f>
         <v>3154360</v>
       </c>
-      <c r="J26" s="8" t="s">
+      <c r="J26" s="37" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3516,7 +3597,7 @@
       <c r="C27" s="8">
         <v>2020</v>
       </c>
-      <c r="D27" s="28">
+      <c r="D27" s="27">
         <v>988.32170015695567</v>
       </c>
       <c r="E27" s="1" t="s">
@@ -3552,7 +3633,7 @@
       <c r="C28" s="8">
         <v>2030</v>
       </c>
-      <c r="D28" s="28">
+      <c r="D28" s="27">
         <v>681.62247956991291</v>
       </c>
       <c r="E28" s="1" t="s">
@@ -3588,7 +3669,7 @@
       <c r="C29" s="8">
         <v>2050</v>
       </c>
-      <c r="D29" s="29">
+      <c r="D29" s="28">
         <v>681.62247956991291</v>
       </c>
       <c r="E29" s="1" t="s">
@@ -3624,7 +3705,7 @@
       <c r="C30" s="8">
         <v>2020</v>
       </c>
-      <c r="D30" s="28">
+      <c r="D30" s="27">
         <v>1727.2344448095646</v>
       </c>
       <c r="E30" s="1" t="s">
@@ -3659,7 +3740,7 @@
       <c r="C31" s="8">
         <v>2030</v>
       </c>
-      <c r="D31" s="28">
+      <c r="D31" s="27">
         <v>1173.7257628388072</v>
       </c>
       <c r="E31" s="1" t="s">
@@ -3694,7 +3775,7 @@
       <c r="C32" s="8">
         <v>2050</v>
       </c>
-      <c r="D32" s="29">
+      <c r="D32" s="28">
         <v>1173.7257628388072</v>
       </c>
       <c r="E32" s="1" t="s">
@@ -3718,70 +3799,70 @@
       </c>
     </row>
     <row r="33" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="38" t="s">
+      <c r="A33" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B33" s="38" t="s">
+      <c r="B33" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="C33" s="38">
+      <c r="C33" s="37">
         <v>2025</v>
       </c>
-      <c r="D33" s="46">
+      <c r="D33" s="43">
         <f>197.8874*2</f>
         <v>395.77480000000003</v>
       </c>
-      <c r="E33" s="39" t="s">
+      <c r="E33" s="38" t="s">
         <v>111</v>
       </c>
-      <c r="F33" s="40" t="s">
+      <c r="F33" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="G33" s="41" t="s">
+      <c r="G33" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="H33" s="47" t="s">
+      <c r="H33" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="I33" s="36">
+      <c r="I33" s="35">
         <f>D33*$Q$4*10^3</f>
         <v>419521.288</v>
       </c>
-      <c r="J33" s="38" t="s">
+      <c r="J33" s="37" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="38" t="s">
+      <c r="A34" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="38" t="s">
+      <c r="B34" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="C34" s="38">
+      <c r="C34" s="37">
         <v>2025</v>
       </c>
-      <c r="D34" s="36">
+      <c r="D34" s="35">
         <f>280.1877*2</f>
         <v>560.37540000000001</v>
       </c>
-      <c r="E34" s="39" t="s">
+      <c r="E34" s="38" t="s">
         <v>111</v>
       </c>
-      <c r="F34" s="40" t="s">
+      <c r="F34" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="G34" s="41" t="s">
+      <c r="G34" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="H34" s="47" t="s">
+      <c r="H34" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="I34" s="36">
+      <c r="I34" s="35">
         <f>D34*$Q$4*10^3</f>
         <v>593997.924</v>
       </c>
-      <c r="J34" s="38" t="s">
+      <c r="J34" s="37" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modified CAPEX nuclear to reflect the value suggested by Lorenzo M.
</commit_message>
<xml_diff>
--- a/dati_casoStudioItalia/altri_dati.xlsx
+++ b/dati_casoStudioItalia/altri_dati.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gianvito.colucci\OneDrive - Politecnico di Torino\Jobs\DRIN DRIN\Energy mix\DrinDrin---Mix-energetico\dati_casoStudioItalia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0954659\PycharmProjects\DrinDrin---Mix-energetico\dati_casoStudioItalia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8C6BD1-24ED-46C2-A2CB-EB83EE27F5C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A08D224-1818-4F22-8512-699BE7D050EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="797" firstSheet="5" activeTab="6" xr2:uid="{B845255D-815F-49EA-8438-49CAB31B3547}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="797" activeTab="3" xr2:uid="{B845255D-815F-49EA-8438-49CAB31B3547}"/>
   </bookViews>
   <sheets>
     <sheet name="discount_rate" sheetId="7" r:id="rId1"/>
@@ -47,6 +47,30 @@
     <author>Bertoni, L. (Luca)</author>
   </authors>
   <commentList>
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{BA01F196-2495-4430-832C-D7D0131A597F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Bertoni, L. (Luca):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Valore proposto da Lorenzo, non dato IAEA</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A7" authorId="0" shapeId="0" xr:uid="{6042687D-A9B5-4779-9A54-E22AF9FBB252}">
       <text>
         <r>
@@ -279,7 +303,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="124">
   <si>
     <t>CAPEX solare</t>
   </si>
@@ -645,6 +669,12 @@
   </si>
   <si>
     <t>Paper di supporto</t>
+  </si>
+  <si>
+    <t>assumed same as coal</t>
+  </si>
+  <si>
+    <t>assumed same as PV</t>
   </si>
 </sst>
 </file>
@@ -654,7 +684,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0E+00"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -821,7 +851,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -968,7 +998,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -976,6 +1006,12 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1316,13 +1352,13 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C9"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35.77734375" bestFit="1" customWidth="1"/>
@@ -1489,14 +1525,14 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.88671875" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35.77734375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1555,23 +1591,31 @@
       <c r="A4" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="52"/>
+      <c r="B4" s="55">
+        <v>3.3000000000000002E-2</v>
+      </c>
       <c r="C4" s="8" t="s">
         <v>81</v>
       </c>
       <c r="D4" s="6"/>
-      <c r="E4" s="26"/>
+      <c r="E4" s="26" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="52"/>
+      <c r="B5" s="55">
+        <v>1.7000000000000001E-2</v>
+      </c>
       <c r="C5" s="8" t="s">
         <v>81</v>
       </c>
       <c r="D5" s="6"/>
-      <c r="E5" s="26"/>
+      <c r="E5" s="26" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -1663,7 +1707,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1727,8 +1771,8 @@
       <c r="A4" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="8">
-        <v>3154360</v>
+      <c r="B4" s="56">
+        <v>7500000</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>7</v>
@@ -1828,14 +1872,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" xr:uid="{76843948-9A3E-4EB0-A540-24DF6B66F999}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{D3DAE58A-78C9-42A3-AACE-003B92F3B755}"/>
-    <hyperlink ref="D3" r:id="rId3" xr:uid="{4F66A19D-E563-4CE0-A0F8-405FBE5A76EE}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{27416DF2-25A2-40A4-ADBE-E01677AB7CAF}"/>
-    <hyperlink ref="D7" r:id="rId5" xr:uid="{0EC7236B-99A1-46EF-8EA3-6832779019E9}"/>
-    <hyperlink ref="D8" r:id="rId6" xr:uid="{34FFE429-8ADC-4F03-A78F-036552A631F1}"/>
-    <hyperlink ref="D6" r:id="rId7" xr:uid="{E8D8F775-B077-49C3-91F8-A7497013BEB0}"/>
-    <hyperlink ref="D9" r:id="rId8" xr:uid="{4A9E0CE3-D16C-464A-84CE-CA642CBCF8D2}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{D3DAE58A-78C9-42A3-AACE-003B92F3B755}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{4F66A19D-E563-4CE0-A0F8-405FBE5A76EE}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{27416DF2-25A2-40A4-ADBE-E01677AB7CAF}"/>
+    <hyperlink ref="D7" r:id="rId4" xr:uid="{0EC7236B-99A1-46EF-8EA3-6832779019E9}"/>
+    <hyperlink ref="D8" r:id="rId5" xr:uid="{34FFE429-8ADC-4F03-A78F-036552A631F1}"/>
+    <hyperlink ref="D6" r:id="rId6" xr:uid="{E8D8F775-B077-49C3-91F8-A7497013BEB0}"/>
+    <hyperlink ref="D9" r:id="rId7" xr:uid="{4A9E0CE3-D16C-464A-84CE-CA642CBCF8D2}"/>
+    <hyperlink ref="D4" r:id="rId8" xr:uid="{76843948-9A3E-4EB0-A540-24DF6B66F999}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId9"/>
@@ -1846,7 +1890,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F36F9B7-E410-4418-9AFE-4DC5A9893242}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -2719,7 +2763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F958822-C8DD-4CF0-BC79-5189EFFDF89D}">
   <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated cost of transmission based on the Excel file line_cost_coefficients
</commit_message>
<xml_diff>
--- a/dati_casoStudioItalia/altri_dati.xlsx
+++ b/dati_casoStudioItalia/altri_dati.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0954659\PycharmProjects\DrinDrin---Mix-energetico\dati_casoStudioItalia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A08D224-1818-4F22-8512-699BE7D050EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75FD7C1A-CCF7-4F7A-80F7-DF589CAE0D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="797" activeTab="3" xr2:uid="{B845255D-815F-49EA-8438-49CAB31B3547}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="797" activeTab="4" xr2:uid="{B845255D-815F-49EA-8438-49CAB31B3547}"/>
   </bookViews>
   <sheets>
     <sheet name="discount_rate" sheetId="7" r:id="rId1"/>
@@ -303,7 +303,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="125">
   <si>
     <t>CAPEX solare</t>
   </si>
@@ -675,6 +675,9 @@
   </si>
   <si>
     <t>assumed same as PV</t>
+  </si>
+  <si>
+    <t>grecia</t>
   </si>
 </sst>
 </file>
@@ -851,7 +854,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -941,9 +944,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1013,6 +1013,10 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1555,7 +1559,7 @@
       <c r="A2" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="52">
+      <c r="B2" s="51">
         <f>1.7275/100</f>
         <v>1.7274999999999999E-2</v>
       </c>
@@ -1565,7 +1569,7 @@
       <c r="D2" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E2" s="46" t="s">
+      <c r="E2" s="45" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1573,7 +1577,7 @@
       <c r="A3" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="52">
+      <c r="B3" s="51">
         <f>1.2347/100</f>
         <v>1.2346999999999999E-2</v>
       </c>
@@ -1591,7 +1595,7 @@
       <c r="A4" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="55">
+      <c r="B4" s="54">
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="C4" s="8" t="s">
@@ -1606,7 +1610,7 @@
       <c r="A5" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="55">
+      <c r="B5" s="54">
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -1621,7 +1625,7 @@
       <c r="A6" t="s">
         <v>70</v>
       </c>
-      <c r="B6" s="52">
+      <c r="B6" s="51">
         <f>1/100</f>
         <v>0.01</v>
       </c>
@@ -1631,7 +1635,7 @@
       <c r="D6" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E6" s="47">
+      <c r="E6" s="46">
         <v>2025</v>
       </c>
     </row>
@@ -1639,7 +1643,7 @@
       <c r="A7" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="52">
+      <c r="B7" s="51">
         <f>3.313/100</f>
         <v>3.313E-2</v>
       </c>
@@ -1657,7 +1661,7 @@
       <c r="A8" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="52">
+      <c r="B8" s="51">
         <f>1.6316/100</f>
         <v>1.6316000000000001E-2</v>
       </c>
@@ -1675,7 +1679,7 @@
       <c r="A9" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="52">
+      <c r="B9" s="51">
         <f>0.43/100</f>
         <v>4.3E-3</v>
       </c>
@@ -1685,7 +1689,7 @@
       <c r="D9" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E9" s="47">
+      <c r="E9" s="46">
         <v>2025</v>
       </c>
     </row>
@@ -1746,7 +1750,7 @@
       <c r="D2" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E2" s="46" t="s">
+      <c r="E2" s="45" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1771,7 +1775,7 @@
       <c r="A4" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="56">
+      <c r="B4" s="55">
         <v>7500000</v>
       </c>
       <c r="C4" s="8" t="s">
@@ -1815,7 +1819,7 @@
       <c r="D6" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E6" s="47">
+      <c r="E6" s="46">
         <v>2025</v>
       </c>
     </row>
@@ -1866,7 +1870,7 @@
       <c r="D9" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E9" s="47">
+      <c r="E9" s="46">
         <v>2025</v>
       </c>
     </row>
@@ -1890,7 +1894,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F36F9B7-E410-4418-9AFE-4DC5A9893242}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1980,10 +1984,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25E773EF-BD6E-41C4-818D-318BE958C680}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2013,7 +2017,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="33" t="s">
         <v>91</v>
       </c>
       <c r="B2" s="8">
@@ -2023,7 +2027,7 @@
         <v>100</v>
       </c>
       <c r="D2">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>77</v>
@@ -2033,90 +2037,101 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="33">
-        <v>1</v>
-      </c>
-      <c r="C3" s="33">
-        <v>1</v>
-      </c>
-      <c r="D3" s="33">
-        <v>1</v>
+      <c r="B3" s="56">
+        <v>0</v>
+      </c>
+      <c r="C3" s="56">
+        <v>0</v>
+      </c>
+      <c r="D3" s="56">
+        <v>0</v>
       </c>
       <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="B4" s="33">
-        <v>1</v>
-      </c>
-      <c r="C4" s="33">
-        <v>1</v>
-      </c>
-      <c r="D4" s="33">
-        <v>1</v>
+      <c r="B4" s="56">
+        <v>0</v>
+      </c>
+      <c r="C4" s="56">
+        <v>0</v>
+      </c>
+      <c r="D4" s="56">
+        <v>0</v>
       </c>
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="B5" s="33">
-        <v>1</v>
-      </c>
-      <c r="C5" s="33">
-        <v>1</v>
-      </c>
-      <c r="D5" s="33">
-        <v>1</v>
+      <c r="B5" s="56">
+        <v>0</v>
+      </c>
+      <c r="C5" s="56">
+        <v>0</v>
+      </c>
+      <c r="D5" s="56">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="B6" s="33">
-        <v>1</v>
-      </c>
-      <c r="C6" s="33">
-        <v>1</v>
-      </c>
-      <c r="D6" s="33">
-        <v>1</v>
+      <c r="B6" s="56">
+        <v>500</v>
+      </c>
+      <c r="C6" s="56">
+        <v>100</v>
+      </c>
+      <c r="D6" s="56">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="33">
-        <v>1</v>
-      </c>
-      <c r="C7" s="33">
-        <v>1</v>
-      </c>
-      <c r="D7" s="33">
-        <v>1</v>
+      <c r="B7" s="56">
+        <v>0</v>
+      </c>
+      <c r="C7" s="56">
+        <v>0</v>
+      </c>
+      <c r="D7" s="56">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="33">
-        <v>1</v>
-      </c>
-      <c r="C8" s="33">
-        <v>1</v>
-      </c>
-      <c r="D8" s="33">
-        <v>1</v>
-      </c>
+      <c r="B8" s="56">
+        <v>0</v>
+      </c>
+      <c r="C8" s="56">
+        <v>0</v>
+      </c>
+      <c r="D8" s="56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="57"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2895,35 +2910,35 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="C4" s="37">
+      <c r="C4" s="36">
         <v>2025</v>
       </c>
-      <c r="D4" s="36">
+      <c r="D4" s="35">
         <v>676.57029999999997</v>
       </c>
-      <c r="E4" s="38" t="s">
+      <c r="E4" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="39" t="s">
+      <c r="F4" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="G4" s="40" t="s">
+      <c r="G4" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="H4" s="40" t="s">
+      <c r="H4" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="I4" s="35">
+      <c r="I4" s="34">
         <f>D4*10^3</f>
         <v>676570.29999999993</v>
       </c>
-      <c r="J4" s="37" t="s">
+      <c r="J4" s="36" t="s">
         <v>37</v>
       </c>
       <c r="P4" s="15" t="s">
@@ -2955,7 +2970,7 @@
       <c r="F5" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="G5" s="40" t="s">
+      <c r="G5" s="39" t="s">
         <v>118</v>
       </c>
       <c r="H5" s="24"/>
@@ -3039,33 +3054,33 @@
       </c>
     </row>
     <row r="8" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="37">
+      <c r="C8" s="36">
         <v>2025</v>
       </c>
-      <c r="D8" s="35">
+      <c r="D8" s="34">
         <v>1139.8825999999999</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="E8" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="F8" s="39" t="s">
+      <c r="F8" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="G8" s="40" t="s">
+      <c r="G8" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="H8" s="41"/>
-      <c r="I8" s="35">
+      <c r="H8" s="40"/>
+      <c r="I8" s="34">
         <f>D8*$Q$4*10^3</f>
         <v>1208275.5560000001</v>
       </c>
-      <c r="J8" s="37" t="s">
+      <c r="J8" s="36" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3091,7 +3106,7 @@
       <c r="G9" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="42"/>
+      <c r="H9" s="41"/>
       <c r="I9" s="23">
         <f t="shared" si="0"/>
         <v>3290320</v>
@@ -3122,7 +3137,7 @@
       <c r="G10" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="42"/>
+      <c r="H10" s="41"/>
       <c r="I10" s="23">
         <f t="shared" si="0"/>
         <v>2427040</v>
@@ -3141,19 +3156,19 @@
       <c r="C11" s="32">
         <v>2025</v>
       </c>
-      <c r="D11" s="48">
+      <c r="D11" s="47">
         <v>1769.1170999999999</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="49" t="s">
+      <c r="F11" s="48" t="s">
         <v>105</v>
       </c>
-      <c r="G11" s="50" t="s">
+      <c r="G11" s="49" t="s">
         <v>118</v>
       </c>
-      <c r="H11" s="51"/>
+      <c r="H11" s="50"/>
       <c r="I11" s="23">
         <f>D11*10^3</f>
         <v>1769117.0999999999</v>
@@ -3357,60 +3372,60 @@
       </c>
     </row>
     <row r="18" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37">
+      <c r="B18" s="36"/>
+      <c r="C18" s="36">
         <v>2025</v>
       </c>
-      <c r="D18" s="35">
+      <c r="D18" s="34">
         <v>2274.8177000000001</v>
       </c>
-      <c r="E18" s="38" t="s">
+      <c r="E18" s="37" t="s">
         <v>113</v>
       </c>
-      <c r="F18" s="39" t="s">
+      <c r="F18" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="G18" s="40" t="s">
+      <c r="G18" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="H18" s="45"/>
-      <c r="I18" s="35">
+      <c r="H18" s="44"/>
+      <c r="I18" s="34">
         <f>D18*$Q$5*10^3</f>
         <v>2593292.1779999998</v>
       </c>
-      <c r="J18" s="37" t="s">
+      <c r="J18" s="36" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37">
+      <c r="B19" s="36"/>
+      <c r="C19" s="36">
         <v>2025</v>
       </c>
-      <c r="D19" s="35">
+      <c r="D19" s="34">
         <v>57074.0625</v>
       </c>
-      <c r="E19" s="38" t="s">
+      <c r="E19" s="37" t="s">
         <v>119</v>
       </c>
-      <c r="F19" s="39" t="s">
+      <c r="F19" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="G19" s="40" t="s">
+      <c r="G19" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="H19" s="45"/>
-      <c r="I19" s="35">
+      <c r="H19" s="44"/>
+      <c r="I19" s="34">
         <f>D19*$Q$4</f>
         <v>60498.506250000006</v>
       </c>
-      <c r="J19" s="37" t="s">
+      <c r="J19" s="36" t="s">
         <v>26</v>
       </c>
     </row>
@@ -3477,31 +3492,31 @@
       </c>
     </row>
     <row r="22" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="37" t="s">
+      <c r="A22" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="B22" s="37"/>
-      <c r="C22" s="37">
+      <c r="B22" s="36"/>
+      <c r="C22" s="36">
         <v>2025</v>
       </c>
-      <c r="D22" s="35">
+      <c r="D22" s="34">
         <v>1989.7080000000001</v>
       </c>
-      <c r="E22" s="38" t="s">
+      <c r="E22" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="F22" s="39" t="s">
+      <c r="F22" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="G22" s="40" t="s">
+      <c r="G22" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="H22" s="45"/>
-      <c r="I22" s="35">
+      <c r="H22" s="44"/>
+      <c r="I22" s="34">
         <f>D22*$Q$4*10^3</f>
         <v>2109090.4800000004</v>
       </c>
-      <c r="J22" s="37" t="s">
+      <c r="J22" s="36" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3568,66 +3583,66 @@
       </c>
     </row>
     <row r="25" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="37" t="s">
+      <c r="A25" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="B25" s="37" t="s">
+      <c r="B25" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="C25" s="37">
+      <c r="C25" s="36">
         <v>2025</v>
       </c>
-      <c r="D25" s="35">
+      <c r="D25" s="34">
         <v>608.47739999999999</v>
       </c>
-      <c r="E25" s="38" t="s">
+      <c r="E25" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="F25" s="39" t="s">
+      <c r="F25" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="G25" s="40" t="s">
+      <c r="G25" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="H25" s="45"/>
-      <c r="I25" s="35">
+      <c r="H25" s="44"/>
+      <c r="I25" s="34">
         <f>D25*$Q$4*10^3</f>
         <v>644986.04399999999</v>
       </c>
-      <c r="J25" s="37" t="s">
+      <c r="J25" s="36" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="37" t="s">
+      <c r="A26" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="37" t="s">
+      <c r="B26" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="37">
+      <c r="C26" s="36">
         <v>2025</v>
       </c>
-      <c r="D26" s="35">
+      <c r="D26" s="34">
         <v>5350</v>
       </c>
-      <c r="E26" s="38" t="s">
+      <c r="E26" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="F26" s="53" t="s">
+      <c r="F26" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="G26" s="45" t="s">
+      <c r="G26" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="H26" s="54" t="s">
+      <c r="H26" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="I26" s="35">
+      <c r="I26" s="34">
         <f>D26*$Q$3*10^3*0.67</f>
         <v>3154360</v>
       </c>
-      <c r="J26" s="37" t="s">
+      <c r="J26" s="36" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3843,70 +3858,70 @@
       </c>
     </row>
     <row r="33" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="B33" s="37" t="s">
+      <c r="B33" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="C33" s="37">
+      <c r="C33" s="36">
         <v>2025</v>
       </c>
-      <c r="D33" s="43">
+      <c r="D33" s="42">
         <f>197.8874*2</f>
         <v>395.77480000000003</v>
       </c>
-      <c r="E33" s="38" t="s">
+      <c r="E33" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="F33" s="39" t="s">
+      <c r="F33" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="G33" s="40" t="s">
+      <c r="G33" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="H33" s="44" t="s">
+      <c r="H33" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="I33" s="35">
+      <c r="I33" s="34">
         <f>D33*$Q$4*10^3</f>
         <v>419521.288</v>
       </c>
-      <c r="J33" s="37" t="s">
+      <c r="J33" s="36" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="37" t="s">
+      <c r="A34" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="37" t="s">
+      <c r="B34" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="C34" s="37">
+      <c r="C34" s="36">
         <v>2025</v>
       </c>
-      <c r="D34" s="35">
+      <c r="D34" s="34">
         <f>280.1877*2</f>
         <v>560.37540000000001</v>
       </c>
-      <c r="E34" s="38" t="s">
+      <c r="E34" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="F34" s="39" t="s">
+      <c r="F34" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="G34" s="40" t="s">
+      <c r="G34" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="H34" s="44" t="s">
+      <c r="H34" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="I34" s="35">
+      <c r="I34" s="34">
         <f>D34*$Q$4*10^3</f>
         <v>593997.924</v>
       </c>
-      <c r="J34" s="37" t="s">
+      <c r="J34" s="36" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated capex Wind to have it in Eur/(1.5MW_turbine)
</commit_message>
<xml_diff>
--- a/dati_casoStudioItalia/altri_dati.xlsx
+++ b/dati_casoStudioItalia/altri_dati.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0954659\PycharmProjects\DrinDrin---Mix-energetico\dati_casoStudioItalia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75FD7C1A-CCF7-4F7A-80F7-DF589CAE0D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70001030-42D7-4A96-99E4-4355B5DA2311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="797" activeTab="4" xr2:uid="{B845255D-815F-49EA-8438-49CAB31B3547}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="797" activeTab="2" xr2:uid="{B845255D-815F-49EA-8438-49CAB31B3547}"/>
   </bookViews>
   <sheets>
     <sheet name="discount_rate" sheetId="7" r:id="rId1"/>
@@ -303,7 +303,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="127">
   <si>
     <t>CAPEX solare</t>
   </si>
@@ -678,6 +678,12 @@
   </si>
   <si>
     <t>grecia</t>
+  </si>
+  <si>
+    <t>WindTurbine_Onshore_1500</t>
+  </si>
+  <si>
+    <t>EUR/(1.5MW_turbine)</t>
   </si>
 </sst>
 </file>
@@ -779,6 +785,7 @@
       <b/>
       <sz val="11"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -854,7 +861,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1017,6 +1024,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1710,15 +1720,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C372154-4B0A-49B9-8FF3-F49D60098BF7}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.88671875" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35.77734375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1756,13 +1766,14 @@
     </row>
     <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" s="8">
-        <v>1208275.5560000001</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>7</v>
+        <v>125</v>
+      </c>
+      <c r="B3" s="58">
+        <f>1208275.556*1.5</f>
+        <v>1812413.3340000003</v>
+      </c>
+      <c r="C3" s="58" t="s">
+        <v>126</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>105</v>
@@ -1986,7 +1997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25E773EF-BD6E-41C4-818D-318BE958C680}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Results optimization with interest rate nuclear at 4.5%
</commit_message>
<xml_diff>
--- a/dati_casoStudioItalia/altri_dati.xlsx
+++ b/dati_casoStudioItalia/altri_dati.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0954659\PycharmProjects\DrinDrin---Mix-energetico\dati_casoStudioItalia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70001030-42D7-4A96-99E4-4355B5DA2311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECACA251-0A23-44A9-8D37-BBEE7E4C81C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="797" activeTab="2" xr2:uid="{B845255D-815F-49EA-8438-49CAB31B3547}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="797" xr2:uid="{B845255D-815F-49EA-8438-49CAB31B3547}"/>
   </bookViews>
   <sheets>
     <sheet name="discount_rate" sheetId="7" r:id="rId1"/>
@@ -36,6 +36,9 @@
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -303,7 +306,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="126">
   <si>
     <t>CAPEX solare</t>
   </si>
@@ -540,9 +543,6 @@
   </si>
   <si>
     <t>Include francia, svizzera, slovenia, austria</t>
-  </si>
-  <si>
-    <t>WindTurbine_Onshore_4000</t>
   </si>
   <si>
     <t>OPEX</t>
@@ -1365,22 +1365,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{923C661C-C997-4238-A47F-A35B6AA9581D}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -1392,7 +1392,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -1400,48 +1400,48 @@
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>29</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>124</v>
       </c>
       <c r="B3" s="8">
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>29</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>76</v>
       </c>
       <c r="B4" s="8">
-        <v>0.1</v>
+        <v>0.45</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>29</v>
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>74</v>
       </c>
@@ -1449,14 +1449,14 @@
         <v>0.08</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>29</v>
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>70</v>
       </c>
@@ -1464,16 +1464,16 @@
         <v>5.1999999999999998E-2</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>29</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -1481,16 +1481,16 @@
         <v>2.7E-2</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>29</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>73</v>
       </c>
@@ -1498,16 +1498,16 @@
         <v>6.2E-2</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>29</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>75</v>
       </c>
@@ -1515,13 +1515,13 @@
         <v>5.1999999999999998E-2</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>29</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1539,21 +1539,21 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -1565,7 +1565,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -1574,34 +1574,34 @@
         <v>1.7274999999999999E-2</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E2" s="45" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>124</v>
       </c>
       <c r="B3" s="51">
         <f>1.2347/100</f>
         <v>1.2346999999999999E-2</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E3" s="26">
         <v>2025</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>76</v>
       </c>
@@ -1609,14 +1609,14 @@
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="26" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>74</v>
       </c>
@@ -1624,14 +1624,14 @@
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="26" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>70</v>
       </c>
@@ -1640,16 +1640,16 @@
         <v>0.01</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E6" s="46">
         <v>2025</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -1658,16 +1658,16 @@
         <v>3.313E-2</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>73</v>
       </c>
@@ -1676,16 +1676,16 @@
         <v>1.6316000000000001E-2</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E8" s="26">
         <v>2025</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>75</v>
       </c>
@@ -1694,10 +1694,10 @@
         <v>4.3E-3</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E9" s="46">
         <v>2025</v>
@@ -1720,20 +1720,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C372154-4B0A-49B9-8FF3-F49D60098BF7}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>69</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -1758,31 +1758,31 @@
         <v>7</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E2" s="45" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B3" s="58">
         <f>1208275.556*1.5</f>
         <v>1812413.3340000003</v>
       </c>
       <c r="C3" s="58" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E3" s="26">
         <v>2025</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>76</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>74</v>
       </c>
@@ -1811,13 +1811,13 @@
         <v>9</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>70</v>
       </c>
@@ -1828,13 +1828,13 @@
         <v>7</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E6" s="46">
         <v>2025</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -1845,13 +1845,13 @@
         <v>7</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>73</v>
       </c>
@@ -1862,13 +1862,13 @@
         <v>7</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E8" s="26">
         <v>2025</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>75</v>
       </c>
@@ -1879,7 +1879,7 @@
         <v>9</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E9" s="46">
         <v>2025</v>
@@ -1909,18 +1909,18 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -1932,9 +1932,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B2" s="23">
         <v>27.538556570687646</v>
@@ -1949,9 +1949,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="23">
         <v>10.331146370574086</v>
@@ -1966,9 +1966,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4" s="23">
         <v>4.8</v>
@@ -2001,24 +2001,24 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" t="s">
         <v>86</v>
       </c>
-      <c r="C1" t="s">
-        <v>87</v>
-      </c>
       <c r="D1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E1" t="s">
         <v>8</v>
@@ -2027,9 +2027,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B2" s="8">
         <v>10138</v>
@@ -2047,9 +2047,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" s="56">
         <v>0</v>
@@ -2062,9 +2062,9 @@
       </c>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" s="56">
         <v>0</v>
@@ -2077,9 +2077,9 @@
       </c>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B5" s="56">
         <v>0</v>
@@ -2091,9 +2091,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B6" s="56">
         <v>500</v>
@@ -2108,12 +2108,12 @@
         <v>77</v>
       </c>
       <c r="F6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B7" s="56">
         <v>0</v>
@@ -2125,9 +2125,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B8" s="56">
         <v>0</v>
@@ -2139,7 +2139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="57"/>
       <c r="C9" s="57"/>
       <c r="D9" s="57"/>
@@ -2157,24 +2157,24 @@
       <selection activeCell="G16" sqref="G16:G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" customWidth="1"/>
-    <col min="5" max="5" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.44140625" customWidth="1"/>
-    <col min="9" max="9" width="18.109375" customWidth="1"/>
-    <col min="12" max="12" width="16.44140625" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" customWidth="1"/>
+    <col min="13" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -2202,7 +2202,7 @@
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>10</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>10</v>
       </c>
@@ -2280,7 +2280,7 @@
       <c r="W3" s="2"/>
       <c r="Y3" s="6"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>10</v>
       </c>
@@ -2316,7 +2316,7 @@
       <c r="W4" s="2"/>
       <c r="Y4" s="4"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>10</v>
       </c>
@@ -2352,7 +2352,7 @@
       <c r="W5" s="2"/>
       <c r="Y5" s="5"/>
     </row>
-    <row r="6" spans="1:25" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>10</v>
       </c>
@@ -2389,7 +2389,7 @@
       </c>
       <c r="Y6" s="10"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>10</v>
       </c>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="Y7" s="10"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>10</v>
       </c>
@@ -2463,7 +2463,7 @@
       </c>
       <c r="Y8" s="10"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>11</v>
       </c>
@@ -2492,7 +2492,7 @@
       <c r="M9" s="13"/>
       <c r="Y9" s="10"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>11</v>
       </c>
@@ -2521,7 +2521,7 @@
       <c r="M10" s="13"/>
       <c r="Y10" s="10"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>11</v>
       </c>
@@ -2550,7 +2550,7 @@
       <c r="M11" s="13"/>
       <c r="Y11" s="10"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>11</v>
       </c>
@@ -2579,7 +2579,7 @@
       <c r="M12" s="13"/>
       <c r="Y12" s="10"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>11</v>
       </c>
@@ -2608,7 +2608,7 @@
       <c r="M13" s="13"/>
       <c r="Y13" s="10"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>11</v>
       </c>
@@ -2637,7 +2637,7 @@
       <c r="M14" s="13"/>
       <c r="Y14" s="10"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>11</v>
       </c>
@@ -2666,7 +2666,7 @@
       <c r="M15" s="13"/>
       <c r="Y15" s="10"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>1</v>
       </c>
@@ -2692,7 +2692,7 @@
       <c r="M16" s="13"/>
       <c r="Y16" s="4"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>1</v>
       </c>
@@ -2718,7 +2718,7 @@
       <c r="M17" s="13"/>
       <c r="Y17" s="5"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>1</v>
       </c>
@@ -2744,21 +2744,21 @@
       <c r="M18" s="13"/>
       <c r="Y18" s="9"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="M19" s="13"/>
       <c r="Y19" s="9"/>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E20" s="22"/>
       <c r="Y20" s="9"/>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E21" s="24"/>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E22" s="29"/>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="Q27" s="17"/>
       <c r="R27" s="9"/>
       <c r="S27" s="9"/>
@@ -2793,22 +2793,22 @@
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
-    <col min="7" max="7" width="27.109375" customWidth="1"/>
-    <col min="8" max="8" width="42.6640625" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" customWidth="1"/>
-    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" customWidth="1"/>
+    <col min="8" max="8" width="42.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -2840,7 +2840,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -2880,7 +2880,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
@@ -2920,12 +2920,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C4" s="36">
         <v>2025</v>
@@ -2937,13 +2937,13 @@
         <v>28</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G4" s="39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H4" s="39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I4" s="34">
         <f>D4*10^3</f>
@@ -2953,7 +2953,7 @@
         <v>37</v>
       </c>
       <c r="P4" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q4" s="11">
         <v>1.06</v>
@@ -2962,12 +2962,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C5" s="8">
         <v>2025</v>
@@ -2979,10 +2979,10 @@
         <v>28</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G5" s="39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H5" s="24"/>
       <c r="I5" s="23">
@@ -2993,7 +2993,7 @@
         <v>37</v>
       </c>
       <c r="P5" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Q5" s="11">
         <v>1.1399999999999999</v>
@@ -3002,7 +3002,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>4</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
         <v>4</v>
       </c>
@@ -3078,13 +3078,13 @@
         <v>1139.8825999999999</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F8" s="38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G8" s="39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H8" s="40"/>
       <c r="I8" s="34">
@@ -3095,7 +3095,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>4</v>
       </c>
@@ -3126,7 +3126,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>4</v>
       </c>
@@ -3157,7 +3157,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="32" t="s">
         <v>4</v>
       </c>
@@ -3174,10 +3174,10 @@
         <v>28</v>
       </c>
       <c r="F11" s="48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G11" s="49" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H11" s="50"/>
       <c r="I11" s="23">
@@ -3188,7 +3188,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>4</v>
       </c>
@@ -3219,7 +3219,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>4</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>5</v>
       </c>
@@ -3283,7 +3283,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>5</v>
       </c>
@@ -3316,7 +3316,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>5</v>
       </c>
@@ -3349,7 +3349,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>5</v>
       </c>
@@ -3382,9 +3382,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B18" s="36"/>
       <c r="C18" s="36">
@@ -3394,13 +3394,13 @@
         <v>2274.8177000000001</v>
       </c>
       <c r="E18" s="37" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F18" s="38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G18" s="39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H18" s="44"/>
       <c r="I18" s="34">
@@ -3411,9 +3411,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="36" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B19" s="36"/>
       <c r="C19" s="36">
@@ -3423,13 +3423,13 @@
         <v>57074.0625</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F19" s="38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G19" s="39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H19" s="44"/>
       <c r="I19" s="34">
@@ -3440,12 +3440,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="C20" s="8">
         <v>2020</v>
@@ -3471,12 +3471,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="C21" s="8">
         <v>2030</v>
@@ -3502,9 +3502,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="36" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B22" s="36"/>
       <c r="C22" s="36">
@@ -3514,13 +3514,13 @@
         <v>1989.7080000000001</v>
       </c>
       <c r="E22" s="37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F22" s="38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G22" s="39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H22" s="44"/>
       <c r="I22" s="34">
@@ -3531,12 +3531,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>100</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>101</v>
       </c>
       <c r="C23" s="8">
         <v>2020</v>
@@ -3562,12 +3562,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>100</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>101</v>
       </c>
       <c r="C24" s="8">
         <v>2030</v>
@@ -3593,12 +3593,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="36" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B25" s="36" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C25" s="36">
         <v>2025</v>
@@ -3607,13 +3607,13 @@
         <v>608.47739999999999</v>
       </c>
       <c r="E25" s="37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F25" s="38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G25" s="39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H25" s="44"/>
       <c r="I25" s="34">
@@ -3624,7 +3624,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="36" t="s">
         <v>5</v>
       </c>
@@ -3657,7 +3657,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>6</v>
       </c>
@@ -3693,7 +3693,7 @@
       <c r="S27" s="6"/>
       <c r="T27" s="6"/>
     </row>
-    <row r="28" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>6</v>
       </c>
@@ -3729,7 +3729,7 @@
       <c r="S28" s="4"/>
       <c r="T28" s="4"/>
     </row>
-    <row r="29" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>6</v>
       </c>
@@ -3765,7 +3765,7 @@
       <c r="S29" s="5"/>
       <c r="T29" s="5"/>
     </row>
-    <row r="30" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>6</v>
       </c>
@@ -3800,7 +3800,7 @@
       <c r="S30" s="9"/>
       <c r="T30" s="10"/>
     </row>
-    <row r="31" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>6</v>
       </c>
@@ -3835,7 +3835,7 @@
       <c r="S31" s="9"/>
       <c r="T31" s="10"/>
     </row>
-    <row r="32" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>6</v>
       </c>
@@ -3868,12 +3868,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="36" t="s">
         <v>6</v>
       </c>
       <c r="B33" s="36" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C33" s="36">
         <v>2025</v>
@@ -3883,16 +3883,16 @@
         <v>395.77480000000003</v>
       </c>
       <c r="E33" s="37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F33" s="38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G33" s="39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H33" s="43" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I33" s="34">
         <f>D33*$Q$4*10^3</f>
@@ -3902,12 +3902,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="36" t="s">
         <v>6</v>
       </c>
       <c r="B34" s="36" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C34" s="36">
         <v>2025</v>
@@ -3917,16 +3917,16 @@
         <v>560.37540000000001</v>
       </c>
       <c r="E34" s="37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F34" s="38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G34" s="39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H34" s="43" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I34" s="34">
         <f>D34*$Q$4*10^3</f>
@@ -3936,7 +3936,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -3948,7 +3948,7 @@
       <c r="I35" s="8"/>
       <c r="J35" s="8"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
@@ -3960,7 +3960,7 @@
       <c r="I36" s="8"/>
       <c r="J36" s="8"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
@@ -3972,7 +3972,7 @@
       <c r="I37" s="23"/>
       <c r="J37" s="8"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
@@ -3984,7 +3984,7 @@
       <c r="I38" s="8"/>
       <c r="J38" s="8"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
@@ -3996,7 +3996,7 @@
       <c r="I39" s="8"/>
       <c r="J39" s="8"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
@@ -4008,7 +4008,7 @@
       <c r="I40" s="8"/>
       <c r="J40" s="8"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>

</xml_diff>

<commit_message>
Fixed lifetime nuclear + added LCOE in altri_dati.xlsx
</commit_message>
<xml_diff>
--- a/dati_casoStudioItalia/altri_dati.xlsx
+++ b/dati_casoStudioItalia/altri_dati.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0954659\PycharmProjects\DrinDrin---Mix-energetico\dati_casoStudioItalia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECACA251-0A23-44A9-8D37-BBEE7E4C81C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79556390-5D4E-454E-A39F-65C4BF347B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="797" xr2:uid="{B845255D-815F-49EA-8438-49CAB31B3547}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="797" activeTab="7" xr2:uid="{B845255D-815F-49EA-8438-49CAB31B3547}"/>
   </bookViews>
   <sheets>
     <sheet name="discount_rate" sheetId="7" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Transmission_abroad" sheetId="4" r:id="rId5"/>
     <sheet name="raw_data_commodity" sheetId="2" r:id="rId6"/>
     <sheet name="raw_data_techs" sheetId="3" r:id="rId7"/>
+    <sheet name="resulting_lcoe_input" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -306,7 +307,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="133">
   <si>
     <t>CAPEX solare</t>
   </si>
@@ -684,13 +685,35 @@
   </si>
   <si>
     <t>EUR/(1.5MW_turbine)</t>
+  </si>
+  <si>
+    <t>discount rate</t>
+  </si>
+  <si>
+    <t>opex_fixed</t>
+  </si>
+  <si>
+    <t>lifetime</t>
+  </si>
+  <si>
+    <t>capex [eur/MW]</t>
+  </si>
+  <si>
+    <t>capacity_factor</t>
+  </si>
+  <si>
+    <t>annualization_factor</t>
+  </si>
+  <si>
+    <t>lcoe [eur/MWh]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
+    <numFmt numFmtId="8" formatCode="&quot;€&quot;#,##0.00_);[Red]\(&quot;€&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0E+00"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
@@ -861,7 +884,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1027,6 +1050,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1363,10 +1388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{923C661C-C997-4238-A47F-A35B6AA9581D}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1431,7 +1456,7 @@
         <v>76</v>
       </c>
       <c r="B4" s="8">
-        <v>0.45</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>80</v>
@@ -1522,6 +1547,12 @@
       </c>
       <c r="E9" s="7" t="s">
         <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="60">
+        <f>PMT(0.07,25,1)</f>
+        <v>-8.5810517220665614E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1718,10 +1749,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C372154-4B0A-49B9-8FF3-F49D60098BF7}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1884,6 +1915,9 @@
       <c r="E9" s="46">
         <v>2025</v>
       </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="59"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4088,4 +4122,143 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CF654B-A1B6-4A16-BEFC-ED44AE47A5E3}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2">
+        <f>discount_rate!B2</f>
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="C2" s="10">
+        <f>CAPEX!B2</f>
+        <v>676570.29999999993</v>
+      </c>
+      <c r="D2">
+        <f>OPEX!B2</f>
+        <v>1.7274999999999999E-2</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>0.15</v>
+      </c>
+      <c r="G2" s="60">
+        <f>PMT(B2,E2,-1)</f>
+        <v>8.5073306425680659E-2</v>
+      </c>
+      <c r="H2">
+        <f>C2*(D2+G2)/(8760*F2*1)</f>
+        <v>52.698496486236436</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3">
+        <f>discount_rate!B3</f>
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="C3" s="10">
+        <f>CAPEX!B3/1.5</f>
+        <v>1208275.5560000001</v>
+      </c>
+      <c r="D3">
+        <f>OPEX!B3</f>
+        <v>1.2346999999999999E-2</v>
+      </c>
+      <c r="E3">
+        <v>25</v>
+      </c>
+      <c r="F3">
+        <v>0.25</v>
+      </c>
+      <c r="G3" s="60">
+        <f t="shared" ref="G3:G4" si="0">PMT(B3,E3,-1)</f>
+        <v>9.0498958147827546E-2</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H4" si="1">C3*(D3+G3)/(8760*F3*1)</f>
+        <v>56.742583225305509</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4">
+        <f>discount_rate!B4</f>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C4" s="10">
+        <f>CAPEX!B4</f>
+        <v>7500000</v>
+      </c>
+      <c r="D4">
+        <f>OPEX!B4</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="E4">
+        <v>60</v>
+      </c>
+      <c r="F4">
+        <v>0.85</v>
+      </c>
+      <c r="G4" s="60">
+        <f t="shared" si="0"/>
+        <v>4.8454255846261174E-2</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>82.044979700101905</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat/update nuclear capex (avg between IAEA and S&P)
</commit_message>
<xml_diff>
--- a/dati_casoStudioItalia/altri_dati.xlsx
+++ b/dati_casoStudioItalia/altri_dati.xlsx
@@ -76,29 +76,6 @@
           </rPr>
           <t xml:space="preserve">in MWh
 </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Bertoni, L. (Luca):
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Valore proposto da Lorenzo, non dato IAEA</t>
         </r>
       </text>
     </comment>
@@ -278,7 +255,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="143">
   <si>
     <t xml:space="preserve">discount_rate</t>
   </si>
@@ -352,282 +329,297 @@
     <t xml:space="preserve">EUR/(1.5MW_turbine)</t>
   </si>
   <si>
+    <t xml:space="preserve">Media tra IAEA e S&amp;P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EPR nuova costruzione, ~2020-2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EUR/MWh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025, 2 h, Average utility-home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fuel_cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">costo_combustibile_gas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> EUR/MWh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">World Bank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average annual value, 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">costo_combustibile_carbone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">costo_combustibile_nucleare </t>
+  </si>
+  <si>
+    <t xml:space="preserve">World Nuclear Association, EIA, NREL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average between values found (2020-2021)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">capacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emission_factor_t/MWh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NORD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electricity map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Include francia, svizzera, slovenia, austria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CNOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSUD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grecia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SARD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SICI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entry voice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model input value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">costo combustibile gas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">($2010/mmbtu)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Natural gas, Europe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(€2020/MWh)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conversion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">€2020/$2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harmonised Index of Consumer Prices (HICP)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MWh/mmbtu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MWh/kcal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard heating value of thermal coal (kcal/kg)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">€2020/$2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">€2020/$2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">costo combustibile carbone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">($2010/mt)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coal, Australian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">costo combustibile nucleare </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(c$2021/kWh)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">World Nuclear Association</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020-2040</t>
+  </si>
+  <si>
+    <t xml:space="preserve">($2020/MWh)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NREL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tech type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAPEX solare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utility scale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(M$2020/GW)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dati elaborati da NREL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(€2020/MW)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dati elaborati da Danish Energy Agency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mixed investment costs based on average of 50% 'solar-rooftop' and 50% 'solar-utility'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">€2020/€2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">€2020/€2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAPEX eolico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Onshore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">€2020/€2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">€2020/€2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(M$2015/GW)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">€2018/$2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Banca d’Italia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offshore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offshore acque profonde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAPEX nucleare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AP1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Include il decommissioning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAPEX idroelettrico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(M€2010/GW)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAPEX PHS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(€2015/MWh)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAPEX carbone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ciclo a vapore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(M€2015/GW)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAPEX gas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ciclo combinato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gas turbine, simple cycle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EPR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(M$2025/GW)</t>
+  </si>
+  <si>
     <t xml:space="preserve">IAEA</t>
   </si>
   <si>
-    <t xml:space="preserve">2020 (EPR Francia)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EUR/MWh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2025, 2 h, Average utility-home</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fuel_cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">costo_combustibile_gas</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> EUR/MWh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">World Bank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average annual value, 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">costo_combustibile_carbone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">costo_combustibile_nucleare </t>
-  </si>
-  <si>
-    <t xml:space="preserve">World Nuclear Association, EIA, NREL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average between values found (2020-2021)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">capacity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">emission_factor_t/MWh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NORD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">electricity map</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Include francia, svizzera, slovenia, austria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CALA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CNOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSUD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SUD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grecia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SARD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SICI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entry voice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Model input value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Model unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">costo combustibile gas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">($2010/mmbtu)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Natural gas, Europe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(€2020/MWh)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conversion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multiplier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">€2020/$2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Harmonised Index of Consumer Prices (HICP)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MWh/mmbtu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MWh/kcal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Standard heating value of thermal coal (kcal/kg)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">€2020/$2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">€2020/$2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">costo combustibile carbone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">($2010/mt)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coal, Australian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">costo combustibile nucleare </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(c$2021/kWh)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">World Nuclear Association</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020-2040</t>
-  </si>
-  <si>
-    <t xml:space="preserve">($2020/MWh)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NREL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EIA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tech type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comment 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comment 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAPEX solare</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utility scale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(M$2020/GW)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dati elaborati da NREL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(€2020/MW)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">General</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dati elaborati da Danish Energy Agency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mixed investment costs based on average of 50% 'solar-rooftop' and 50% 'solar-utility'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">€2020/€2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">€2010/€2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAPEX eolico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Onshore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(M$2015/GW)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Offshore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Offshore acque profonde</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAPEX nucleare</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AP1000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Include il decommissioning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAPEX idroelettrico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(M€2010/GW)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAPEX PHS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(€2015/MWh)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAPEX carbone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ciclo a vapore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(M€2015/GW)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAPEX gas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ciclo combinato</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gas turbine, simple cycle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EPR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(M$2025/GW)</t>
-  </si>
-  <si>
     <t xml:space="preserve">EPR Francia</t>
   </si>
   <si>
@@ -671,9 +663,6 @@
   </si>
   <si>
     <t xml:space="preserve">EPR EU, nuova costruzione</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Media tra IAEA e S&amp;P</t>
   </si>
   <si>
     <t xml:space="preserve">discount rate</t>
@@ -945,12 +934,16 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="64">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -962,55 +955,55 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1018,7 +1011,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1026,79 +1019,71 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1110,19 +1095,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1130,11 +1115,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1142,7 +1127,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1150,7 +1135,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1166,15 +1151,15 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1190,15 +1175,15 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1465,161 +1450,161 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="35.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="35.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="2" t="n">
         <v>0.057</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="2" t="n">
         <v>0.076</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="2" t="n">
         <v>0.045</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="2" t="n">
         <v>0.08</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="2" t="n">
         <v>0.052</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7" s="2" t="n">
         <v>0.027</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="2" t="n">
         <v>0.062</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="B9" s="2" t="n">
         <v>0.052</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D17" s="4" t="n">
+      <c r="D17" s="5" t="n">
         <f aca="false">PMT(0.07,25,1)</f>
         <v>-0.0858105172206656</v>
       </c>
@@ -1659,162 +1644,162 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="35.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="35.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="n">
+      <c r="B2" s="6" t="n">
         <f aca="false">1.7275/100</f>
         <v>0.017275</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="5" t="n">
+      <c r="B3" s="6" t="n">
         <f aca="false">1.2347/100</f>
         <v>0.012347</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="7" t="n">
+      <c r="E3" s="8" t="n">
         <v>2025</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="8" t="n">
+      <c r="B4" s="9" t="n">
         <v>0.033</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="7" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="8" t="n">
+      <c r="B5" s="9" t="n">
         <v>0.017</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="7" t="s">
+      <c r="D5" s="3"/>
+      <c r="E5" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="5" t="n">
+      <c r="B6" s="6" t="n">
         <f aca="false">1/100</f>
         <v>0.01</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="9" t="n">
+      <c r="E6" s="10" t="n">
         <v>2025</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="5" t="n">
+      <c r="B7" s="6" t="n">
         <f aca="false">3.313/100</f>
         <v>0.03313</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="5" t="n">
+      <c r="B8" s="6" t="n">
         <f aca="false">1.6316/100</f>
         <v>0.016316</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="7" t="n">
+      <c r="E8" s="8" t="n">
         <v>2025</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="5" t="n">
+      <c r="B9" s="6" t="n">
         <f aca="false">0.43/100</f>
         <v>0.0043</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="9" t="n">
+      <c r="E9" s="10" t="n">
         <v>2025</v>
       </c>
     </row>
@@ -1845,183 +1830,183 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="35.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="35.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="10" t="n">
+      <c r="B2" s="11" t="n">
         <v>676570.3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="11" t="n">
+      <c r="B3" s="12" t="n">
         <f aca="false">1208275.556*1.5</f>
         <v>1812413.334</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="7" t="n">
+      <c r="E3" s="8" t="n">
         <v>2025</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="12" t="n">
-        <v>7500000</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="13" t="n">
+        <f aca="false">1000*raw_data_techs!I37</f>
+        <v>5887449.78165939</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="13" t="n">
+      <c r="B5" s="14" t="n">
         <f aca="false">506759.606*0.3</f>
         <v>152027.8818</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="2" t="n">
         <v>2593292.178</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="9" t="n">
+      <c r="E6" s="10" t="n">
         <v>2025</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="14" t="n">
+      <c r="B7" s="15" t="n">
         <v>644986.044</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="14" t="n">
+      <c r="B8" s="15" t="n">
         <v>2109090.48</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="7" t="n">
+      <c r="E8" s="8" t="n">
         <v>2025</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="15" t="n">
+      <c r="B9" s="16" t="n">
         <v>60498.50625</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="9" t="n">
+      <c r="E9" s="10" t="n">
         <v>2025</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E18" s="16"/>
+      <c r="E18" s="17"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId2" display="PyPSA/technology-data"/>
     <hyperlink ref="D3" r:id="rId3" display="PyPSA/technology-data"/>
-    <hyperlink ref="D4" r:id="rId4" display="IAEA"/>
-    <hyperlink ref="D5" r:id="rId5" display="PyPSA/technology-data"/>
-    <hyperlink ref="D6" r:id="rId6" display="PyPSA/technology-data"/>
-    <hyperlink ref="D7" r:id="rId7" display="PyPSA/technology-data"/>
-    <hyperlink ref="D8" r:id="rId8" display="PyPSA/technology-data"/>
-    <hyperlink ref="D9" r:id="rId9" display="PyPSA/technology-data"/>
+    <hyperlink ref="D5" r:id="rId4" display="PyPSA/technology-data"/>
+    <hyperlink ref="D6" r:id="rId5" display="PyPSA/technology-data"/>
+    <hyperlink ref="D7" r:id="rId6" display="PyPSA/technology-data"/>
+    <hyperlink ref="D8" r:id="rId7" display="PyPSA/technology-data"/>
+    <hyperlink ref="D9" r:id="rId8" display="PyPSA/technology-data"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2030,7 +2015,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <legacyDrawing r:id="rId10"/>
+  <legacyDrawing r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -2047,75 +2032,75 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="35.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="35.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="10" t="n">
+      <c r="B2" s="11" t="n">
         <v>27.5385565706876</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="19" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="10" t="n">
+      <c r="B3" s="11" t="n">
         <v>10.3311463705741</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="19" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="10" t="n">
+      <c r="B4" s="11" t="n">
         <v>4.8</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="19" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2139,7 +2124,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
@@ -2147,146 +2132,141 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="35.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="35.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="2" t="n">
         <v>10138</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="C2" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="21" t="n">
+      <c r="B3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="C3" s="21" t="n">
+      <c r="C3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D3" s="21" t="n">
+      <c r="D3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="21" t="n">
+      <c r="B4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="C4" s="21" t="n">
+      <c r="C4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D4" s="21" t="n">
+      <c r="D4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="21" t="n">
+      <c r="B5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="C5" s="21" t="n">
+      <c r="C5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D5" s="21" t="n">
+      <c r="D5" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="21" t="n">
+      <c r="B6" s="2" t="n">
         <v>500</v>
       </c>
-      <c r="C6" s="21" t="n">
+      <c r="C6" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="D6" s="21" t="n">
+      <c r="D6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="19" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="21" t="n">
+      <c r="B7" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="C7" s="21" t="n">
+      <c r="C7" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D7" s="21" t="n">
+      <c r="D7" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="21" t="n">
+      <c r="B8" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="C8" s="21" t="n">
+      <c r="C8" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D8" s="21" t="n">
+      <c r="D8" s="2" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2312,609 +2292,609 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="9.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="10.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="23.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="10.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="23.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="25" t="n">
+      <c r="B2" s="24" t="n">
         <v>2018</v>
       </c>
-      <c r="C2" s="26" t="n">
+      <c r="C2" s="25" t="n">
         <v>7.54140943832</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="29" t="n">
+      <c r="G2" s="28" t="n">
         <f aca="false">C2*$M$3/$M$4</f>
         <v>21.8055455217419</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23" t="s">
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="M2" s="23" t="s">
+      <c r="M2" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="N2" s="23" t="s">
+      <c r="N2" s="22" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="25" t="n">
+      <c r="B3" s="24" t="n">
         <v>2019</v>
       </c>
-      <c r="C3" s="26" t="n">
+      <c r="C3" s="25" t="n">
         <v>4.82745402713</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="28" t="s">
+      <c r="F3" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="29" t="n">
+      <c r="G3" s="28" t="n">
         <f aca="false">C3*$M$3/$M$4</f>
         <v>13.9583017476571</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="30" t="s">
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="M3" s="31" t="n">
+      <c r="M3" s="30" t="n">
         <v>0.85</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="W3" s="23"/>
-      <c r="Y3" s="2"/>
+      <c r="W3" s="22"/>
+      <c r="Y3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="25" t="n">
+      <c r="B4" s="24" t="n">
         <v>2020</v>
       </c>
-      <c r="C4" s="26" t="n">
+      <c r="C4" s="25" t="n">
         <v>3.31156694524004</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="29" t="n">
+      <c r="G4" s="28" t="n">
         <f aca="false">C4*$M$3/$M$4</f>
         <v>9.57520266779388</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="L4" s="30" t="s">
+      <c r="L4" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="M4" s="32" t="n">
+      <c r="M4" s="31" t="n">
         <v>0.293971</v>
       </c>
-      <c r="N4" s="1"/>
-      <c r="W4" s="23"/>
-      <c r="Y4" s="24"/>
+      <c r="N4" s="2"/>
+      <c r="W4" s="22"/>
+      <c r="Y4" s="23"/>
     </row>
     <row r="5" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="25" t="n">
+      <c r="B5" s="24" t="n">
         <v>2021</v>
       </c>
-      <c r="C5" s="26" t="n">
+      <c r="C5" s="25" t="n">
         <v>14.7311498614077</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="F5" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="G5" s="29" t="n">
+      <c r="G5" s="28" t="n">
         <f aca="false">C5*$M$3/$M$4</f>
         <v>42.5942605978023</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="L5" s="30" t="s">
+      <c r="L5" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="M5" s="33" t="n">
+      <c r="M5" s="32" t="n">
         <f aca="false">1.622*10^-6</f>
         <v>1.622E-006</v>
       </c>
-      <c r="W5" s="23"/>
-      <c r="Y5" s="34"/>
+      <c r="W5" s="22"/>
+      <c r="Y5" s="33"/>
     </row>
     <row r="6" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="25" t="n">
+      <c r="B6" s="24" t="n">
         <v>2022</v>
       </c>
-      <c r="C6" s="26" t="n">
+      <c r="C6" s="25" t="n">
         <v>34.346664233461</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="28" t="s">
+      <c r="F6" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="G6" s="29" t="n">
+      <c r="G6" s="28" t="n">
         <f aca="false">C6*$M$3/$M$4</f>
         <v>99.3113762869191</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="L6" s="35" t="s">
+      <c r="L6" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="M6" s="31" t="n">
+      <c r="M6" s="30" t="n">
         <v>6000</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="N6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="Y6" s="13"/>
+      <c r="Y6" s="14"/>
     </row>
     <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="25" t="n">
+      <c r="B7" s="24" t="n">
         <v>2023</v>
       </c>
-      <c r="C7" s="26" t="n">
+      <c r="C7" s="25" t="n">
         <v>11.4929038091148</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="F7" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="G7" s="29" t="n">
+      <c r="G7" s="28" t="n">
         <f aca="false">C7*$M$3/$M$4</f>
         <v>33.2310610153641</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="L7" s="30" t="s">
+      <c r="L7" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="M7" s="31" t="n">
+      <c r="M7" s="30" t="n">
         <v>0.82</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="N7" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="Y7" s="13"/>
+      <c r="Y7" s="14"/>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="25" t="n">
+      <c r="B8" s="24" t="n">
         <v>2024</v>
       </c>
-      <c r="C8" s="26" t="n">
+      <c r="C8" s="25" t="n">
         <v>9.52416119251955</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="F8" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="G8" s="29" t="n">
+      <c r="G8" s="28" t="n">
         <f aca="false">C8*$M$3/$M$4</f>
         <v>27.5385565706876</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="L8" s="30" t="s">
+      <c r="L8" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="M8" s="31" t="n">
+      <c r="M8" s="30" t="n">
         <v>0.88</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="N8" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="Y8" s="13"/>
+      <c r="Y8" s="14"/>
     </row>
     <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="25" t="n">
+      <c r="B9" s="24" t="n">
         <v>2018</v>
       </c>
-      <c r="C9" s="26" t="n">
+      <c r="C9" s="25" t="n">
         <v>105.06823090516</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="28" t="s">
+      <c r="F9" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="G9" s="29" t="n">
+      <c r="G9" s="28" t="n">
         <f aca="false">C9*$M$3/$M$6/$M$5/1000</f>
         <v>9.17673615591718</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="M9" s="36"/>
-      <c r="Y9" s="13"/>
+      <c r="M9" s="35"/>
+      <c r="Y9" s="14"/>
     </row>
     <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="B10" s="25" t="n">
+      <c r="B10" s="24" t="n">
         <v>2019</v>
       </c>
-      <c r="C10" s="26" t="n">
+      <c r="C10" s="25" t="n">
         <v>78.29295670822</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="G10" s="29" t="n">
+      <c r="G10" s="28" t="n">
         <f aca="false">C10*$M$3/$M$6/$M$5/1000</f>
         <v>6.83816411857655</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="M10" s="36"/>
-      <c r="Y10" s="13"/>
+      <c r="M10" s="35"/>
+      <c r="Y10" s="14"/>
     </row>
     <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="25" t="n">
+      <c r="B11" s="24" t="n">
         <v>2020</v>
       </c>
-      <c r="C11" s="26" t="n">
+      <c r="C11" s="25" t="n">
         <v>62.0888661899898</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="F11" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="G11" s="29" t="n">
+      <c r="G11" s="28" t="n">
         <f aca="false">C11*$M$3/$M$6/$M$5/1000</f>
         <v>5.42288699768715</v>
       </c>
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="M11" s="36"/>
-      <c r="Y11" s="13"/>
+      <c r="M11" s="35"/>
+      <c r="Y11" s="14"/>
     </row>
     <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="25" t="n">
+      <c r="B12" s="24" t="n">
         <v>2021</v>
       </c>
-      <c r="C12" s="26" t="n">
+      <c r="C12" s="25" t="n">
         <v>126.188299817185</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="28" t="s">
+      <c r="F12" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="G12" s="29" t="n">
+      <c r="G12" s="28" t="n">
         <f aca="false">C12*$M$3/$M$6/$M$5/1000</f>
         <v>11.0213784262851</v>
       </c>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="M12" s="36"/>
-      <c r="Y12" s="13"/>
+      <c r="M12" s="35"/>
+      <c r="Y12" s="14"/>
     </row>
     <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="25" t="n">
+      <c r="B13" s="24" t="n">
         <v>2022</v>
       </c>
-      <c r="C13" s="26" t="n">
+      <c r="C13" s="25" t="n">
         <v>293.651199091809</v>
       </c>
-      <c r="D13" s="27" t="s">
+      <c r="D13" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="28" t="s">
+      <c r="F13" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="G13" s="29" t="n">
+      <c r="G13" s="28" t="n">
         <f aca="false">C13*$M$3/$M$6/$M$5/1000</f>
         <v>25.6477105659718</v>
       </c>
-      <c r="H13" s="18" t="s">
+      <c r="H13" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="M13" s="36"/>
-      <c r="Y13" s="13"/>
+      <c r="M13" s="35"/>
+      <c r="Y13" s="14"/>
     </row>
     <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="B14" s="25" t="n">
+      <c r="B14" s="24" t="n">
         <v>2023</v>
       </c>
-      <c r="C14" s="26" t="n">
+      <c r="C14" s="25" t="n">
         <v>151.427841075083</v>
       </c>
-      <c r="D14" s="27" t="s">
+      <c r="D14" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="28" t="s">
+      <c r="F14" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="G14" s="29" t="n">
+      <c r="G14" s="28" t="n">
         <f aca="false">C14*$M$3/$M$6/$M$5/1000</f>
         <v>13.2258184251768</v>
       </c>
-      <c r="H14" s="18" t="s">
+      <c r="H14" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="M14" s="36"/>
-      <c r="Y14" s="13"/>
+      <c r="M14" s="35"/>
+      <c r="Y14" s="14"/>
     </row>
     <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="25" t="n">
+      <c r="B15" s="24" t="n">
         <v>2024</v>
       </c>
-      <c r="C15" s="26" t="n">
+      <c r="C15" s="25" t="n">
         <v>118.285548798149</v>
       </c>
-      <c r="D15" s="27" t="s">
+      <c r="D15" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="28" t="s">
+      <c r="F15" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="G15" s="29" t="n">
+      <c r="G15" s="28" t="n">
         <f aca="false">C15*$M$3/$M$6/$M$5/1000</f>
         <v>10.3311463705741</v>
       </c>
-      <c r="H15" s="18" t="s">
+      <c r="H15" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="M15" s="36"/>
-      <c r="Y15" s="13"/>
+      <c r="M15" s="35"/>
+      <c r="Y15" s="14"/>
     </row>
     <row r="16" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="25" t="n">
+      <c r="B16" s="24" t="n">
         <v>2021</v>
       </c>
-      <c r="C16" s="26" t="n">
+      <c r="C16" s="25" t="n">
         <v>0.46</v>
       </c>
-      <c r="D16" s="27" t="s">
+      <c r="D16" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E16" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="G16" s="29" t="n">
+      <c r="G16" s="28" t="n">
         <f aca="false">C16*M7/100*1000</f>
         <v>3.772</v>
       </c>
-      <c r="H16" s="18" t="s">
+      <c r="H16" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="M16" s="36"/>
-      <c r="Y16" s="24"/>
+      <c r="M16" s="35"/>
+      <c r="Y16" s="23"/>
     </row>
     <row r="17" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="C17" s="26" t="n">
+      <c r="C17" s="25" t="n">
         <v>7</v>
       </c>
-      <c r="D17" s="38" t="s">
+      <c r="D17" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="E17" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="G17" s="29" t="n">
+      <c r="G17" s="28" t="n">
         <f aca="false">C17*M7</f>
         <v>5.74</v>
       </c>
-      <c r="H17" s="18" t="s">
+      <c r="H17" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="M17" s="36"/>
-      <c r="Y17" s="34"/>
+      <c r="M17" s="35"/>
+      <c r="Y17" s="33"/>
     </row>
     <row r="18" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B18" s="25" t="n">
+      <c r="B18" s="24" t="n">
         <v>2021</v>
       </c>
-      <c r="C18" s="26" t="n">
+      <c r="C18" s="25" t="n">
         <v>0.61</v>
       </c>
-      <c r="D18" s="27" t="s">
+      <c r="D18" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="E18" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="G18" s="29" t="n">
+      <c r="G18" s="28" t="n">
         <f aca="false">C18*M7/100*1000</f>
         <v>5.002</v>
       </c>
-      <c r="H18" s="18" t="s">
+      <c r="H18" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="M18" s="36"/>
-      <c r="Y18" s="29"/>
+      <c r="M18" s="35"/>
+      <c r="Y18" s="28"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M19" s="36"/>
-      <c r="Y19" s="29"/>
+      <c r="M19" s="35"/>
+      <c r="Y19" s="28"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E20" s="17"/>
-      <c r="Y20" s="29"/>
+      <c r="E20" s="18"/>
+      <c r="Y20" s="28"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E21" s="39"/>
+      <c r="E21" s="38"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E22" s="40"/>
+      <c r="E22" s="39"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q27" s="41"/>
-      <c r="R27" s="29"/>
-      <c r="S27" s="29"/>
+      <c r="Q27" s="40"/>
+      <c r="R27" s="28"/>
+      <c r="S27" s="28"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2957,1279 +2937,1316 @@
   </sheetPr>
   <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M29" activeCellId="0" sqref="M29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I36" activeCellId="0" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="42.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="27.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="42.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="12.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="12.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="7.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="12.48"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="J1" s="23" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="C2" s="2" t="n">
         <v>2020</v>
       </c>
-      <c r="D2" s="10" t="n">
+      <c r="D2" s="11" t="n">
         <v>1333</v>
       </c>
-      <c r="E2" s="38" t="s">
+      <c r="E2" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="39" t="s">
+      <c r="G2" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="H2" s="39"/>
-      <c r="I2" s="10" t="n">
+      <c r="H2" s="38"/>
+      <c r="I2" s="11" t="n">
         <f aca="false">D2*$Q$3*10^3</f>
         <v>1173040</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="P2" s="23" t="s">
+      <c r="P2" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="Q2" s="23" t="s">
+      <c r="Q2" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="R2" s="23" t="s">
+      <c r="R2" s="22" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="2" t="n">
         <v>2030</v>
       </c>
-      <c r="D3" s="10" t="n">
+      <c r="D3" s="11" t="n">
         <v>754</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="39" t="s">
+      <c r="G3" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="H3" s="39"/>
-      <c r="I3" s="10" t="n">
+      <c r="H3" s="38"/>
+      <c r="I3" s="11" t="n">
         <f aca="false">D3*$Q$3*10^3</f>
         <v>663520</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="P3" s="30" t="s">
+      <c r="P3" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="Q3" s="31" t="n">
+      <c r="Q3" s="30" t="n">
         <v>0.88</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="R3" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="42" t="s">
+    <row r="4" customFormat="false" ht="28.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="C4" s="42" t="n">
+      <c r="C4" s="41" t="n">
         <v>2025</v>
       </c>
-      <c r="D4" s="43" t="n">
+      <c r="D4" s="42" t="n">
         <v>676.5703</v>
       </c>
-      <c r="E4" s="44" t="s">
+      <c r="E4" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="F4" s="45" t="s">
+      <c r="F4" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="46" t="s">
+      <c r="G4" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="H4" s="46" t="s">
+      <c r="H4" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="I4" s="47" t="n">
+      <c r="I4" s="46" t="n">
         <f aca="false">D4*10^3</f>
         <v>676570.3</v>
       </c>
-      <c r="J4" s="42" t="s">
+      <c r="J4" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="P4" s="30" t="s">
+      <c r="P4" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="Q4" s="31" t="n">
+      <c r="Q4" s="30" t="n">
         <v>1.06</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="R4" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="2" t="n">
         <v>2025</v>
       </c>
-      <c r="D5" s="10" t="n">
+      <c r="D5" s="11" t="n">
         <v>473.1156</v>
       </c>
-      <c r="E5" s="38" t="s">
+      <c r="E5" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="46" t="s">
+      <c r="G5" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="H5" s="39"/>
-      <c r="I5" s="10" t="n">
+      <c r="H5" s="38"/>
+      <c r="I5" s="11" t="n">
         <f aca="false">D5*10^3</f>
         <v>473115.6</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="P5" s="30" t="s">
+      <c r="P5" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="Q5" s="31" t="n">
+      <c r="Q5" s="30" t="n">
         <v>1.14</v>
       </c>
-      <c r="R5" s="3" t="s">
+      <c r="R5" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="C6" s="2" t="n">
         <v>2020</v>
       </c>
-      <c r="D6" s="10" t="n">
+      <c r="D6" s="11" t="n">
         <v>1462</v>
       </c>
-      <c r="E6" s="38" t="s">
+      <c r="E6" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="39" t="s">
+      <c r="G6" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="H6" s="39"/>
-      <c r="I6" s="10" t="n">
+      <c r="H6" s="38"/>
+      <c r="I6" s="11" t="n">
         <f aca="false">D6*$Q$3*10^3</f>
         <v>1286560</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="2" t="s">
         <v>88</v>
       </c>
+      <c r="P6" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q6" s="30" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="C7" s="2" t="n">
         <v>2030</v>
       </c>
-      <c r="D7" s="10" t="n">
+      <c r="D7" s="11" t="n">
         <v>956</v>
       </c>
-      <c r="E7" s="38" t="s">
+      <c r="E7" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="39" t="s">
+      <c r="G7" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="H7" s="39"/>
-      <c r="I7" s="10" t="n">
+      <c r="H7" s="38"/>
+      <c r="I7" s="11" t="n">
         <f aca="false">D7*$Q$3*10^3</f>
         <v>841280</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="42" t="s">
+      <c r="P7" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q7" s="30" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="23.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="C8" s="42" t="n">
+      <c r="C8" s="41" t="n">
         <v>2025</v>
       </c>
-      <c r="D8" s="47" t="n">
+      <c r="D8" s="46" t="n">
         <v>1139.8826</v>
       </c>
-      <c r="E8" s="44" t="s">
-        <v>97</v>
-      </c>
-      <c r="F8" s="45" t="s">
+      <c r="E8" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="F8" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="46" t="s">
+      <c r="G8" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="H8" s="48"/>
-      <c r="I8" s="47" t="n">
+      <c r="H8" s="47"/>
+      <c r="I8" s="46" t="n">
         <f aca="false">D8*$Q$4*10^3</f>
         <v>1208275.556</v>
       </c>
-      <c r="J8" s="42" t="s">
+      <c r="J8" s="41" t="s">
         <v>88</v>
       </c>
+      <c r="P8" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q8" s="31" t="n">
+        <f aca="false">1/1.145</f>
+        <v>0.873362445414847</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C9" s="1" t="n">
+      <c r="B9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" s="2" t="n">
         <v>2020</v>
       </c>
-      <c r="D9" s="10" t="n">
+      <c r="D9" s="11" t="n">
         <v>3739</v>
       </c>
-      <c r="E9" s="38" t="s">
+      <c r="E9" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="39" t="s">
+      <c r="G9" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="H9" s="39"/>
-      <c r="I9" s="10" t="n">
+      <c r="H9" s="38"/>
+      <c r="I9" s="11" t="n">
         <f aca="false">D9*$Q$3*10^3</f>
         <v>3290320</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="2" t="s">
         <v>88</v>
       </c>
+      <c r="P9" s="29"/>
     </row>
     <row r="10" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C10" s="1" t="n">
+      <c r="B10" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="2" t="n">
         <v>2030</v>
       </c>
-      <c r="D10" s="10" t="n">
+      <c r="D10" s="11" t="n">
         <v>2758</v>
       </c>
-      <c r="E10" s="38" t="s">
+      <c r="E10" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="39" t="s">
+      <c r="G10" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="H10" s="39"/>
-      <c r="I10" s="10" t="n">
+      <c r="H10" s="38"/>
+      <c r="I10" s="11" t="n">
         <f aca="false">D10*$Q$3*10^3</f>
         <v>2427040</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="B11" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="C11" s="14" t="n">
+      <c r="B11" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" s="15" t="n">
         <v>2025</v>
       </c>
-      <c r="D11" s="49" t="n">
+      <c r="D11" s="48" t="n">
         <v>1769.1171</v>
       </c>
-      <c r="E11" s="38" t="s">
+      <c r="E11" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="F11" s="50" t="s">
+      <c r="F11" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="51" t="s">
+      <c r="G11" s="50" t="s">
         <v>90</v>
       </c>
-      <c r="H11" s="52"/>
-      <c r="I11" s="10" t="n">
+      <c r="H11" s="51"/>
+      <c r="I11" s="11" t="n">
         <f aca="false">D11*10^3</f>
         <v>1769117.1</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J11" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C12" s="1" t="n">
+      <c r="B12" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" s="2" t="n">
         <v>2020</v>
       </c>
-      <c r="D12" s="10" t="n">
+      <c r="D12" s="11" t="n">
         <v>4049</v>
       </c>
-      <c r="E12" s="38" t="s">
+      <c r="E12" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="39" t="s">
+      <c r="G12" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="H12" s="39"/>
-      <c r="I12" s="10" t="n">
+      <c r="H12" s="38"/>
+      <c r="I12" s="11" t="n">
         <f aca="false">D12*$Q$3*10^3</f>
         <v>3563120</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J12" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C13" s="1" t="n">
+      <c r="B13" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C13" s="2" t="n">
         <v>2030</v>
       </c>
-      <c r="D13" s="10" t="n">
+      <c r="D13" s="11" t="n">
         <v>3467</v>
       </c>
-      <c r="E13" s="38" t="s">
+      <c r="E13" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="39" t="s">
+      <c r="G13" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="H13" s="39"/>
-      <c r="I13" s="10" t="n">
+      <c r="H13" s="38"/>
+      <c r="I13" s="11" t="n">
         <f aca="false">D13*$Q$3*10^3</f>
         <v>3050960</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="J13" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C14" s="1" t="n">
+      <c r="A14" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="2" t="n">
         <v>2035</v>
       </c>
-      <c r="D14" s="10" t="n">
+      <c r="D14" s="11" t="n">
         <v>6160</v>
       </c>
-      <c r="E14" s="38" t="s">
+      <c r="E14" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="39" t="s">
+      <c r="G14" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="H14" s="53" t="s">
-        <v>102</v>
-      </c>
-      <c r="I14" s="10" t="n">
+      <c r="H14" s="52" t="s">
+        <v>106</v>
+      </c>
+      <c r="I14" s="11" t="n">
         <f aca="false">D14*$Q$3*10^3</f>
         <v>5420800</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="J14" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C15" s="1" t="n">
+      <c r="A15" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="2" t="n">
         <v>2050</v>
       </c>
-      <c r="D15" s="10" t="n">
+      <c r="D15" s="11" t="n">
         <v>5500</v>
       </c>
-      <c r="E15" s="38" t="s">
+      <c r="E15" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="39" t="s">
+      <c r="G15" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="H15" s="53" t="s">
-        <v>102</v>
-      </c>
-      <c r="I15" s="10" t="n">
+      <c r="H15" s="52" t="s">
+        <v>106</v>
+      </c>
+      <c r="I15" s="11" t="n">
         <f aca="false">D15*$Q$3*10^3</f>
         <v>4840000</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="J15" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C16" s="1" t="n">
+      <c r="A16" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" s="2" t="n">
         <v>2035</v>
       </c>
-      <c r="D16" s="10" t="n">
+      <c r="D16" s="11" t="n">
         <v>6820</v>
       </c>
-      <c r="E16" s="38" t="s">
+      <c r="E16" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="39" t="s">
+      <c r="G16" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="H16" s="53" t="s">
-        <v>102</v>
-      </c>
-      <c r="I16" s="10" t="n">
+      <c r="H16" s="52" t="s">
+        <v>106</v>
+      </c>
+      <c r="I16" s="11" t="n">
         <f aca="false">D16*$Q$3*10^3</f>
         <v>6001600</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="J16" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C17" s="1" t="n">
+      <c r="A17" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" s="2" t="n">
         <v>2050</v>
       </c>
-      <c r="D17" s="10" t="n">
+      <c r="D17" s="11" t="n">
         <v>6050</v>
       </c>
-      <c r="E17" s="38" t="s">
+      <c r="E17" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="39" t="s">
+      <c r="G17" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="H17" s="53" t="s">
-        <v>102</v>
-      </c>
-      <c r="I17" s="10" t="n">
+      <c r="H17" s="52" t="s">
+        <v>106</v>
+      </c>
+      <c r="I17" s="11" t="n">
         <f aca="false">D17*$Q$3*10^3</f>
         <v>5324000</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="J17" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="42" t="s">
-        <v>104</v>
-      </c>
-      <c r="B18" s="42"/>
-      <c r="C18" s="42" t="n">
+      <c r="A18" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="B18" s="41"/>
+      <c r="C18" s="41" t="n">
         <v>2025</v>
       </c>
-      <c r="D18" s="47" t="n">
+      <c r="D18" s="46" t="n">
         <v>2274.8177</v>
       </c>
-      <c r="E18" s="44" t="s">
-        <v>105</v>
-      </c>
-      <c r="F18" s="45" t="s">
+      <c r="E18" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="F18" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="46" t="s">
+      <c r="G18" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="H18" s="54"/>
-      <c r="I18" s="47" t="n">
+      <c r="H18" s="53"/>
+      <c r="I18" s="46" t="n">
         <f aca="false">D18*$Q$5*10^3</f>
         <v>2593292.178</v>
       </c>
-      <c r="J18" s="42" t="s">
+      <c r="J18" s="41" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="42" t="s">
-        <v>106</v>
-      </c>
-      <c r="B19" s="42"/>
-      <c r="C19" s="42" t="n">
+      <c r="A19" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41" t="n">
         <v>2025</v>
       </c>
-      <c r="D19" s="47" t="n">
+      <c r="D19" s="46" t="n">
         <v>57074.0625</v>
       </c>
-      <c r="E19" s="44" t="s">
-        <v>107</v>
-      </c>
-      <c r="F19" s="45" t="s">
+      <c r="E19" s="43" t="s">
+        <v>111</v>
+      </c>
+      <c r="F19" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="G19" s="46" t="s">
+      <c r="G19" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="H19" s="54"/>
-      <c r="I19" s="47" t="n">
+      <c r="H19" s="53"/>
+      <c r="I19" s="46" t="n">
         <f aca="false">D19*$Q$4</f>
         <v>60498.50625</v>
       </c>
-      <c r="J19" s="42" t="s">
+      <c r="J19" s="41" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C20" s="1" t="n">
+      <c r="A20" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20" s="2" t="n">
         <v>2020</v>
       </c>
-      <c r="D20" s="10" t="n">
+      <c r="D20" s="11" t="n">
         <v>3075</v>
       </c>
-      <c r="E20" s="38" t="s">
+      <c r="E20" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="39" t="s">
+      <c r="G20" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="H20" s="53"/>
-      <c r="I20" s="10" t="n">
+      <c r="H20" s="52"/>
+      <c r="I20" s="11" t="n">
         <f aca="false">D20*$Q$3*10^3</f>
         <v>2706000</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="J20" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C21" s="1" t="n">
+      <c r="A21" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C21" s="2" t="n">
         <v>2030</v>
       </c>
-      <c r="D21" s="10" t="n">
+      <c r="D21" s="11" t="n">
         <v>2240</v>
       </c>
-      <c r="E21" s="38" t="s">
+      <c r="E21" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G21" s="39" t="s">
+      <c r="G21" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="H21" s="53"/>
-      <c r="I21" s="10" t="n">
+      <c r="H21" s="52"/>
+      <c r="I21" s="11" t="n">
         <f aca="false">D21*$Q$3*10^3</f>
         <v>1971200</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="J21" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="42" t="s">
-        <v>108</v>
-      </c>
-      <c r="B22" s="42"/>
-      <c r="C22" s="42" t="n">
+      <c r="A22" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="B22" s="41"/>
+      <c r="C22" s="41" t="n">
         <v>2025</v>
       </c>
-      <c r="D22" s="47" t="n">
+      <c r="D22" s="46" t="n">
         <v>1989.708</v>
       </c>
-      <c r="E22" s="44" t="s">
-        <v>110</v>
-      </c>
-      <c r="F22" s="45" t="s">
+      <c r="E22" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="F22" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="G22" s="46" t="s">
+      <c r="G22" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="H22" s="54"/>
-      <c r="I22" s="47" t="n">
+      <c r="H22" s="53"/>
+      <c r="I22" s="46" t="n">
         <f aca="false">D22*$Q$4*10^3</f>
         <v>2109090.48</v>
       </c>
-      <c r="J22" s="42" t="s">
+      <c r="J22" s="41" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C23" s="1" t="n">
+      <c r="A23" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C23" s="2" t="n">
         <v>2020</v>
       </c>
-      <c r="D23" s="10" t="n">
+      <c r="D23" s="11" t="n">
         <v>1038</v>
       </c>
-      <c r="E23" s="38" t="s">
+      <c r="E23" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G23" s="39" t="s">
+      <c r="G23" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="H23" s="53"/>
-      <c r="I23" s="10" t="n">
+      <c r="H23" s="52"/>
+      <c r="I23" s="11" t="n">
         <f aca="false">D23*$Q$3*10^3</f>
         <v>913440</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="J23" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C24" s="1" t="n">
+      <c r="A24" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C24" s="2" t="n">
         <v>2030</v>
       </c>
-      <c r="D24" s="10" t="n">
+      <c r="D24" s="11" t="n">
         <v>838</v>
       </c>
-      <c r="E24" s="38" t="s">
+      <c r="E24" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G24" s="39" t="s">
+      <c r="G24" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="H24" s="53"/>
-      <c r="I24" s="10" t="n">
+      <c r="H24" s="52"/>
+      <c r="I24" s="11" t="n">
         <f aca="false">D24*$Q$3*10^3</f>
         <v>737440</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="J24" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="42" t="s">
-        <v>111</v>
-      </c>
-      <c r="B25" s="42" t="s">
-        <v>113</v>
-      </c>
-      <c r="C25" s="42" t="n">
+      <c r="A25" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="B25" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25" s="41" t="n">
         <v>2025</v>
       </c>
-      <c r="D25" s="47" t="n">
+      <c r="D25" s="46" t="n">
         <v>608.4774</v>
       </c>
-      <c r="E25" s="44" t="s">
-        <v>110</v>
-      </c>
-      <c r="F25" s="45" t="s">
+      <c r="E25" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="F25" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="G25" s="46" t="s">
+      <c r="G25" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="H25" s="54"/>
-      <c r="I25" s="47" t="n">
+      <c r="H25" s="53"/>
+      <c r="I25" s="46" t="n">
         <f aca="false">D25*$Q$4*10^3</f>
         <v>644986.044</v>
       </c>
-      <c r="J25" s="42" t="s">
+      <c r="J25" s="41" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="55" t="s">
-        <v>100</v>
-      </c>
-      <c r="B26" s="55" t="s">
-        <v>114</v>
-      </c>
-      <c r="C26" s="55" t="n">
+      <c r="A26" s="54" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="C26" s="54" t="n">
         <v>2025</v>
       </c>
-      <c r="D26" s="56" t="n">
+      <c r="D26" s="55" t="n">
         <v>5350</v>
       </c>
-      <c r="E26" s="57" t="s">
-        <v>115</v>
-      </c>
-      <c r="F26" s="58" t="s">
-        <v>24</v>
-      </c>
-      <c r="G26" s="59" t="s">
-        <v>116</v>
-      </c>
-      <c r="H26" s="60" t="s">
-        <v>117</v>
-      </c>
-      <c r="I26" s="56" t="n">
+      <c r="E26" s="56" t="s">
+        <v>119</v>
+      </c>
+      <c r="F26" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="G26" s="58" t="s">
+        <v>121</v>
+      </c>
+      <c r="H26" s="59" t="s">
+        <v>122</v>
+      </c>
+      <c r="I26" s="55" t="n">
         <f aca="false">D26*$Q$3*10^3*0.67</f>
         <v>3154360</v>
       </c>
-      <c r="J26" s="55" t="s">
+      <c r="J26" s="54" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C27" s="1" t="n">
+      <c r="A27" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C27" s="2" t="n">
         <v>2020</v>
       </c>
-      <c r="D27" s="61" t="n">
+      <c r="D27" s="60" t="n">
         <v>988.321700156956</v>
       </c>
-      <c r="E27" s="38" t="s">
+      <c r="E27" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F27" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G27" s="39" t="s">
+      <c r="G27" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="H27" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="I27" s="10" t="n">
+      <c r="H27" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="I27" s="11" t="n">
         <f aca="false">D27*$Q$3*10^3</f>
         <v>869723.096138121</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="J27" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="R27" s="23"/>
-      <c r="S27" s="2"/>
-      <c r="T27" s="2"/>
+      <c r="R27" s="22"/>
+      <c r="S27" s="3"/>
+      <c r="T27" s="3"/>
     </row>
     <row r="28" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C28" s="1" t="n">
+      <c r="A28" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C28" s="2" t="n">
         <v>2030</v>
       </c>
-      <c r="D28" s="61" t="n">
+      <c r="D28" s="60" t="n">
         <v>681.622479569913</v>
       </c>
-      <c r="E28" s="38" t="s">
+      <c r="E28" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G28" s="39" t="s">
+      <c r="G28" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="H28" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="I28" s="10" t="n">
+      <c r="H28" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="I28" s="11" t="n">
         <f aca="false">D28*$Q$3*10^3</f>
         <v>599827.782021523</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="J28" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="R28" s="23"/>
-      <c r="S28" s="24"/>
-      <c r="T28" s="24"/>
+      <c r="R28" s="22"/>
+      <c r="S28" s="23"/>
+      <c r="T28" s="23"/>
     </row>
     <row r="29" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C29" s="1" t="n">
+      <c r="A29" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C29" s="2" t="n">
         <v>2050</v>
       </c>
-      <c r="D29" s="62" t="n">
+      <c r="D29" s="61" t="n">
         <v>681.622479569913</v>
       </c>
-      <c r="E29" s="38" t="s">
+      <c r="E29" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F29" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G29" s="39" t="s">
+      <c r="G29" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="H29" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="I29" s="10" t="n">
+      <c r="H29" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="I29" s="11" t="n">
         <f aca="false">D29*$Q$3*10^3</f>
         <v>599827.782021523</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="J29" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="R29" s="23"/>
-      <c r="S29" s="34"/>
-      <c r="T29" s="34"/>
+      <c r="R29" s="22"/>
+      <c r="S29" s="33"/>
+      <c r="T29" s="33"/>
     </row>
     <row r="30" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C30" s="1" t="n">
+      <c r="A30" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C30" s="2" t="n">
         <v>2020</v>
       </c>
-      <c r="D30" s="61" t="n">
+      <c r="D30" s="60" t="n">
         <v>1727.23444480956</v>
       </c>
-      <c r="E30" s="38" t="s">
+      <c r="E30" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F30" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G30" s="39" t="s">
+      <c r="G30" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="H30" s="39" t="s">
-        <v>122</v>
-      </c>
-      <c r="I30" s="10" t="n">
+      <c r="H30" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="I30" s="11" t="n">
         <f aca="false">D30*$Q$3*10^3</f>
         <v>1519966.31143242</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="J30" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="S30" s="29"/>
-      <c r="T30" s="13"/>
+      <c r="S30" s="28"/>
+      <c r="T30" s="14"/>
     </row>
     <row r="31" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C31" s="1" t="n">
+      <c r="A31" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C31" s="2" t="n">
         <v>2030</v>
       </c>
-      <c r="D31" s="61" t="n">
+      <c r="D31" s="60" t="n">
         <v>1173.72576283881</v>
       </c>
-      <c r="E31" s="38" t="s">
+      <c r="E31" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G31" s="39" t="s">
+      <c r="G31" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="H31" s="39" t="s">
-        <v>122</v>
-      </c>
-      <c r="I31" s="10" t="n">
+      <c r="H31" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="I31" s="11" t="n">
         <f aca="false">D31*$Q$3*10^3</f>
         <v>1032878.67129815</v>
       </c>
-      <c r="J31" s="1" t="s">
+      <c r="J31" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="S31" s="29"/>
-      <c r="T31" s="13"/>
+      <c r="S31" s="28"/>
+      <c r="T31" s="14"/>
     </row>
     <row r="32" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C32" s="1" t="n">
+      <c r="A32" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C32" s="2" t="n">
         <v>2050</v>
       </c>
-      <c r="D32" s="62" t="n">
+      <c r="D32" s="61" t="n">
         <v>1173.72576283881</v>
       </c>
-      <c r="E32" s="38" t="s">
+      <c r="E32" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G32" s="39" t="s">
+      <c r="G32" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="H32" s="39" t="s">
-        <v>122</v>
-      </c>
-      <c r="I32" s="10" t="n">
+      <c r="H32" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="I32" s="11" t="n">
         <f aca="false">D32*$Q$3*10^3</f>
         <v>1032878.67129815</v>
       </c>
-      <c r="J32" s="1" t="s">
+      <c r="J32" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="42" t="s">
-        <v>118</v>
-      </c>
-      <c r="B33" s="42" t="s">
+      <c r="A33" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="C33" s="42" t="n">
+      <c r="B33" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="C33" s="41" t="n">
         <v>2025</v>
       </c>
-      <c r="D33" s="63" t="n">
+      <c r="D33" s="62" t="n">
         <f aca="false">197.8874*2</f>
         <v>395.7748</v>
       </c>
-      <c r="E33" s="44" t="s">
-        <v>110</v>
-      </c>
-      <c r="F33" s="45" t="s">
+      <c r="E33" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="F33" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="G33" s="46" t="s">
+      <c r="G33" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="H33" s="64" t="s">
-        <v>124</v>
-      </c>
-      <c r="I33" s="47" t="n">
+      <c r="H33" s="63" t="s">
+        <v>129</v>
+      </c>
+      <c r="I33" s="46" t="n">
         <f aca="false">D33*$Q$4*10^3</f>
         <v>419521.288</v>
       </c>
-      <c r="J33" s="42" t="s">
+      <c r="J33" s="41" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="31.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="42" t="s">
-        <v>118</v>
-      </c>
-      <c r="B34" s="42" t="s">
-        <v>125</v>
-      </c>
-      <c r="C34" s="42" t="n">
+      <c r="A34" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="B34" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="C34" s="41" t="n">
         <v>2025</v>
       </c>
-      <c r="D34" s="47" t="n">
+      <c r="D34" s="46" t="n">
         <f aca="false">280.1877*2</f>
         <v>560.3754</v>
       </c>
-      <c r="E34" s="44" t="s">
-        <v>110</v>
-      </c>
-      <c r="F34" s="45" t="s">
+      <c r="E34" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="F34" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="G34" s="46" t="s">
+      <c r="G34" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="H34" s="64" t="s">
-        <v>124</v>
-      </c>
-      <c r="I34" s="47" t="n">
+      <c r="H34" s="63" t="s">
+        <v>129</v>
+      </c>
+      <c r="I34" s="46" t="n">
         <f aca="false">D34*$Q$4*10^3</f>
         <v>593997.924</v>
       </c>
-      <c r="J34" s="42" t="s">
+      <c r="J34" s="41" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C35" s="1" t="n">
+      <c r="A35" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35" s="2" t="n">
         <v>2020</v>
       </c>
-      <c r="D35" s="10" t="n">
+      <c r="D35" s="11" t="n">
         <v>4013</v>
       </c>
-      <c r="E35" s="38" t="s">
-        <v>126</v>
-      </c>
-      <c r="F35" s="2" t="s">
+      <c r="E35" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H35" s="2"/>
+      <c r="I35" s="11" t="n">
+        <f aca="false">D35*Q8*Q7</f>
+        <v>3574.89956331878</v>
+      </c>
+      <c r="J35" s="54" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" s="2" t="n">
+        <v>2024</v>
+      </c>
+      <c r="D36" s="11" t="n">
+        <v>10000</v>
+      </c>
+      <c r="E36" s="37" t="s">
+        <v>133</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2" t="n">
+        <f aca="false">D36*Q6</f>
+        <v>8200</v>
+      </c>
+      <c r="J36" s="54" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C37" s="2"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="44"/>
+      <c r="G37" s="45"/>
+      <c r="H37" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="G35" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="55" t="s">
+      <c r="I37" s="46" t="n">
+        <f aca="false">AVERAGE(I35:I36)</f>
+        <v>5887.44978165939</v>
+      </c>
+      <c r="J37" s="41" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="16.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C36" s="1" t="n">
-        <v>2024</v>
-      </c>
-      <c r="D36" s="10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="E36" s="38" t="s">
-        <v>128</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="55" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="42" t="s">
-        <v>100</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C37" s="1"/>
-      <c r="D37" s="47"/>
-      <c r="E37" s="44"/>
-      <c r="F37" s="45"/>
-      <c r="G37" s="46"/>
-      <c r="H37" s="64" t="s">
-        <v>131</v>
-      </c>
-      <c r="I37" s="47" t="e">
-        <f aca="false">AVERAGE(I35:I36)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J37" s="42" t="s">
-        <v>88</v>
-      </c>
-    </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="38"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="38"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="38"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="38"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4244,64 +4261,67 @@
     <hyperlink ref="R5" r:id="rId9" display="Harmonised Index of Consumer Prices (HICP)"/>
     <hyperlink ref="F6" r:id="rId10" display="TEMOA-Italy"/>
     <hyperlink ref="G6" r:id="rId11" display="Dati elaborati da NREL"/>
-    <hyperlink ref="F7" r:id="rId12" display="TEMOA-Italy"/>
-    <hyperlink ref="G7" r:id="rId13" display="Dati elaborati da NREL"/>
-    <hyperlink ref="F8" r:id="rId14" display="PyPSA/technology-data"/>
-    <hyperlink ref="F9" r:id="rId15" display="TEMOA-Italy"/>
-    <hyperlink ref="G9" r:id="rId16" display="Dati elaborati da NREL"/>
-    <hyperlink ref="F10" r:id="rId17" display="TEMOA-Italy"/>
-    <hyperlink ref="G10" r:id="rId18" display="Dati elaborati da NREL"/>
-    <hyperlink ref="F11" r:id="rId19" display="PyPSA/technology-data"/>
-    <hyperlink ref="F12" r:id="rId20" display="TEMOA-Italy"/>
-    <hyperlink ref="G12" r:id="rId21" display="Dati elaborati da NREL"/>
-    <hyperlink ref="F13" r:id="rId22" display="TEMOA-Italy"/>
-    <hyperlink ref="G13" r:id="rId23" display="Dati elaborati da NREL"/>
-    <hyperlink ref="F14" r:id="rId24" display="TEMOA-Italy"/>
-    <hyperlink ref="G14" r:id="rId25" display="Dati elaborati da NREL"/>
-    <hyperlink ref="F15" r:id="rId26" display="TEMOA-Italy"/>
-    <hyperlink ref="G15" r:id="rId27" display="Dati elaborati da NREL"/>
-    <hyperlink ref="F16" r:id="rId28" display="TEMOA-Italy"/>
-    <hyperlink ref="G16" r:id="rId29" display="Dati elaborati da NREL"/>
-    <hyperlink ref="F17" r:id="rId30" display="TEMOA-Italy"/>
-    <hyperlink ref="G17" r:id="rId31" display="Dati elaborati da NREL"/>
-    <hyperlink ref="F18" r:id="rId32" display="PyPSA/technology-data"/>
-    <hyperlink ref="F19" r:id="rId33" display="PyPSA/technology-data"/>
-    <hyperlink ref="F20" r:id="rId34" display="TEMOA-Italy"/>
-    <hyperlink ref="G20" r:id="rId35" display="Dati elaborati da NREL"/>
-    <hyperlink ref="F21" r:id="rId36" display="TEMOA-Italy"/>
-    <hyperlink ref="G21" r:id="rId37" display="Dati elaborati da NREL"/>
-    <hyperlink ref="F22" r:id="rId38" display="PyPSA/technology-data"/>
-    <hyperlink ref="F23" r:id="rId39" display="TEMOA-Italy"/>
-    <hyperlink ref="G23" r:id="rId40" display="Dati elaborati da NREL"/>
-    <hyperlink ref="F24" r:id="rId41" display="TEMOA-Italy"/>
-    <hyperlink ref="G24" r:id="rId42" display="Dati elaborati da NREL"/>
-    <hyperlink ref="F25" r:id="rId43" display="PyPSA/technology-data"/>
-    <hyperlink ref="F26" r:id="rId44" display="IAEA"/>
-    <hyperlink ref="H26" r:id="rId45" display="Overnight cost suggerito da Lorenzo Mazzocco, portato dal 2020 al 2025 tramite inflazione di circa il 33% (vedi messaggio discord su Coordinamento energia)"/>
-    <hyperlink ref="F27" r:id="rId46" display="TEMOA-Italy"/>
-    <hyperlink ref="G27" r:id="rId47" display="Dati elaborati da NREL"/>
-    <hyperlink ref="H27" r:id="rId48" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 2 ore. Per ulteriori info, vedere questo paper"/>
-    <hyperlink ref="F28" r:id="rId49" display="TEMOA-Italy"/>
-    <hyperlink ref="G28" r:id="rId50" display="Dati elaborati da NREL"/>
-    <hyperlink ref="H28" r:id="rId51" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 2 ore. Per ulteriori info, vedere questo paper"/>
-    <hyperlink ref="F29" r:id="rId52" display="TEMOA-Italy"/>
-    <hyperlink ref="G29" r:id="rId53" display="Dati elaborati da NREL"/>
-    <hyperlink ref="H29" r:id="rId54" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 2 ore. Per ulteriori info, vedere questo paper"/>
-    <hyperlink ref="F30" r:id="rId55" display="TEMOA-Italy"/>
-    <hyperlink ref="G30" r:id="rId56" display="Dati elaborati da NREL"/>
-    <hyperlink ref="H30" r:id="rId57" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 4 ore. Per ulteriori info, vedere questo paper"/>
-    <hyperlink ref="F31" r:id="rId58" display="TEMOA-Italy"/>
-    <hyperlink ref="G31" r:id="rId59" display="Dati elaborati da NREL"/>
-    <hyperlink ref="H31" r:id="rId60" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 4 ore. Per ulteriori info, vedere questo paper"/>
-    <hyperlink ref="F32" r:id="rId61" display="TEMOA-Italy"/>
-    <hyperlink ref="G32" r:id="rId62" display="Dati elaborati da NREL"/>
-    <hyperlink ref="H32" r:id="rId63" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 4 ore. Per ulteriori info, vedere questo paper"/>
-    <hyperlink ref="F33" r:id="rId64" display="PyPSA/technology-data"/>
-    <hyperlink ref="H33" r:id="rId65" display="Durata dovrebbe essere di 2 h"/>
-    <hyperlink ref="F34" r:id="rId66" display="PyPSA/technology-data"/>
-    <hyperlink ref="H34" r:id="rId67" display="Durata dovrebbe essere di 2 h"/>
-    <hyperlink ref="F35" r:id="rId68" display="IAEA"/>
-    <hyperlink ref="F36" r:id="rId69" display="S&amp;P"/>
+    <hyperlink ref="R6" r:id="rId12" display="Harmonised Index of Consumer Prices (HICP)"/>
+    <hyperlink ref="F7" r:id="rId13" display="TEMOA-Italy"/>
+    <hyperlink ref="G7" r:id="rId14" display="Dati elaborati da NREL"/>
+    <hyperlink ref="R7" r:id="rId15" display="Harmonised Index of Consumer Prices (HICP)"/>
+    <hyperlink ref="F8" r:id="rId16" display="PyPSA/technology-data"/>
+    <hyperlink ref="R8" r:id="rId17" display="Banca d’Italia"/>
+    <hyperlink ref="F9" r:id="rId18" display="TEMOA-Italy"/>
+    <hyperlink ref="G9" r:id="rId19" display="Dati elaborati da NREL"/>
+    <hyperlink ref="F10" r:id="rId20" display="TEMOA-Italy"/>
+    <hyperlink ref="G10" r:id="rId21" display="Dati elaborati da NREL"/>
+    <hyperlink ref="F11" r:id="rId22" display="PyPSA/technology-data"/>
+    <hyperlink ref="F12" r:id="rId23" display="TEMOA-Italy"/>
+    <hyperlink ref="G12" r:id="rId24" display="Dati elaborati da NREL"/>
+    <hyperlink ref="F13" r:id="rId25" display="TEMOA-Italy"/>
+    <hyperlink ref="G13" r:id="rId26" display="Dati elaborati da NREL"/>
+    <hyperlink ref="F14" r:id="rId27" display="TEMOA-Italy"/>
+    <hyperlink ref="G14" r:id="rId28" display="Dati elaborati da NREL"/>
+    <hyperlink ref="F15" r:id="rId29" display="TEMOA-Italy"/>
+    <hyperlink ref="G15" r:id="rId30" display="Dati elaborati da NREL"/>
+    <hyperlink ref="F16" r:id="rId31" display="TEMOA-Italy"/>
+    <hyperlink ref="G16" r:id="rId32" display="Dati elaborati da NREL"/>
+    <hyperlink ref="F17" r:id="rId33" display="TEMOA-Italy"/>
+    <hyperlink ref="G17" r:id="rId34" display="Dati elaborati da NREL"/>
+    <hyperlink ref="F18" r:id="rId35" display="PyPSA/technology-data"/>
+    <hyperlink ref="F19" r:id="rId36" display="PyPSA/technology-data"/>
+    <hyperlink ref="F20" r:id="rId37" display="TEMOA-Italy"/>
+    <hyperlink ref="G20" r:id="rId38" display="Dati elaborati da NREL"/>
+    <hyperlink ref="F21" r:id="rId39" display="TEMOA-Italy"/>
+    <hyperlink ref="G21" r:id="rId40" display="Dati elaborati da NREL"/>
+    <hyperlink ref="F22" r:id="rId41" display="PyPSA/technology-data"/>
+    <hyperlink ref="F23" r:id="rId42" display="TEMOA-Italy"/>
+    <hyperlink ref="G23" r:id="rId43" display="Dati elaborati da NREL"/>
+    <hyperlink ref="F24" r:id="rId44" display="TEMOA-Italy"/>
+    <hyperlink ref="G24" r:id="rId45" display="Dati elaborati da NREL"/>
+    <hyperlink ref="F25" r:id="rId46" display="PyPSA/technology-data"/>
+    <hyperlink ref="F26" r:id="rId47" display="IAEA"/>
+    <hyperlink ref="H26" r:id="rId48" display="Overnight cost suggerito da Lorenzo Mazzocco, portato dal 2020 al 2025 tramite inflazione di circa il 33% (vedi messaggio discord su Coordinamento energia)"/>
+    <hyperlink ref="F27" r:id="rId49" display="TEMOA-Italy"/>
+    <hyperlink ref="G27" r:id="rId50" display="Dati elaborati da NREL"/>
+    <hyperlink ref="H27" r:id="rId51" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 2 ore. Per ulteriori info, vedere questo paper"/>
+    <hyperlink ref="F28" r:id="rId52" display="TEMOA-Italy"/>
+    <hyperlink ref="G28" r:id="rId53" display="Dati elaborati da NREL"/>
+    <hyperlink ref="H28" r:id="rId54" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 2 ore. Per ulteriori info, vedere questo paper"/>
+    <hyperlink ref="F29" r:id="rId55" display="TEMOA-Italy"/>
+    <hyperlink ref="G29" r:id="rId56" display="Dati elaborati da NREL"/>
+    <hyperlink ref="H29" r:id="rId57" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 2 ore. Per ulteriori info, vedere questo paper"/>
+    <hyperlink ref="F30" r:id="rId58" display="TEMOA-Italy"/>
+    <hyperlink ref="G30" r:id="rId59" display="Dati elaborati da NREL"/>
+    <hyperlink ref="H30" r:id="rId60" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 4 ore. Per ulteriori info, vedere questo paper"/>
+    <hyperlink ref="F31" r:id="rId61" display="TEMOA-Italy"/>
+    <hyperlink ref="G31" r:id="rId62" display="Dati elaborati da NREL"/>
+    <hyperlink ref="H31" r:id="rId63" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 4 ore. Per ulteriori info, vedere questo paper"/>
+    <hyperlink ref="F32" r:id="rId64" display="TEMOA-Italy"/>
+    <hyperlink ref="G32" r:id="rId65" display="Dati elaborati da NREL"/>
+    <hyperlink ref="H32" r:id="rId66" display="Due componenti di costo considerate: power capital cost (€/MW) e energy capital cost (€/MWh). Quest'ultimo moltiplicato per uno &quot;storage duration&quot; di 4 ore. Per ulteriori info, vedere questo paper"/>
+    <hyperlink ref="F33" r:id="rId67" display="PyPSA/technology-data"/>
+    <hyperlink ref="H33" r:id="rId68" display="Durata dovrebbe essere di 2 h"/>
+    <hyperlink ref="F34" r:id="rId69" display="PyPSA/technology-data"/>
+    <hyperlink ref="H34" r:id="rId70" display="Durata dovrebbe essere di 2 h"/>
+    <hyperlink ref="F35" r:id="rId71" display="IAEA"/>
+    <hyperlink ref="F36" r:id="rId72" display="S&amp;P"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -4326,128 +4346,128 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="F1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>138</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <f aca="false">discount_rate!B2</f>
         <v>0.057</v>
       </c>
-      <c r="C2" s="13" t="n">
+      <c r="C2" s="14" t="n">
         <f aca="false">CAPEX!B2</f>
         <v>676570.3</v>
       </c>
-      <c r="D2" s="18" t="n">
+      <c r="D2" s="19" t="n">
         <f aca="false">OPEX!B2</f>
         <v>0.017275</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <v>0.15</v>
       </c>
-      <c r="G2" s="4" t="n">
+      <c r="G2" s="5" t="n">
         <f aca="false">PMT(B2,E2,-1)</f>
         <v>0.0850733064256807</v>
       </c>
-      <c r="H2" s="18" t="n">
+      <c r="H2" s="19" t="n">
         <f aca="false">C2*(D2+G2)/(8760*F2*1)</f>
         <v>52.6984964862364</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <f aca="false">discount_rate!B3</f>
         <v>0.076</v>
       </c>
-      <c r="C3" s="13" t="n">
+      <c r="C3" s="14" t="n">
         <f aca="false">CAPEX!B3/1.5</f>
         <v>1208275.556</v>
       </c>
-      <c r="D3" s="18" t="n">
+      <c r="D3" s="19" t="n">
         <f aca="false">OPEX!B3</f>
         <v>0.012347</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>0.25</v>
       </c>
-      <c r="G3" s="4" t="n">
+      <c r="G3" s="5" t="n">
         <f aca="false">PMT(B3,E3,-1)</f>
         <v>0.0904989581478276</v>
       </c>
-      <c r="H3" s="18" t="n">
+      <c r="H3" s="19" t="n">
         <f aca="false">C3*(D3+G3)/(8760*F3*1)</f>
         <v>56.7425832253055</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="18" t="n">
+      <c r="B4" s="19" t="n">
         <f aca="false">discount_rate!B4</f>
         <v>0.045</v>
       </c>
-      <c r="C4" s="13" t="n">
+      <c r="C4" s="14" t="n">
         <f aca="false">CAPEX!B4</f>
-        <v>7500000</v>
-      </c>
-      <c r="D4" s="18" t="n">
+        <v>5887449.78165939</v>
+      </c>
+      <c r="D4" s="19" t="n">
         <f aca="false">OPEX!B4</f>
         <v>0.033</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="1" t="n">
         <v>0.85</v>
       </c>
-      <c r="G4" s="4" t="n">
+      <c r="G4" s="5" t="n">
         <f aca="false">PMT(B4,E4,-1)</f>
         <v>0.0484542558462612</v>
       </c>
-      <c r="H4" s="18" t="n">
+      <c r="H4" s="19" t="n">
         <f aca="false">C4*(D4+G4)/(8760*F4*1)</f>
-        <v>82.0449797001019</v>
+        <v>64.4047597095486</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added long duration energy storage through LiquidAirStorage
</commit_message>
<xml_diff>
--- a/dati_casoStudioItalia/altri_dati.xlsx
+++ b/dati_casoStudioItalia/altri_dati.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0954659\PycharmProjects\DrinDrin---Mix-energetico\dati_casoStudioItalia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A2CD15-513F-45E2-99AE-BBB522DB3291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B705C48-62F7-4342-B766-48F7B7607B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="discount_rate" sheetId="1" r:id="rId1"/>
@@ -271,7 +271,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="162">
   <si>
     <t>discount_rate</t>
   </si>
@@ -727,6 +727,36 @@
   </si>
   <si>
     <t>tunisia</t>
+  </si>
+  <si>
+    <t>LiquidAirStorage</t>
+  </si>
+  <si>
+    <t>Capex power LDES</t>
+  </si>
+  <si>
+    <t>Capex energy LDES</t>
+  </si>
+  <si>
+    <t>EU</t>
+  </si>
+  <si>
+    <t>EUR2022/MW</t>
+  </si>
+  <si>
+    <t>EUR2022/MWh</t>
+  </si>
+  <si>
+    <t>(€2025/MW)</t>
+  </si>
+  <si>
+    <t>(€2025/MWh)</t>
+  </si>
+  <si>
+    <t>2025,data for capex_power to be input manually in json using values from the sheet "raw_data_techs"</t>
+  </si>
+  <si>
+    <t>no source, just put the same as Li-ion</t>
   </si>
 </sst>
 </file>
@@ -739,7 +769,7 @@
     <numFmt numFmtId="166" formatCode="\€#,##0.00_);[Red]&quot;(€&quot;#,##0.00\)"/>
     <numFmt numFmtId="167" formatCode="0.0E+00"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -908,6 +938,18 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -943,7 +985,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
@@ -1120,6 +1162,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1385,8 +1432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1542,6 +1589,20 @@
       </c>
       <c r="E9" s="4" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B10" s="65">
+        <v>0.08</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="68" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.3">
@@ -1569,10 +1630,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1736,6 +1797,20 @@
         <v>2025</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="67" t="s">
+        <v>155</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
@@ -1744,6 +1819,7 @@
     <hyperlink ref="D7" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
     <hyperlink ref="D8" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
     <hyperlink ref="D9" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="D10" r:id="rId7" xr:uid="{E8CA2C79-76F6-4A5E-9BE6-E6C3A5138E15}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1755,13 +1831,13 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A10" sqref="A10:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="55.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.44140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="19.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="35.6640625" style="1" customWidth="1"/>
@@ -1962,6 +2038,23 @@
         <v>60498.506249999999</v>
       </c>
     </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B10" s="1">
+        <v>499500.00000000006</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="67" t="s">
+        <v>155</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>160</v>
+      </c>
+    </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E18" s="16"/>
     </row>
@@ -1975,10 +2068,11 @@
     <hyperlink ref="D7" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
     <hyperlink ref="D8" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
     <hyperlink ref="D9" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="D10" r:id="rId9" xr:uid="{07254F85-3A08-4573-A953-D92D99343ED3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <legacyDrawing r:id="rId9"/>
+  <legacyDrawing r:id="rId10"/>
 </worksheet>
 </file>
 
@@ -2078,7 +2172,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -2879,13 +2973,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:T41"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView topLeftCell="B31" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="1" customWidth="1"/>
     <col min="4" max="4" width="14.44140625" style="1" customWidth="1"/>
@@ -4167,28 +4261,62 @@
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" s="40"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="45"/>
-      <c r="E38" s="42"/>
-      <c r="F38" s="43"/>
+      <c r="A38" s="66" t="s">
+        <v>153</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C38" s="2">
+        <v>2030</v>
+      </c>
+      <c r="D38" s="45">
+        <v>2000000</v>
+      </c>
+      <c r="E38" s="42" t="s">
+        <v>156</v>
+      </c>
+      <c r="F38" s="67" t="s">
+        <v>155</v>
+      </c>
       <c r="G38" s="44"/>
       <c r="H38" s="62"/>
-      <c r="I38" s="45"/>
-      <c r="J38" s="40"/>
+      <c r="I38" s="45">
+        <f>D38*1.11</f>
+        <v>2220000</v>
+      </c>
+      <c r="J38" s="53" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="2"/>
+      <c r="A39" s="66" t="s">
+        <v>154</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C39" s="2">
+        <v>2030</v>
+      </c>
+      <c r="D39" s="15">
+        <v>450000</v>
+      </c>
+      <c r="E39" s="36" t="s">
+        <v>157</v>
+      </c>
+      <c r="F39" s="67" t="s">
+        <v>155</v>
+      </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
+      <c r="I39" s="45">
+        <f>D39*1.11</f>
+        <v>499500.00000000006</v>
+      </c>
+      <c r="J39" s="53" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
@@ -4291,6 +4419,8 @@
     <hyperlink ref="F35" r:id="rId73" xr:uid="{00000000-0004-0000-0600-000048000000}"/>
     <hyperlink ref="F36" r:id="rId74" xr:uid="{00000000-0004-0000-0600-000049000000}"/>
     <hyperlink ref="F37" r:id="rId75" xr:uid="{00000000-0004-0000-0600-00004A000000}"/>
+    <hyperlink ref="F38" r:id="rId76" xr:uid="{923873DF-CEAE-4A3A-9AFA-1A1D1F42FD8C}"/>
+    <hyperlink ref="F39" r:id="rId77" xr:uid="{0456D716-3B3A-4889-9BAA-6D8482BC5B9F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Fixed bug export price
</commit_message>
<xml_diff>
--- a/dati_casoStudioItalia/altri_dati.xlsx
+++ b/dati_casoStudioItalia/altri_dati.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0954659\PycharmProjects\DrinDrin---Mix-energetico\dati_casoStudioItalia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A494A9B9-15E1-4563-8B78-84DC7EB0D91B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B8D09E-1EBA-409F-97DC-235D3ADBB4AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="699" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="699" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="discount_rate" sheetId="1" r:id="rId1"/>
@@ -271,7 +271,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="169">
   <si>
     <t>discount_rate</t>
   </si>
@@ -384,9 +384,6 @@
     <t>capacity</t>
   </si>
   <si>
-    <t>price</t>
-  </si>
-  <si>
     <t>emission_factor_t/MWh</t>
   </si>
   <si>
@@ -775,6 +772,12 @@
   </si>
   <si>
     <t>Capex per underground reservoir</t>
+  </si>
+  <si>
+    <t>import_price</t>
+  </si>
+  <si>
+    <t>export_price</t>
   </si>
 </sst>
 </file>
@@ -1595,7 +1598,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B9" s="2">
         <v>5.1999999999999998E-2</v>
@@ -1612,7 +1615,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B10" s="65">
         <v>0.08</v>
@@ -1621,7 +1624,7 @@
         <v>5</v>
       </c>
       <c r="D10" s="68" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.3">
@@ -1800,7 +1803,7 @@
     </row>
     <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B9" s="6">
         <f>0.43/100</f>
@@ -1818,7 +1821,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B10" s="1">
         <v>4.2999999999999997E-2</v>
@@ -1827,7 +1830,7 @@
         <v>5</v>
       </c>
       <c r="D10" s="69" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -1849,7 +1852,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -1878,10 +1881,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1982,7 +1985,7 @@
         <v>5137.2665966719487</v>
       </c>
       <c r="C6" s="65" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>15</v>
@@ -2038,7 +2041,7 @@
     </row>
     <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B9" s="11">
         <f t="shared" si="0"/>
@@ -2059,7 +2062,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B10" s="1">
         <f>raw_data_techs!I41</f>
@@ -2069,10 +2072,10 @@
         <v>25</v>
       </c>
       <c r="D10" s="69" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.3">
@@ -2190,61 +2193,68 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.44140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="35.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="35.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
         <v>38</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
-        <v>39</v>
       </c>
       <c r="B2" s="2">
         <v>10138</v>
       </c>
       <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
         <v>100</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>0</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
-        <v>42</v>
       </c>
       <c r="B3" s="2">
         <v>0</v>
@@ -2253,13 +2263,16 @@
         <v>0</v>
       </c>
       <c r="D3" s="2">
+        <v>100</v>
+      </c>
+      <c r="E3" s="2">
         <v>0</v>
       </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="2">
         <v>0</v>
@@ -2268,13 +2281,16 @@
         <v>0</v>
       </c>
       <c r="D4" s="2">
+        <v>100</v>
+      </c>
+      <c r="E4" s="2">
         <v>0</v>
       </c>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="2">
         <v>600</v>
@@ -2283,35 +2299,41 @@
         <v>0</v>
       </c>
       <c r="D5" s="2">
+        <v>100</v>
+      </c>
+      <c r="E5" s="2">
         <v>0</v>
       </c>
-      <c r="F5" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="2">
         <v>500</v>
       </c>
       <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
         <v>100</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>0</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="20" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="20" t="s">
-        <v>47</v>
       </c>
       <c r="B7" s="2">
         <v>0</v>
@@ -2320,15 +2342,18 @@
         <v>0</v>
       </c>
       <c r="D7" s="2">
+        <v>100</v>
+      </c>
+      <c r="E7" s="2">
         <v>0</v>
       </c>
-      <c r="F7" s="18" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" s="18" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" s="2">
         <v>600</v>
@@ -2337,6 +2362,9 @@
         <v>0</v>
       </c>
       <c r="D8" s="2">
+        <v>100</v>
+      </c>
+      <c r="E8" s="2">
         <v>0</v>
       </c>
     </row>
@@ -2373,35 +2401,35 @@
   <sheetData>
     <row r="1" spans="1:25" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="C1" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="D1" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="F1" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="G1" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="H1" s="22" t="s">
         <v>55</v>
-      </c>
-      <c r="H1" s="22" t="s">
-        <v>56</v>
       </c>
       <c r="J1" s="21"/>
       <c r="K1" s="21"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" s="23">
         <v>2018</v>
@@ -2410,36 +2438,36 @@
         <v>7.5414094383199997</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>30</v>
       </c>
       <c r="F2" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G2" s="27">
         <f t="shared" ref="G2:G8" si="0">C2*$M$3/$M$4</f>
         <v>21.805545521741941</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J2" s="21"/>
       <c r="K2" s="21"/>
       <c r="L2" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="M2" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="M2" s="21" t="s">
-        <v>62</v>
-      </c>
       <c r="N2" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" s="23">
         <v>2019</v>
@@ -2448,38 +2476,38 @@
         <v>4.8274540271299999</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E3" s="17" t="s">
         <v>30</v>
       </c>
       <c r="F3" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G3" s="27">
         <f t="shared" si="0"/>
         <v>13.958301747657082</v>
       </c>
       <c r="H3" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M3" s="29">
         <v>0.85</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W3" s="21"/>
       <c r="Y3" s="3"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="23">
         <v>2020</v>
@@ -2488,23 +2516,23 @@
         <v>3.31156694524004</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E4" s="17" t="s">
         <v>30</v>
       </c>
       <c r="F4" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G4" s="27">
         <f t="shared" si="0"/>
         <v>9.575202667793878</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L4" s="28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M4" s="30">
         <v>0.29397099999999998</v>
@@ -2515,7 +2543,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="23">
         <v>2021</v>
@@ -2524,23 +2552,23 @@
         <v>14.731149861407699</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E5" s="17" t="s">
         <v>30</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G5" s="27">
         <f t="shared" si="0"/>
         <v>42.594260597802318</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L5" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M5" s="31">
         <f>1.622*10^-6</f>
@@ -2551,7 +2579,7 @@
     </row>
     <row r="6" spans="1:25" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B6" s="23">
         <v>2022</v>
@@ -2560,23 +2588,23 @@
         <v>34.346664233460999</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>30</v>
       </c>
       <c r="F6" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G6" s="27">
         <f t="shared" si="0"/>
         <v>99.311376286918943</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L6" s="33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M6" s="29">
         <v>6000</v>
@@ -2588,7 +2616,7 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" s="23">
         <v>2023</v>
@@ -2597,35 +2625,35 @@
         <v>11.4929038091148</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E7" s="17" t="s">
         <v>30</v>
       </c>
       <c r="F7" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G7" s="27">
         <f t="shared" si="0"/>
         <v>33.231061015364034</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L7" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M7" s="29">
         <v>0.82</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Y7" s="13"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="23">
         <v>2024</v>
@@ -2634,35 +2662,35 @@
         <v>9.52416119251955</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E8" s="17" t="s">
         <v>30</v>
       </c>
       <c r="F8" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G8" s="27">
         <f t="shared" si="0"/>
         <v>27.538556570687646</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L8" s="28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M8" s="29">
         <v>0.88</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Y8" s="13"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B9" s="23">
         <v>2018</v>
@@ -2671,27 +2699,27 @@
         <v>105.06823090515999</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E9" s="17" t="s">
         <v>30</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G9" s="27">
         <f t="shared" ref="G9:G15" si="1">C9*$M$3/$M$6/$M$5/1000</f>
         <v>9.1767361559171796</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M9" s="34"/>
       <c r="Y9" s="13"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10" s="23">
         <v>2019</v>
@@ -2700,27 +2728,27 @@
         <v>78.292956708220004</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E10" s="17" t="s">
         <v>30</v>
       </c>
       <c r="F10" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G10" s="27">
         <f t="shared" si="1"/>
         <v>6.8381641185765512</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M10" s="34"/>
       <c r="Y10" s="13"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B11" s="23">
         <v>2020</v>
@@ -2729,27 +2757,27 @@
         <v>62.088866189989801</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E11" s="17" t="s">
         <v>30</v>
       </c>
       <c r="F11" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G11" s="27">
         <f t="shared" si="1"/>
         <v>5.4228869976871481</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M11" s="34"/>
       <c r="Y11" s="13"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B12" s="23">
         <v>2021</v>
@@ -2758,27 +2786,27 @@
         <v>126.188299817185</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E12" s="17" t="s">
         <v>30</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G12" s="27">
         <f t="shared" si="1"/>
         <v>11.021378426285166</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M12" s="34"/>
       <c r="Y12" s="13"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B13" s="23">
         <v>2022</v>
@@ -2787,27 +2815,27 @@
         <v>293.65119909180902</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E13" s="17" t="s">
         <v>30</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G13" s="27">
         <f t="shared" si="1"/>
         <v>25.64771056597181</v>
       </c>
       <c r="H13" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M13" s="34"/>
       <c r="Y13" s="13"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B14" s="23">
         <v>2023</v>
@@ -2816,27 +2844,27 @@
         <v>151.42784107508299</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E14" s="17" t="s">
         <v>30</v>
       </c>
       <c r="F14" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G14" s="27">
         <f t="shared" si="1"/>
         <v>13.22581842517679</v>
       </c>
       <c r="H14" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M14" s="34"/>
       <c r="Y14" s="13"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B15" s="23">
         <v>2024</v>
@@ -2845,27 +2873,27 @@
         <v>118.28554879814899</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E15" s="17" t="s">
         <v>30</v>
       </c>
       <c r="F15" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G15" s="27">
         <f t="shared" si="1"/>
         <v>10.331146370574048</v>
       </c>
       <c r="H15" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M15" s="34"/>
       <c r="Y15" s="13"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B16" s="23">
         <v>2021</v>
@@ -2874,50 +2902,50 @@
         <v>0.46</v>
       </c>
       <c r="D16" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="17" t="s">
         <v>74</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>75</v>
       </c>
       <c r="G16" s="27">
         <f>C16*M7/100*1000</f>
         <v>3.7719999999999998</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M16" s="34"/>
       <c r="Y16" s="22"/>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B17" s="35" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C17" s="24">
         <v>7</v>
       </c>
       <c r="D17" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="17" t="s">
         <v>77</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>78</v>
       </c>
       <c r="G17" s="27">
         <f>C17*M7</f>
         <v>5.7399999999999993</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M17" s="34"/>
       <c r="Y17" s="32"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B18" s="23">
         <v>2021</v>
@@ -2926,17 +2954,17 @@
         <v>0.61</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G18" s="27">
         <f>C18*M7/100*1000</f>
         <v>5.0019999999999998</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M18" s="34"/>
       <c r="Y18" s="27"/>
@@ -3016,42 +3044,42 @@
   <sheetData>
     <row r="1" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="D1" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" s="21" t="s">
+      <c r="H1" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="H1" s="21" t="s">
-        <v>82</v>
-      </c>
       <c r="I1" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="22" t="s">
         <v>55</v>
-      </c>
-      <c r="J1" s="22" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="C2" s="2">
         <v>2020</v>
@@ -3060,13 +3088,13 @@
         <v>1333</v>
       </c>
       <c r="E2" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H2" s="37"/>
       <c r="I2" s="11">
@@ -3074,24 +3102,24 @@
         <v>1173040</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P2" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q2" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="Q2" s="21" t="s">
-        <v>62</v>
-      </c>
       <c r="R2" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="C3" s="2">
         <v>2030</v>
@@ -3100,13 +3128,13 @@
         <v>754</v>
       </c>
       <c r="E3" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G3" s="37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H3" s="37"/>
       <c r="I3" s="11">
@@ -3114,24 +3142,24 @@
         <v>663520</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P3" s="28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q3" s="29">
         <v>0.88</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="40" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C4" s="40">
         <v>2025</v>
@@ -3140,40 +3168,40 @@
         <v>676.57029999999997</v>
       </c>
       <c r="E4" s="42" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F4" s="43" t="s">
         <v>15</v>
       </c>
       <c r="G4" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="H4" s="44" t="s">
         <v>89</v>
-      </c>
-      <c r="H4" s="44" t="s">
-        <v>90</v>
       </c>
       <c r="I4" s="45">
         <f>D4*10^3</f>
         <v>676570.29999999993</v>
       </c>
       <c r="J4" s="40" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P4" s="28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q4" s="29">
         <v>1.06</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C5" s="2">
         <v>2025</v>
@@ -3182,13 +3210,13 @@
         <v>473.11559999999997</v>
       </c>
       <c r="E5" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G5" s="44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H5" s="37"/>
       <c r="I5" s="11">
@@ -3196,24 +3224,24 @@
         <v>473115.6</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P5" s="28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q5" s="29">
         <v>1.1399999999999999</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="C6" s="2">
         <v>2020</v>
@@ -3222,13 +3250,13 @@
         <v>1462</v>
       </c>
       <c r="E6" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G6" s="37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H6" s="37"/>
       <c r="I6" s="11">
@@ -3236,24 +3264,24 @@
         <v>1286560</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P6" s="28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q6" s="29">
         <v>0.82</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="C7" s="2">
         <v>2030</v>
@@ -3262,13 +3290,13 @@
         <v>956</v>
       </c>
       <c r="E7" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G7" s="37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="11">
@@ -3276,24 +3304,24 @@
         <v>841280</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P7" s="28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q7" s="29">
         <v>1.02</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="23.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="40" t="s">
         <v>94</v>
-      </c>
-      <c r="B8" s="40" t="s">
-        <v>95</v>
       </c>
       <c r="C8" s="40">
         <v>2025</v>
@@ -3302,13 +3330,13 @@
         <v>1139.8825999999999</v>
       </c>
       <c r="E8" s="42" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F8" s="43" t="s">
         <v>15</v>
       </c>
       <c r="G8" s="44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H8" s="46"/>
       <c r="I8" s="45">
@@ -3316,25 +3344,25 @@
         <v>1208275.5560000001</v>
       </c>
       <c r="J8" s="40" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P8" s="28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Q8" s="30">
         <f>1/1.145</f>
         <v>0.8733624454148472</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C9" s="2">
         <v>2020</v>
@@ -3343,13 +3371,13 @@
         <v>3739</v>
       </c>
       <c r="E9" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G9" s="37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H9" s="37"/>
       <c r="I9" s="11">
@@ -3357,25 +3385,25 @@
         <v>3290320</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P9" s="28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q9" s="5">
         <f>1/1.0541</f>
         <v>0.94867659614837296</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C10" s="2">
         <v>2030</v>
@@ -3384,13 +3412,13 @@
         <v>2758</v>
       </c>
       <c r="E10" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G10" s="37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H10" s="37"/>
       <c r="I10" s="11">
@@ -3398,24 +3426,24 @@
         <v>2427040</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P10" s="28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q10" s="1">
         <v>1.06</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C11" s="14">
         <v>2025</v>
@@ -3424,13 +3452,13 @@
         <v>1769.1170999999999</v>
       </c>
       <c r="E11" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F11" s="48" t="s">
         <v>15</v>
       </c>
       <c r="G11" s="49" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H11" s="50"/>
       <c r="I11" s="11">
@@ -3438,15 +3466,15 @@
         <v>1769117.0999999999</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C12" s="2">
         <v>2020</v>
@@ -3455,13 +3483,13 @@
         <v>4049</v>
       </c>
       <c r="E12" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G12" s="37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H12" s="37"/>
       <c r="I12" s="11">
@@ -3469,15 +3497,15 @@
         <v>3563120</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C13" s="2">
         <v>2030</v>
@@ -3486,13 +3514,13 @@
         <v>3467</v>
       </c>
       <c r="E13" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G13" s="37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H13" s="37"/>
       <c r="I13" s="11">
@@ -3500,15 +3528,15 @@
         <v>3050960</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="C14" s="2">
         <v>2035</v>
@@ -3517,31 +3545,31 @@
         <v>6160</v>
       </c>
       <c r="E14" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G14" s="37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H14" s="51" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I14" s="11">
         <f t="shared" si="0"/>
         <v>5420800</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="C15" s="2">
         <v>2050</v>
@@ -3550,31 +3578,31 @@
         <v>5500</v>
       </c>
       <c r="E15" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G15" s="37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H15" s="51" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I15" s="11">
         <f t="shared" si="0"/>
         <v>4840000</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C16" s="2">
         <v>2035</v>
@@ -3583,31 +3611,31 @@
         <v>6820</v>
       </c>
       <c r="E16" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G16" s="37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H16" s="51" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I16" s="11">
         <f t="shared" si="0"/>
         <v>6001600</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C17" s="2">
         <v>2050</v>
@@ -3616,28 +3644,28 @@
         <v>6050</v>
       </c>
       <c r="E17" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G17" s="37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H17" s="51" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I17" s="11">
         <f t="shared" si="0"/>
         <v>5324000</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="40" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B18" s="40"/>
       <c r="C18" s="40">
@@ -3647,13 +3675,13 @@
         <v>2274.8177000000001</v>
       </c>
       <c r="E18" s="42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F18" s="43" t="s">
         <v>15</v>
       </c>
       <c r="G18" s="44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H18" s="52"/>
       <c r="I18" s="45">
@@ -3661,12 +3689,12 @@
         <v>2593292.1779999998</v>
       </c>
       <c r="J18" s="40" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="40" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B19" s="40"/>
       <c r="C19" s="40">
@@ -3676,13 +3704,13 @@
         <v>57074.0625</v>
       </c>
       <c r="E19" s="42" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F19" s="43" t="s">
         <v>15</v>
       </c>
       <c r="G19" s="44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H19" s="52"/>
       <c r="I19" s="45">
@@ -3690,15 +3718,15 @@
         <v>60498.506250000006</v>
       </c>
       <c r="J19" s="40" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="C20" s="2">
         <v>2020</v>
@@ -3707,13 +3735,13 @@
         <v>3075</v>
       </c>
       <c r="E20" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G20" s="37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H20" s="51"/>
       <c r="I20" s="11">
@@ -3721,15 +3749,15 @@
         <v>2706000</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="C21" s="2">
         <v>2030</v>
@@ -3738,13 +3766,13 @@
         <v>2240</v>
       </c>
       <c r="E21" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G21" s="37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H21" s="51"/>
       <c r="I21" s="11">
@@ -3752,12 +3780,12 @@
         <v>1971200</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="40" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B22" s="40"/>
       <c r="C22" s="40">
@@ -3767,13 +3795,13 @@
         <v>1989.7080000000001</v>
       </c>
       <c r="E22" s="42" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F22" s="43" t="s">
         <v>15</v>
       </c>
       <c r="G22" s="44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H22" s="52"/>
       <c r="I22" s="45">
@@ -3781,15 +3809,15 @@
         <v>2109090.4800000004</v>
       </c>
       <c r="J22" s="40" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="C23" s="2">
         <v>2020</v>
@@ -3798,13 +3826,13 @@
         <v>1038</v>
       </c>
       <c r="E23" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G23" s="37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H23" s="51"/>
       <c r="I23" s="11">
@@ -3812,15 +3840,15 @@
         <v>913440</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="C24" s="2">
         <v>2030</v>
@@ -3829,13 +3857,13 @@
         <v>838</v>
       </c>
       <c r="E24" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G24" s="37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H24" s="51"/>
       <c r="I24" s="11">
@@ -3843,15 +3871,15 @@
         <v>737440</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="40" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B25" s="40" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C25" s="40">
         <v>2025</v>
@@ -3860,13 +3888,13 @@
         <v>608.47739999999999</v>
       </c>
       <c r="E25" s="42" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F25" s="43" t="s">
         <v>15</v>
       </c>
       <c r="G25" s="44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H25" s="52"/>
       <c r="I25" s="45">
@@ -3874,15 +3902,15 @@
         <v>644986.04399999999</v>
       </c>
       <c r="J25" s="40" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A26" s="53" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B26" s="53" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C26" s="53">
         <v>2025</v>
@@ -3891,31 +3919,31 @@
         <v>5350</v>
       </c>
       <c r="E26" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="F26" s="56" t="s">
         <v>120</v>
       </c>
-      <c r="F26" s="56" t="s">
+      <c r="G26" s="57" t="s">
         <v>121</v>
       </c>
-      <c r="G26" s="57" t="s">
+      <c r="H26" s="58" t="s">
         <v>122</v>
-      </c>
-      <c r="H26" s="58" t="s">
-        <v>123</v>
       </c>
       <c r="I26" s="54">
         <f>D26*$Q$3*10^3*0.67</f>
         <v>3154360</v>
       </c>
       <c r="J26" s="53" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:20" ht="72" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="C27" s="2">
         <v>2020</v>
@@ -3924,23 +3952,23 @@
         <v>988.32170015695601</v>
       </c>
       <c r="E27" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G27" s="37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H27" s="37" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I27" s="11">
         <f t="shared" ref="I27:I32" si="1">D27*$Q$3*10^3</f>
         <v>869723.09613812121</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R27" s="21"/>
       <c r="S27" s="3"/>
@@ -3948,10 +3976,10 @@
     </row>
     <row r="28" spans="1:20" ht="72" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="C28" s="2">
         <v>2030</v>
@@ -3960,23 +3988,23 @@
         <v>681.62247956991303</v>
       </c>
       <c r="E28" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G28" s="37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H28" s="37" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I28" s="11">
         <f t="shared" si="1"/>
         <v>599827.78202152345</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R28" s="21"/>
       <c r="S28" s="22"/>
@@ -3984,10 +4012,10 @@
     </row>
     <row r="29" spans="1:20" ht="72" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="C29" s="2">
         <v>2050</v>
@@ -3996,23 +4024,23 @@
         <v>681.62247956991303</v>
       </c>
       <c r="E29" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G29" s="37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H29" s="37" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I29" s="11">
         <f t="shared" si="1"/>
         <v>599827.78202152345</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R29" s="21"/>
       <c r="S29" s="32"/>
@@ -4020,10 +4048,10 @@
     </row>
     <row r="30" spans="1:20" ht="72" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C30" s="2">
         <v>2020</v>
@@ -4032,33 +4060,33 @@
         <v>1727.23444480956</v>
       </c>
       <c r="E30" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G30" s="37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H30" s="37" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I30" s="11">
         <f t="shared" si="1"/>
         <v>1519966.3114324128</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="S30" s="27"/>
       <c r="T30" s="13"/>
     </row>
     <row r="31" spans="1:20" ht="72" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C31" s="2">
         <v>2030</v>
@@ -4067,33 +4095,33 @@
         <v>1173.7257628388099</v>
       </c>
       <c r="E31" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G31" s="37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H31" s="37" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I31" s="11">
         <f t="shared" si="1"/>
         <v>1032878.6712981528</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="S31" s="27"/>
       <c r="T31" s="13"/>
     </row>
     <row r="32" spans="1:20" ht="72" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C32" s="2">
         <v>2050</v>
@@ -4102,31 +4130,31 @@
         <v>1173.7257628388099</v>
       </c>
       <c r="E32" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G32" s="37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H32" s="37" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I32" s="11">
         <f t="shared" si="1"/>
         <v>1032878.6712981528</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="40" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B33" s="40" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C33" s="40">
         <v>2025</v>
@@ -4136,31 +4164,31 @@
         <v>395.77480000000003</v>
       </c>
       <c r="E33" s="42" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F33" s="43" t="s">
         <v>15</v>
       </c>
       <c r="G33" s="44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H33" s="62" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I33" s="45">
         <f>D33*$Q$4*10^3</f>
         <v>419521.288</v>
       </c>
       <c r="J33" s="40" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="40" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B34" s="40" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C34" s="40">
         <v>2025</v>
@@ -4170,31 +4198,31 @@
         <v>560.37540000000001</v>
       </c>
       <c r="E34" s="42" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F34" s="43" t="s">
         <v>15</v>
       </c>
       <c r="G34" s="44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H34" s="62" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I34" s="45">
         <f>D34*$Q$4*10^3</f>
         <v>593997.924</v>
       </c>
       <c r="J34" s="40" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C35" s="2">
         <v>2020</v>
@@ -4203,13 +4231,13 @@
         <v>4013</v>
       </c>
       <c r="E35" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G35" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="11">
@@ -4217,15 +4245,15 @@
         <v>3574.8995633187774</v>
       </c>
       <c r="J35" s="53" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C36" s="2">
         <v>2024</v>
@@ -4234,13 +4262,13 @@
         <v>10000</v>
       </c>
       <c r="E36" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="F36" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="G36" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="H36" s="2"/>
       <c r="I36" s="2">
@@ -4248,12 +4276,12 @@
         <v>8200</v>
       </c>
       <c r="J36" s="53" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37">
@@ -4263,13 +4291,13 @@
         <v>6600</v>
       </c>
       <c r="E37" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>23</v>
       </c>
       <c r="G37" s="63" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H37"/>
       <c r="I37" s="64">
@@ -4277,15 +4305,15 @@
         <v>6636.9414666540169</v>
       </c>
       <c r="J37" s="53" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="66" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C38" s="2">
         <v>2030</v>
@@ -4294,10 +4322,10 @@
         <v>2000000</v>
       </c>
       <c r="E38" s="42" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F38" s="67" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G38" s="44"/>
       <c r="H38" s="62"/>
@@ -4306,15 +4334,15 @@
         <v>2220000</v>
       </c>
       <c r="J38" s="53" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="66" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C39" s="2">
         <v>2030</v>
@@ -4323,10 +4351,10 @@
         <v>450000</v>
       </c>
       <c r="E39" s="36" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F39" s="67" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
@@ -4335,15 +4363,15 @@
         <v>499500.00000000006</v>
       </c>
       <c r="J39" s="53" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="66" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C40" s="2">
         <v>2030</v>
@@ -4353,29 +4381,29 @@
         <v>1061000</v>
       </c>
       <c r="E40" s="36" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F40" s="69" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G40" s="2"/>
       <c r="H40" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I40" s="2">
         <f>D40*0.951*1.11</f>
         <v>1120002.2100000002</v>
       </c>
       <c r="J40" s="53" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="66" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C41" s="2">
         <v>2030</v>
@@ -4385,21 +4413,21 @@
         <v>5680</v>
       </c>
       <c r="E41" s="36" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F41" s="69" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I41" s="2">
         <f>D41*0.951*1.11</f>
         <v>5995.8648000000003</v>
       </c>
       <c r="J41" s="53" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -4509,25 +4537,25 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>